<commit_message>
Updated results with MKL-2017 GOLD update 1 numbers
</commit_message>
<xml_diff>
--- a/results/DeepBench_IA_KNL7250.xlsx
+++ b/results/DeepBench_IA_KNL7250.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmudiger\Documents\Work\DL\DeepBench\my_DeepBench_gh_pub\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="25040" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="555" yWindow="0" windowWidth="25035" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Specs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="72">
   <si>
     <t xml:space="preserve">OSU MPI </t>
   </si>
@@ -193,9 +198,6 @@
     <t>16.0.3 20160415</t>
   </si>
   <si>
-    <t>11.3.3</t>
-  </si>
-  <si>
     <t>3.10.0-327.el7.mpsp_1.3.1.45.x86_64</t>
   </si>
   <si>
@@ -216,6 +218,30 @@
   <si>
     <t>Total Time</t>
   </si>
+  <si>
+    <t>FWD Lib</t>
+  </si>
+  <si>
+    <t>BWD INPUTS Lib</t>
+  </si>
+  <si>
+    <t>BWD PARAMS Lib</t>
+  </si>
+  <si>
+    <t>MKL</t>
+  </si>
+  <si>
+    <t>LIBXSMM</t>
+  </si>
+  <si>
+    <t>LIBXSMM version</t>
+  </si>
+  <si>
+    <t>master-1.5.2-190</t>
+  </si>
+  <si>
+    <t>MKL 2017 Gold u1, MKLML (2017.0.1)</t>
+  </si>
 </sst>
 </file>
 
@@ -224,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,6 +300,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -338,7 +370,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -354,6 +386,9 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="38">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -730,33 +765,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X207"/>
+  <dimension ref="A1:AA207"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView showRuler="0" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="32.625" customWidth="1"/>
+    <col min="9" max="9" width="26.125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" customWidth="1"/>
+    <col min="11" max="11" width="24.125" customWidth="1"/>
+    <col min="12" max="12" width="18.625" customWidth="1"/>
+    <col min="13" max="13" width="15.875" customWidth="1"/>
+    <col min="14" max="14" width="20.125" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" customWidth="1"/>
+    <col min="20" max="20" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="14.375" customWidth="1"/>
+    <col min="25" max="27" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -782,7 +818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1760</v>
       </c>
@@ -799,18 +835,18 @@
         <v>8</v>
       </c>
       <c r="I2" s="2">
-        <v>7.7499999999999999E-2</v>
+        <v>7.8700000000000006E-2</v>
       </c>
       <c r="J2" s="2">
         <f>(2*C2*D2*E2)/(I2/1000)/10^12</f>
-        <v>1.2790090322580645</v>
+        <v>1.2595069885641677</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1760</v>
       </c>
@@ -827,18 +863,18 @@
         <v>8</v>
       </c>
       <c r="I3" s="2">
-        <v>0.11</v>
+        <v>0.10390000000000001</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J66" si="0">(2*C3*D3*E3)/(I3/1000)/10^12</f>
-        <v>1.8022400000000001</v>
+        <v>1.9080500481231952</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1760</v>
       </c>
@@ -855,18 +891,18 @@
         <v>8</v>
       </c>
       <c r="I4" s="2">
-        <v>0.19990000000000002</v>
+        <v>0.1862</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>1.9834557278639315</v>
+        <v>2.1293920515574651</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1760</v>
       </c>
@@ -883,18 +919,18 @@
         <v>8</v>
       </c>
       <c r="I5" s="2">
-        <v>0.39989999999999998</v>
+        <v>0.39189999999999997</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>1.9829597399349839</v>
+        <v>2.0234386323041593</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1760</v>
       </c>
@@ -911,18 +947,18 @@
         <v>8</v>
       </c>
       <c r="I6" s="2">
-        <v>9.9863</v>
+        <v>10.011700000000001</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>4.342589347405946</v>
+        <v>4.3315720606889929</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2048</v>
       </c>
@@ -939,18 +975,18 @@
         <v>8</v>
       </c>
       <c r="I7" s="2">
-        <v>8.0799999999999997E-2</v>
+        <v>8.0500000000000002E-2</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6611104950495048</v>
+        <v>1.6673009689440994</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>2048</v>
       </c>
@@ -967,18 +1003,18 @@
         <v>8</v>
       </c>
       <c r="I8" s="2">
-        <v>0.1236</v>
+        <v>0.13069999999999998</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>2.1718078964401295</v>
+        <v>2.0538290436113238</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>2048</v>
       </c>
@@ -995,18 +1031,18 @@
         <v>8</v>
       </c>
       <c r="I9" s="2">
-        <v>0.19440000000000002</v>
+        <v>0.19219999999999998</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>2.7616816460905347</v>
+        <v>2.7932929864724247</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>2048</v>
       </c>
@@ -1023,18 +1059,18 @@
         <v>8</v>
       </c>
       <c r="I10" s="2">
-        <v>0.36669999999999997</v>
+        <v>0.36940000000000001</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>2.9281205999454598</v>
+        <v>2.9067185273416354</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>2048</v>
       </c>
@@ -1051,18 +1087,18 @@
         <v>8</v>
       </c>
       <c r="I11" s="2">
-        <v>13.766200000000001</v>
+        <v>13.191700000000001</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>4.2655384928302649</v>
+        <v>4.4513031679010284</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>2560</v>
       </c>
@@ -1079,18 +1115,18 @@
         <v>8</v>
       </c>
       <c r="I12" s="2">
-        <v>0.14899999999999999</v>
+        <v>0.1482</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>1.4074845637583895</v>
+        <v>1.4150823211875845</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>2560</v>
       </c>
@@ -1107,18 +1143,18 @@
         <v>8</v>
       </c>
       <c r="I13" s="2">
-        <v>0.2082</v>
+        <v>0.2162</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>2.0145552353506244</v>
+        <v>1.9400111008325625</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>2560</v>
       </c>
@@ -1135,18 +1171,18 @@
         <v>8</v>
       </c>
       <c r="I14" s="2">
-        <v>0.34510000000000002</v>
+        <v>0.31869999999999998</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>2.4307760069545057</v>
+        <v>2.6321330404769374</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>2560</v>
       </c>
@@ -1163,18 +1199,18 @@
         <v>8</v>
       </c>
       <c r="I15" s="2">
-        <v>0.57410000000000005</v>
+        <v>0.57950000000000002</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>2.922350809963421</v>
+        <v>2.8951192407247626</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>2560</v>
       </c>
@@ -1191,18 +1227,18 @@
         <v>8</v>
       </c>
       <c r="I16" s="2">
-        <v>20.121599999999997</v>
+        <v>20.099799999999998</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>4.5597964376590339</v>
+        <v>4.5647419377307248</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="3:18">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>4096</v>
       </c>
@@ -1219,18 +1255,18 @@
         <v>8</v>
       </c>
       <c r="I17" s="2">
-        <v>0.39200000000000002</v>
+        <v>0.37640000000000001</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>1.3695686530612243</v>
+        <v>1.4263307970244421</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="3:18">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>4096</v>
       </c>
@@ -1247,18 +1283,18 @@
         <v>8</v>
       </c>
       <c r="I18" s="2">
-        <v>0.4652</v>
+        <v>0.47110000000000002</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>2.3081294582975063</v>
+        <v>2.279222721290596</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="3:18">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>4096</v>
       </c>
@@ -1275,18 +1311,18 @@
         <v>8</v>
       </c>
       <c r="I19" s="2">
-        <v>0.68510000000000004</v>
+        <v>0.68720000000000003</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
-        <v>3.1345550255437162</v>
+        <v>3.1249762048894061</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="3:18">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>4096</v>
       </c>
@@ -1303,18 +1339,18 @@
         <v>8</v>
       </c>
       <c r="I20" s="2">
-        <v>1.2495000000000001</v>
+        <v>1.2370999999999999</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="0"/>
-        <v>3.4373487763105244</v>
+        <v>3.4718028421307898</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="3:18">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>4096</v>
       </c>
@@ -1331,18 +1367,18 @@
         <v>8</v>
       </c>
       <c r="I21" s="2">
-        <v>52.081099999999999</v>
+        <v>51.761600000000001</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
-        <v>4.5099090456998798</v>
+        <v>4.5377465920682507</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" spans="3:18">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>1760</v>
       </c>
@@ -1359,18 +1395,18 @@
         <v>8</v>
       </c>
       <c r="I22" s="2">
-        <v>7.9500000000000001E-2</v>
+        <v>9.1499999999999998E-2</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="0"/>
-        <v>1.2468327044025156</v>
+        <v>1.0833136612021859</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="3:18">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1760</v>
       </c>
@@ -1387,18 +1423,18 @@
         <v>8</v>
       </c>
       <c r="I23" s="2">
-        <v>0.10350000000000001</v>
+        <v>0.10070000000000001</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="0"/>
-        <v>1.9154241545893718</v>
+        <v>1.9686832174776563</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="3:18">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>1760</v>
       </c>
@@ -1415,18 +1451,18 @@
         <v>8</v>
       </c>
       <c r="I24" s="2">
-        <v>0.15530000000000002</v>
+        <v>0.16280000000000003</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="0"/>
-        <v>2.5530766258853825</v>
+        <v>2.4354594594594592</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="3:18">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>1760</v>
       </c>
@@ -1443,18 +1479,18 @@
         <v>8</v>
       </c>
       <c r="I25" s="2">
-        <v>0.27789999999999998</v>
+        <v>0.26350000000000001</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>2.853492623245772</v>
+        <v>3.0094330170777988</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="3:18">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1760</v>
       </c>
@@ -1471,18 +1507,18 @@
         <v>8</v>
       </c>
       <c r="I26" s="2">
-        <v>10.0008</v>
+        <v>10.022200000000002</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" si="0"/>
-        <v>4.336293096552275</v>
+        <v>4.3270339845542889</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="3:18">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>2048</v>
       </c>
@@ -1499,18 +1535,18 @@
         <v>8</v>
       </c>
       <c r="I27" s="2">
-        <v>8.5500000000000007E-2</v>
+        <v>8.1599999999999992E-2</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" si="0"/>
-        <v>1.5697979883040936</v>
+        <v>1.6448250980392158</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="3:18">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>2048</v>
       </c>
@@ -1527,18 +1563,18 @@
         <v>8</v>
       </c>
       <c r="I28" s="2">
-        <v>0.1245</v>
+        <v>0.1212</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="0"/>
-        <v>2.1561080803212853</v>
+        <v>2.21481399339934</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="3:18">
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>2048</v>
       </c>
@@ -1555,18 +1591,18 @@
         <v>8</v>
       </c>
       <c r="I29" s="2">
-        <v>0.19350000000000001</v>
+        <v>0.1961</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" si="0"/>
-        <v>2.774526677002584</v>
+        <v>2.7377404997450285</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="3:18">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>2048</v>
       </c>
@@ -1583,18 +1619,18 @@
         <v>8</v>
       </c>
       <c r="I30" s="2">
-        <v>0.35960000000000003</v>
+        <v>0.36969999999999997</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" si="0"/>
-        <v>2.9859338820912122</v>
+        <v>2.9043598160670814</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="3:18">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>2048</v>
       </c>
@@ -1611,18 +1647,18 @@
         <v>8</v>
       </c>
       <c r="I31" s="2">
-        <v>13.7113</v>
+        <v>13.147</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" si="0"/>
-        <v>4.2826176948939922</v>
+        <v>4.466437666387769</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="3:18">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>2560</v>
       </c>
@@ -1639,18 +1675,18 @@
         <v>8</v>
       </c>
       <c r="I32" s="2">
-        <v>0.16390000000000002</v>
+        <v>0.15940000000000001</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" si="0"/>
-        <v>1.2795314215985354</v>
+        <v>1.3156537013801755</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="3:18">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>2560</v>
       </c>
@@ -1667,18 +1703,18 @@
         <v>8</v>
       </c>
       <c r="I33" s="2">
-        <v>0.24980000000000002</v>
+        <v>0.2036</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="0"/>
-        <v>1.6790648518815052</v>
+        <v>2.0600707269155203</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="3:18">
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>2560</v>
       </c>
@@ -1695,18 +1731,18 @@
         <v>8</v>
       </c>
       <c r="I34" s="2">
-        <v>0.41930000000000001</v>
+        <v>0.32110000000000005</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" si="0"/>
-        <v>2.0006219890293346</v>
+        <v>2.6124596698847706</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="3:18">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>2560</v>
       </c>
@@ -1723,18 +1759,18 @@
         <v>8</v>
       </c>
       <c r="I35" s="2">
-        <v>0.80820000000000003</v>
+        <v>0.56329999999999991</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>2.0758742885424399</v>
+        <v>2.9783802591869351</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="3:18">
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>2560</v>
       </c>
@@ -1751,18 +1787,18 @@
         <v>8</v>
       </c>
       <c r="I36" s="2">
-        <v>20.717099999999999</v>
+        <v>20.104500000000002</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="0"/>
-        <v>4.4287279590290147</v>
+        <v>4.5636747991743141</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
     </row>
-    <row r="37" spans="3:18">
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>4096</v>
       </c>
@@ -1779,18 +1815,18 @@
         <v>8</v>
       </c>
       <c r="I37" s="2">
-        <v>0.38239999999999996</v>
+        <v>0.36860000000000004</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="0"/>
-        <v>1.403951129707113</v>
+        <v>1.4565135973955508</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
     </row>
-    <row r="38" spans="3:18">
+    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>4096</v>
       </c>
@@ -1807,18 +1843,18 @@
         <v>8</v>
       </c>
       <c r="I38" s="2">
-        <v>0.46400000000000002</v>
+        <v>0.46450000000000002</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" si="0"/>
-        <v>2.3140987586206894</v>
+        <v>2.3116078019375674</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="3:18">
+    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>4096</v>
       </c>
@@ -1835,18 +1871,18 @@
         <v>8</v>
       </c>
       <c r="I39" s="2">
-        <v>0.68889999999999996</v>
+        <v>0.69189999999999996</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="0"/>
-        <v>3.1172646944404123</v>
+        <v>3.1037485879462352</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="3:18">
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>4096</v>
       </c>
@@ -1863,18 +1899,18 @@
         <v>8</v>
       </c>
       <c r="I40" s="2">
-        <v>1.2384999999999999</v>
+        <v>1.2324999999999999</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" si="0"/>
-        <v>3.4678783173193377</v>
+        <v>3.4847604835699801</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
     </row>
-    <row r="41" spans="3:18">
+    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>4096</v>
       </c>
@@ -1891,18 +1927,18 @@
         <v>8</v>
       </c>
       <c r="I41" s="2">
-        <v>51.83</v>
+        <v>52.286099999999998</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" si="0"/>
-        <v>4.5317581323557787</v>
+        <v>4.4922268824792821</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="3:18">
+    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>1760</v>
       </c>
@@ -1922,18 +1958,18 @@
         <v>25</v>
       </c>
       <c r="I42" s="2">
-        <v>11.221299999999999</v>
+        <v>11.495200000000001</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" si="0"/>
-        <v>3.9380786183419034</v>
+        <v>3.8442446934372607</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="3:18">
+    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>2048</v>
       </c>
@@ -1950,18 +1986,18 @@
         <v>24</v>
       </c>
       <c r="I43" s="2">
-        <v>15.1691</v>
+        <v>15.4033</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" si="0"/>
-        <v>3.9445940012261773</v>
+        <v>3.8846182872501349</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="3:18">
+    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>2560</v>
       </c>
@@ -1978,18 +2014,18 @@
         <v>24</v>
       </c>
       <c r="I44" s="2">
-        <v>23.776</v>
+        <v>23.782799999999998</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="0"/>
-        <v>3.9322702557200544</v>
+        <v>3.9311459374001383</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
     </row>
-    <row r="45" spans="3:18">
+    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C45" s="3">
         <v>4096</v>
       </c>
@@ -2006,18 +2042,18 @@
         <v>24</v>
       </c>
       <c r="I45" s="2">
-        <v>54.2879</v>
+        <v>55.115699999999997</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="0"/>
-        <v>4.4087865519940905</v>
+        <v>4.342569602781059</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="3:18">
+    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="M46" s="2"/>
@@ -2025,7 +2061,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="3:18">
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="M47" s="2"/>
@@ -2033,7 +2069,7 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
-    <row r="48" spans="3:18">
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>5124</v>
       </c>
@@ -2050,18 +2086,18 @@
         <v>8</v>
       </c>
       <c r="I48" s="2">
-        <v>37.983199999999997</v>
+        <v>38.194600000000001</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="0"/>
-        <v>4.332569228501022</v>
+        <v>4.3085892644509958</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
-    <row r="49" spans="3:18">
+    <row r="49" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>35</v>
       </c>
@@ -2078,18 +2114,18 @@
         <v>8</v>
       </c>
       <c r="I49" s="2">
-        <v>0.56720000000000004</v>
+        <v>0.54730000000000001</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="0"/>
-        <v>1.8369224259520451</v>
+        <v>1.9037135026493697</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
     </row>
-    <row r="50" spans="3:18">
+    <row r="50" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>5124</v>
       </c>
@@ -2106,18 +2142,18 @@
         <v>8</v>
       </c>
       <c r="I50" s="2">
-        <v>44.197000000000003</v>
+        <v>44.437100000000001</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="0"/>
-        <v>4.3327292824399848</v>
+        <v>4.3093189271127059</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
     </row>
-    <row r="51" spans="3:18">
+    <row r="51" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>35</v>
       </c>
@@ -2134,18 +2170,18 @@
         <v>8</v>
       </c>
       <c r="I51" s="2">
-        <v>0.65629999999999999</v>
+        <v>0.66190000000000004</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" si="0"/>
-        <v>1.8473190918787141</v>
+        <v>1.8316898625169964</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
     </row>
-    <row r="52" spans="3:18">
+    <row r="52" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>5124</v>
       </c>
@@ -2162,18 +2198,18 @@
         <v>8</v>
       </c>
       <c r="I52" s="2">
-        <v>55.025400000000005</v>
+        <v>55.539699999999996</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" si="0"/>
-        <v>4.3501191289840691</v>
+        <v>4.3098368395940208</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
-    <row r="53" spans="3:18">
+    <row r="53" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>35</v>
       </c>
@@ -2190,18 +2226,18 @@
         <v>8</v>
       </c>
       <c r="I53" s="2">
-        <v>0.79670000000000007</v>
+        <v>0.80349999999999999</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" si="0"/>
-        <v>1.9022146353709048</v>
+        <v>1.8861162414436841</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="3:18">
+    <row r="54" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>5124</v>
       </c>
@@ -2218,18 +2254,18 @@
         <v>8</v>
       </c>
       <c r="I54" s="2">
-        <v>88.071600000000004</v>
+        <v>87.715199999999996</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" si="0"/>
-        <v>4.3485899221996647</v>
+        <v>4.3662588946043561</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="3:18">
+    <row r="55" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>35</v>
       </c>
@@ -2246,18 +2282,18 @@
         <v>8</v>
       </c>
       <c r="I55" s="2">
-        <v>1.35</v>
+        <v>1.2481</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" si="0"/>
-        <v>1.796141511111111</v>
+        <v>1.9427858665171061</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="3:18">
+    <row r="56" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>5124</v>
       </c>
@@ -2274,18 +2310,18 @@
         <v>8</v>
       </c>
       <c r="I56" s="2">
-        <v>37.591900000000003</v>
+        <v>37.909599999999998</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" si="0"/>
-        <v>4.3776676230783753</v>
+        <v>4.340980741553591</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="3:18">
+    <row r="57" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>35</v>
       </c>
@@ -2302,18 +2338,18 @@
         <v>8</v>
       </c>
       <c r="I57" s="2">
-        <v>0.58250000000000002</v>
+        <v>0.53960000000000008</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" si="0"/>
-        <v>1.7886736480686694</v>
+        <v>1.930879169755374</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="3:18">
+    <row r="58" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>5124</v>
       </c>
@@ -2330,18 +2366,18 @@
         <v>8</v>
       </c>
       <c r="I58" s="2">
-        <v>44.316600000000001</v>
+        <v>44.522400000000005</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="0"/>
-        <v>4.3210362729992831</v>
+        <v>4.3010627480998327</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
     </row>
-    <row r="59" spans="3:18">
+    <row r="59" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>35</v>
       </c>
@@ -2358,18 +2394,18 @@
         <v>8</v>
       </c>
       <c r="I59" s="2">
-        <v>0.72150000000000003</v>
+        <v>0.64229999999999998</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" si="0"/>
-        <v>1.680381871101871</v>
+        <v>1.8875844932274639</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
     </row>
-    <row r="60" spans="3:18">
+    <row r="60" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>5124</v>
       </c>
@@ -2386,18 +2422,18 @@
         <v>8</v>
       </c>
       <c r="I60" s="2">
-        <v>55.169600000000003</v>
+        <v>55.704500000000003</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" si="0"/>
-        <v>4.338748968997419</v>
+        <v>4.2970863237260897</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
-    <row r="61" spans="3:18">
+    <row r="61" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>35</v>
       </c>
@@ -2414,18 +2450,18 @@
         <v>8</v>
       </c>
       <c r="I61" s="2">
-        <v>0.87620000000000009</v>
+        <v>0.83720000000000006</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" si="0"/>
-        <v>1.7296215475918739</v>
+        <v>1.8101939799331102</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="3:18">
+    <row r="62" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>5124</v>
       </c>
@@ -2442,18 +2478,18 @@
         <v>8</v>
       </c>
       <c r="I62" s="2">
-        <v>88.371399999999994</v>
+        <v>87.778100000000009</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" si="0"/>
-        <v>4.3338373296337958</v>
+        <v>4.3631301223425885</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
     </row>
-    <row r="63" spans="3:18">
+    <row r="63" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>35</v>
       </c>
@@ -2470,18 +2506,18 @@
         <v>8</v>
       </c>
       <c r="I63" s="2">
-        <v>1.2795000000000001</v>
+        <v>1.2887999999999999</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" si="0"/>
-        <v>1.8951082766705745</v>
+        <v>1.8814331471135943</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
     </row>
-    <row r="64" spans="3:18">
+    <row r="64" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="M64" s="2"/>
@@ -2489,7 +2525,7 @@
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
     </row>
-    <row r="65" spans="3:18">
+    <row r="65" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>7680</v>
       </c>
@@ -2517,7 +2553,7 @@
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
     </row>
-    <row r="66" spans="3:18">
+    <row r="66" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>7680</v>
       </c>
@@ -2534,18 +2570,18 @@
         <v>8</v>
       </c>
       <c r="I66" s="2">
-        <v>0.58629999999999993</v>
+        <v>0.59089999999999998</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" si="0"/>
-        <v>2.1461558928876006</v>
+        <v>2.1294486376713491</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
     </row>
-    <row r="67" spans="3:18">
+    <row r="67" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>7680</v>
       </c>
@@ -2562,18 +2598,18 @@
         <v>8</v>
       </c>
       <c r="I67" s="2">
-        <v>0.82529999999999992</v>
+        <v>0.82400000000000007</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" ref="J67:J83" si="1">(2*C67*D67*E67)/(I67/1000)/10^12</f>
-        <v>3.0492940748818613</v>
+        <v>3.0541048543689318</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
-    <row r="68" spans="3:18">
+    <row r="68" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>7680</v>
       </c>
@@ -2590,18 +2626,18 @@
         <v>8</v>
       </c>
       <c r="I68" s="2">
-        <v>1.3689000000000002</v>
+        <v>1.3814000000000002</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" si="1"/>
-        <v>3.6767950909489366</v>
+        <v>3.6435245403214132</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
     </row>
-    <row r="69" spans="3:18">
+    <row r="69" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>7680</v>
       </c>
@@ -2618,18 +2654,18 @@
         <v>8</v>
       </c>
       <c r="I69" s="2">
-        <v>0.43810000000000004</v>
+        <v>0.43280000000000002</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" si="1"/>
-        <v>1.4360776078520885</v>
+        <v>1.4536635859519409</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="3:18">
+    <row r="70" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>7680</v>
       </c>
@@ -2646,18 +2682,18 @@
         <v>8</v>
       </c>
       <c r="I70" s="2">
-        <v>0.52949999999999997</v>
+        <v>0.52860000000000007</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" si="1"/>
-        <v>2.3763762039660055</v>
+        <v>2.3804222474460839</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
     </row>
-    <row r="71" spans="3:18">
+    <row r="71" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>7680</v>
       </c>
@@ -2674,18 +2710,18 @@
         <v>8</v>
       </c>
       <c r="I71" s="2">
-        <v>0.77179999999999993</v>
+        <v>0.76290000000000002</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" si="1"/>
-        <v>3.2606664939103398</v>
+        <v>3.2987054659850568</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
     </row>
-    <row r="72" spans="3:18">
+    <row r="72" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>7680</v>
       </c>
@@ -2702,18 +2738,18 @@
         <v>8</v>
       </c>
       <c r="I72" s="2">
-        <v>1.3352999999999999</v>
+        <v>1.3599000000000001</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" si="1"/>
-        <v>3.7693138620534712</v>
+        <v>3.7011286123979703</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
     </row>
-    <row r="73" spans="3:18">
+    <row r="73" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C73">
         <f t="shared" ref="C73:C80" si="2">3*1024</f>
         <v>3072</v>
@@ -2731,18 +2767,18 @@
         <v>8</v>
       </c>
       <c r="I73" s="2">
-        <v>5.9500000000000004E-2</v>
+        <v>5.6399999999999999E-2</v>
       </c>
       <c r="J73" s="2">
         <f t="shared" si="1"/>
-        <v>1.691820100840336</v>
+        <v>1.7848102127659573</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
     </row>
-    <row r="74" spans="3:18">
+    <row r="74" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C74">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2760,18 +2796,18 @@
         <v>8</v>
       </c>
       <c r="I74" s="2">
-        <v>9.5200000000000007E-2</v>
+        <v>9.06E-2</v>
       </c>
       <c r="J74" s="2">
         <f t="shared" si="1"/>
-        <v>2.1147751260504197</v>
+        <v>2.2221478145695359</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="Q74" s="2"/>
       <c r="R74" s="2"/>
     </row>
-    <row r="75" spans="3:18">
+    <row r="75" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C75">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2789,18 +2825,18 @@
         <v>8</v>
       </c>
       <c r="I75" s="2">
-        <v>0.14319999999999999</v>
+        <v>0.16419999999999998</v>
       </c>
       <c r="J75" s="2">
         <f t="shared" si="1"/>
-        <v>2.8118239106145255</v>
+        <v>2.4522118392204635</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
     </row>
-    <row r="76" spans="3:18">
+    <row r="76" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C76">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2818,18 +2854,18 @@
         <v>8</v>
       </c>
       <c r="I76" s="2">
-        <v>0.25800000000000001</v>
+        <v>0.25630000000000003</v>
       </c>
       <c r="J76" s="2">
         <f t="shared" si="1"/>
-        <v>3.1213425116279074</v>
+        <v>3.1420459149434254</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
     </row>
-    <row r="77" spans="3:18">
+    <row r="77" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C77">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2847,18 +2883,18 @@
         <v>8</v>
       </c>
       <c r="I77" s="2">
-        <v>8.1299999999999997E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="J77" s="2">
         <f t="shared" si="1"/>
-        <v>1.238170922509225</v>
+        <v>1.2742189367088608</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="3:18">
+    <row r="78" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C78">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2876,18 +2912,18 @@
         <v>8</v>
       </c>
       <c r="I78" s="2">
-        <v>0.1095</v>
+        <v>0.1077</v>
       </c>
       <c r="J78" s="2">
         <f t="shared" si="1"/>
-        <v>1.8385990136986301</v>
+        <v>1.8693276880222842</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
     </row>
-    <row r="79" spans="3:18">
+    <row r="79" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C79">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2905,18 +2941,18 @@
         <v>8</v>
       </c>
       <c r="I79" s="2">
-        <v>0.159</v>
+        <v>0.15959999999999999</v>
       </c>
       <c r="J79" s="2">
         <f t="shared" si="1"/>
-        <v>2.5324099622641509</v>
+        <v>2.5228896240601504</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="Q79" s="2"/>
       <c r="R79" s="2"/>
     </row>
-    <row r="80" spans="3:18">
+    <row r="80" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C80">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2934,18 +2970,18 @@
         <v>8</v>
       </c>
       <c r="I80" s="2">
-        <v>0.27430000000000004</v>
+        <v>0.27239999999999998</v>
       </c>
       <c r="J80" s="2">
         <f t="shared" si="1"/>
-        <v>2.9358598906306956</v>
+        <v>2.9563376211453751</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="Q80" s="2"/>
       <c r="R80" s="2"/>
     </row>
-    <row r="81" spans="1:24">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="M81" s="2"/>
@@ -2953,7 +2989,7 @@
       <c r="Q81" s="2"/>
       <c r="R81" s="2"/>
     </row>
-    <row r="82" spans="1:24">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C82">
         <v>3072</v>
       </c>
@@ -2970,18 +3006,18 @@
         <v>24</v>
       </c>
       <c r="I82" s="2">
-        <v>10.896600000000001</v>
+        <v>10.945200000000002</v>
       </c>
       <c r="J82" s="2">
         <f t="shared" si="1"/>
-        <v>4.2928046693464017</v>
+        <v>4.2737433176186812</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
     </row>
-    <row r="83" spans="1:24">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C83">
         <v>7680</v>
       </c>
@@ -2998,31 +3034,31 @@
         <v>24</v>
       </c>
       <c r="I83" s="2">
-        <v>51.992699999999999</v>
+        <v>52.102900000000005</v>
       </c>
       <c r="J83" s="2">
         <f t="shared" si="1"/>
-        <v>4.1452298034147104</v>
+        <v>4.1364624541052413</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="Q83" s="2"/>
       <c r="R83" s="2"/>
     </row>
-    <row r="85" spans="1:24">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J85" s="2"/>
       <c r="N85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="87" spans="1:24">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J87" s="1"/>
     </row>
-    <row r="89" spans="1:24">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:24">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>22</v>
       </c>
@@ -3072,7 +3108,7 @@
         <v>38</v>
       </c>
       <c r="T90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U90" t="s">
         <v>39</v>
@@ -3083,8 +3119,17 @@
       <c r="W90" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="91" spans="1:24">
+      <c r="Y90" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z90" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA90" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>700</v>
       </c>
@@ -3119,13 +3164,13 @@
         <v>2</v>
       </c>
       <c r="N91" s="2">
-        <v>0.19317863360107504</v>
+        <v>0.17917</v>
       </c>
       <c r="O91" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P91" s="2">
-        <v>3.1055000000000001</v>
+        <v>2.6216999999999997</v>
       </c>
       <c r="R91" s="4">
         <f>(D91-H91+1+2*J91)/L91</f>
@@ -3137,21 +3182,31 @@
       </c>
       <c r="T91" s="10">
         <f>N91+P91</f>
-        <v>3.2986786336010754</v>
+        <v>2.8008699999999997</v>
       </c>
       <c r="U91" s="2">
         <f>(2*$R91*$S91*$F91*$G91*$E91*$H91*$I91)/(N91/1000)/10^12</f>
-        <v>3.5421557096891694</v>
+        <v>3.8191036445833566</v>
       </c>
       <c r="V91" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W91" s="2">
         <f>(2*$R91*$S91*$F91*$G91*$E91*$H91*$I91)/(P91/1000)/10^12</f>
-        <v>0.22034094348736111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:24">
+        <v>0.26100194530266624</v>
+      </c>
+      <c r="X91" s="2"/>
+      <c r="Y91" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA91" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C92">
         <v>700</v>
       </c>
@@ -3186,13 +3241,13 @@
         <v>2</v>
       </c>
       <c r="N92" s="2">
-        <v>0.41029079233289006</v>
+        <v>0.35833000000000004</v>
       </c>
       <c r="O92" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P92" s="2">
-        <v>5.9086000000000007</v>
+        <v>2.6246</v>
       </c>
       <c r="R92" s="4">
         <f t="shared" ref="R92:R126" si="3">(D92-H92+1+2*J92)/L92</f>
@@ -3204,21 +3259,31 @@
       </c>
       <c r="T92" s="10">
         <f>N92+P92</f>
-        <v>6.3188907923328905</v>
+        <v>2.9829300000000001</v>
       </c>
       <c r="U92" s="2">
         <f>(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(N92/1000)/10^12</f>
-        <v>3.3355308614618751</v>
+        <v>3.8192102252113971</v>
       </c>
       <c r="V92" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W92" s="2">
         <f>(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(P92/1000)/10^12</f>
-        <v>0.23161791287276171</v>
-      </c>
-    </row>
-    <row r="93" spans="1:24">
+        <v>0.52142711270288811</v>
+      </c>
+      <c r="X92" s="2"/>
+      <c r="Y92" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>700</v>
       </c>
@@ -3253,13 +3318,13 @@
         <v>2</v>
       </c>
       <c r="N93" s="2">
-        <v>0.88766066729817916</v>
+        <v>0.76228000000000007</v>
       </c>
       <c r="O93" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P93" s="2">
-        <v>11.585000000000001</v>
+        <v>2.6320999999999999</v>
       </c>
       <c r="R93" s="4">
         <f t="shared" si="3"/>
@@ -3271,21 +3336,31 @@
       </c>
       <c r="T93" s="10">
         <f>N93+P93</f>
-        <v>12.472660667298181</v>
+        <v>3.39438</v>
       </c>
       <c r="U93" s="2">
         <f>(2*$R93*$S93*$F93*$G93*$E93*$H93*$I93)/(N93/1000)/10^12</f>
-        <v>3.0834701827343367</v>
+        <v>3.5906428084168547</v>
       </c>
       <c r="V93" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W93" s="2">
         <f>(2*$R93*$S93*$F93*$G93*$E93*$H93*$I93)/(P93/1000)/10^12</f>
-        <v>0.23626026758739746</v>
-      </c>
-    </row>
-    <row r="94" spans="1:24">
+        <v>1.0398826792295126</v>
+      </c>
+      <c r="X93" s="2"/>
+      <c r="Y93" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z93" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA93" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C94">
         <v>700</v>
       </c>
@@ -3320,13 +3395,13 @@
         <v>2</v>
       </c>
       <c r="N94" s="2">
-        <v>1.7338353263662845</v>
+        <v>1.5425</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P94" s="2">
-        <v>22.779</v>
+        <v>2.6388000000000003</v>
       </c>
       <c r="R94" s="4">
         <f t="shared" si="3"/>
@@ -3338,21 +3413,31 @@
       </c>
       <c r="T94" s="10">
         <f>N94+P94</f>
-        <v>24.512835326366286</v>
+        <v>4.1813000000000002</v>
       </c>
       <c r="U94" s="2">
         <f>(2*$R94*$S94*$F94*$G94*$E94*$H94*$I94)/(N94/1000)/10^12</f>
-        <v>3.1572493170228255</v>
+        <v>3.5488819448946516</v>
       </c>
       <c r="V94" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W94" s="2">
         <f>(2*$R94*$S94*$F94*$G94*$E94*$H94*$I94)/(P94/1000)/10^12</f>
-        <v>0.24031565915975242</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24">
+        <v>2.0744847658026373</v>
+      </c>
+      <c r="X94" s="2"/>
+      <c r="Y94" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z94" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>341</v>
       </c>
@@ -3387,13 +3472,13 @@
         <v>2</v>
       </c>
       <c r="N95" s="2">
-        <v>0.91041034119945885</v>
+        <v>1.0842000000000001</v>
       </c>
       <c r="O95" s="2">
-        <v>68.790000000000006</v>
+        <v>86.45</v>
       </c>
       <c r="P95" s="2">
-        <v>74.98</v>
+        <v>3.63</v>
       </c>
       <c r="R95" s="4">
         <f t="shared" si="3"/>
@@ -3405,23 +3490,32 @@
       </c>
       <c r="T95" s="2">
         <f>N95+O95+P95</f>
-        <v>144.68041034119949</v>
+        <v>91.164199999999994</v>
       </c>
       <c r="U95" s="2">
         <f t="shared" ref="U95:U126" si="5">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(N95/1000)/10^12</f>
-        <v>2.8006711749788678</v>
+        <v>2.3517432208079687</v>
       </c>
       <c r="V95" s="2">
         <f t="shared" ref="V95:V126" si="6">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(O95/1000)/10^12</f>
-        <v>3.7065852594853906E-2</v>
+        <v>2.9494042799305956E-2</v>
       </c>
       <c r="W95" s="2">
         <f t="shared" ref="W95:W126" si="7">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(P95/1000)/10^12</f>
-        <v>3.4005868231528402E-2</v>
-      </c>
-      <c r="X95" s="3"/>
-    </row>
-    <row r="96" spans="1:24">
+        <v>0.70241322314049581</v>
+      </c>
+      <c r="X95" s="2"/>
+      <c r="Y95" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z95" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C96">
         <v>341</v>
       </c>
@@ -3456,13 +3550,13 @@
         <v>2</v>
       </c>
       <c r="N96" s="2">
-        <v>1.6416750237159505</v>
+        <v>1.8062</v>
       </c>
       <c r="O96" s="2">
-        <v>69.460000000000008</v>
+        <v>86.61</v>
       </c>
       <c r="P96" s="2">
-        <v>74.36</v>
+        <v>3.67</v>
       </c>
       <c r="R96" s="4">
         <f t="shared" si="3"/>
@@ -3474,23 +3568,32 @@
       </c>
       <c r="T96" s="2">
         <f t="shared" ref="T96:T98" si="8">N96+O96+P96</f>
-        <v>145.46167502371594</v>
+        <v>92.086200000000005</v>
       </c>
       <c r="U96" s="2">
         <f t="shared" si="5"/>
-        <v>3.10629078613694</v>
+        <v>2.8233418226110065</v>
       </c>
       <c r="V96" s="2">
         <f t="shared" si="6"/>
-        <v>7.3416642672041454E-2</v>
+        <v>5.8879113266366481E-2</v>
       </c>
       <c r="W96" s="2">
         <f t="shared" si="7"/>
-        <v>6.8578805809575039E-2</v>
-      </c>
-      <c r="X96" s="3"/>
-    </row>
-    <row r="97" spans="3:24">
+        <v>1.3895149863760217</v>
+      </c>
+      <c r="X96" s="2"/>
+      <c r="Y96" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z96" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA96" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="97" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>341</v>
       </c>
@@ -3525,13 +3628,13 @@
         <v>2</v>
       </c>
       <c r="N97" s="2">
-        <v>3.2716008372155834</v>
+        <v>3.6389999999999998</v>
       </c>
       <c r="O97" s="2">
-        <v>70.600000000000009</v>
+        <v>86.84</v>
       </c>
       <c r="P97" s="2">
-        <v>77.61</v>
+        <v>3.73</v>
       </c>
       <c r="R97" s="4">
         <f t="shared" si="3"/>
@@ -3543,23 +3646,32 @@
       </c>
       <c r="T97" s="2">
         <f t="shared" si="8"/>
-        <v>151.48160083721558</v>
+        <v>94.209000000000003</v>
       </c>
       <c r="U97" s="2">
         <f t="shared" si="5"/>
-        <v>3.1174463229078615</v>
+        <v>2.802704039571311</v>
       </c>
       <c r="V97" s="2">
         <f t="shared" si="6"/>
-        <v>0.14446232294617564</v>
+        <v>0.11744633809304468</v>
       </c>
       <c r="W97" s="2">
         <f t="shared" si="7"/>
-        <v>0.13141399304213375</v>
-      </c>
-      <c r="X97" s="3"/>
-    </row>
-    <row r="98" spans="3:24">
+        <v>2.7343270777479893</v>
+      </c>
+      <c r="X97" s="2"/>
+      <c r="Y97" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z97" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA97" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>341</v>
       </c>
@@ -3594,13 +3706,13 @@
         <v>2</v>
       </c>
       <c r="N98" s="2">
-        <v>6.2727829379591569</v>
+        <v>6.2116000000000007</v>
       </c>
       <c r="O98" s="2">
-        <v>73.27</v>
+        <v>87.55</v>
       </c>
       <c r="P98" s="2">
-        <v>95.18</v>
+        <v>7.24</v>
       </c>
       <c r="R98" s="4">
         <f t="shared" si="3"/>
@@ -3612,23 +3724,32 @@
       </c>
       <c r="T98" s="2">
         <f t="shared" si="8"/>
-        <v>174.72278293795915</v>
+        <v>101.0016</v>
       </c>
       <c r="U98" s="2">
         <f t="shared" si="5"/>
-        <v>3.2518389687235847</v>
+        <v>3.2838688904630042</v>
       </c>
       <c r="V98" s="2">
         <f t="shared" si="6"/>
-        <v>0.27839606933260541</v>
+        <v>0.23298777841233581</v>
       </c>
       <c r="W98" s="2">
         <f t="shared" si="7"/>
-        <v>0.21431056944736288</v>
-      </c>
-      <c r="X98" s="3"/>
-    </row>
-    <row r="99" spans="3:24">
+        <v>2.8174143646408836</v>
+      </c>
+      <c r="X98" s="2"/>
+      <c r="Y98" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z98" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA98" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>480</v>
       </c>
@@ -3663,13 +3784,13 @@
         <v>1</v>
       </c>
       <c r="N99" s="2">
-        <v>0.24355559633869375</v>
-      </c>
-      <c r="O99" s="2" t="s">
-        <v>63</v>
+        <v>8.4348000000000006E-2</v>
+      </c>
+      <c r="O99" s="2">
+        <v>2.94</v>
       </c>
       <c r="P99" s="2">
-        <v>25.55</v>
+        <v>0.66164999999999996</v>
       </c>
       <c r="R99" s="4">
         <f t="shared" si="3"/>
@@ -3681,22 +3802,31 @@
       </c>
       <c r="T99" s="2">
         <f>N99+P99</f>
-        <v>25.793555596338695</v>
+        <v>0.74599799999999994</v>
       </c>
       <c r="U99" s="2">
         <f t="shared" si="5"/>
-        <v>0.43591000000000002</v>
+        <v>1.2586939820742638</v>
       </c>
       <c r="V99" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W99" s="2">
         <f t="shared" si="7"/>
-        <v>4.1553158512720153E-3</v>
-      </c>
-      <c r="X99" s="3"/>
-    </row>
-    <row r="100" spans="3:24">
+        <v>0.16045994105644981</v>
+      </c>
+      <c r="X99" s="2"/>
+      <c r="Y99" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z99" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA99" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>240</v>
       </c>
@@ -3731,13 +3861,13 @@
         <v>1</v>
       </c>
       <c r="N100" s="2">
-        <v>0.19266549314944201</v>
+        <v>0.21876000000000001</v>
       </c>
       <c r="O100" s="2">
-        <v>582.05999999999995</v>
+        <v>11.76</v>
       </c>
       <c r="P100" s="2">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
       <c r="R100" s="4">
         <f t="shared" si="3"/>
@@ -3749,23 +3879,32 @@
       </c>
       <c r="T100" s="2">
         <f>N100+O100+P100</f>
-        <v>582.99266549314939</v>
+        <v>12.648759999999999</v>
       </c>
       <c r="U100" s="2">
         <f t="shared" si="5"/>
-        <v>4.4083999999999994</v>
+        <v>3.8825496434448712</v>
       </c>
       <c r="V100" s="2">
         <f t="shared" si="6"/>
-        <v>1.4592079167096178E-3</v>
+        <v>7.2223346938775509E-2</v>
       </c>
       <c r="W100" s="2">
         <f t="shared" si="7"/>
-        <v>1.1477656216216217</v>
-      </c>
-      <c r="X100" s="3"/>
-    </row>
-    <row r="101" spans="3:24">
+        <v>1.2676814328358208</v>
+      </c>
+      <c r="X100" s="2"/>
+      <c r="Y100" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z100" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>120</v>
       </c>
@@ -3800,13 +3939,13 @@
         <v>1</v>
       </c>
       <c r="N101" s="2">
-        <v>0.22</v>
+        <v>0.19597000000000001</v>
       </c>
       <c r="O101" s="2">
-        <v>571.42999999999995</v>
+        <v>6.02</v>
       </c>
       <c r="P101" s="2">
-        <v>0.31</v>
+        <v>0.23</v>
       </c>
       <c r="R101" s="4">
         <f t="shared" si="3"/>
@@ -3818,23 +3957,32 @@
       </c>
       <c r="T101" s="2">
         <f t="shared" ref="T101:T102" si="9">N101+O101+P101</f>
-        <v>571.95999999999992</v>
+        <v>6.44597</v>
       </c>
       <c r="U101" s="2">
         <f t="shared" si="5"/>
-        <v>3.8606661818181816</v>
+        <v>4.334064193499005</v>
       </c>
       <c r="V101" s="2">
         <f t="shared" si="6"/>
-        <v>1.4863527641180896E-3</v>
+        <v>0.1410874684385382</v>
       </c>
       <c r="W101" s="2">
         <f t="shared" si="7"/>
-        <v>2.7398276129032255</v>
-      </c>
-      <c r="X101" s="3"/>
-    </row>
-    <row r="102" spans="3:24">
+        <v>3.6928111304347828</v>
+      </c>
+      <c r="X101" s="2"/>
+      <c r="Y101" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z101" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA101" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C102">
         <v>60</v>
       </c>
@@ -3869,13 +4017,13 @@
         <v>1</v>
       </c>
       <c r="N102" s="2">
-        <v>0.23</v>
+        <v>0.19139999999999999</v>
       </c>
       <c r="O102" s="2">
-        <v>0.22</v>
+        <v>0.24948000000000001</v>
       </c>
       <c r="P102" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="R102" s="4">
         <f t="shared" si="3"/>
@@ -3887,23 +4035,32 @@
       </c>
       <c r="T102" s="2">
         <f t="shared" si="9"/>
-        <v>0.74</v>
+        <v>0.64088000000000001</v>
       </c>
       <c r="U102" s="2">
         <f t="shared" si="5"/>
-        <v>3.6928111304347828</v>
+        <v>4.4375473354231971</v>
       </c>
       <c r="V102" s="2">
         <f t="shared" si="6"/>
-        <v>3.8606661818181816</v>
+        <v>3.4044675324675322</v>
       </c>
       <c r="W102" s="2">
         <f t="shared" si="7"/>
-        <v>2.9287812413793106</v>
-      </c>
-      <c r="X102" s="3"/>
-    </row>
-    <row r="103" spans="3:24">
+        <v>4.2467328000000002</v>
+      </c>
+      <c r="X102" s="2"/>
+      <c r="Y102" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z102" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA102" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>108</v>
       </c>
@@ -3940,11 +4097,11 @@
       <c r="N103" s="2">
         <v>0.04</v>
       </c>
-      <c r="O103" s="2" t="s">
-        <v>63</v>
+      <c r="O103" s="2">
+        <v>2.89</v>
       </c>
       <c r="P103" s="2">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="R103" s="4">
         <f t="shared" si="3"/>
@@ -3956,22 +4113,31 @@
       </c>
       <c r="T103" s="2">
         <f>N103+P103</f>
-        <v>0.13</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="U103" s="2">
         <f t="shared" si="5"/>
         <v>2.0155391999999996</v>
       </c>
       <c r="V103" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W103" s="2">
         <f t="shared" si="7"/>
-        <v>0.89579520000000012</v>
-      </c>
-      <c r="X103" s="3"/>
-    </row>
-    <row r="104" spans="3:24">
+        <v>1.1517366857142857</v>
+      </c>
+      <c r="X103" s="2"/>
+      <c r="Y103" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z103" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA103" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="104" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C104">
         <v>54</v>
       </c>
@@ -4006,13 +4172,13 @@
         <v>1</v>
       </c>
       <c r="N104" s="2">
-        <v>0.39754224852071013</v>
+        <v>0.66998999999999997</v>
       </c>
       <c r="O104" s="2">
-        <v>1</v>
+        <v>0.90490999999999999</v>
       </c>
       <c r="P104" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.53</v>
       </c>
       <c r="R104" s="4">
         <f t="shared" si="3"/>
@@ -4024,23 +4190,32 @@
       </c>
       <c r="T104" s="2">
         <f>N104+O104+P104</f>
-        <v>1.9775422485207099</v>
+        <v>2.1048999999999998</v>
       </c>
       <c r="U104" s="2">
         <f t="shared" si="5"/>
-        <v>4.3263999999999996</v>
+        <v>2.5670932163166618</v>
       </c>
       <c r="V104" s="2">
         <f t="shared" si="6"/>
-        <v>1.7199267840000001</v>
+        <v>1.9006606005017073</v>
       </c>
       <c r="W104" s="2">
         <f t="shared" si="7"/>
-        <v>2.9653910068965517</v>
-      </c>
-      <c r="X104" s="3"/>
-    </row>
-    <row r="105" spans="3:24">
+        <v>3.2451448754716981</v>
+      </c>
+      <c r="X104" s="2"/>
+      <c r="Y104" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z104" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>27</v>
       </c>
@@ -4075,13 +4250,13 @@
         <v>1</v>
       </c>
       <c r="N105" s="2">
-        <v>0.370266901466061</v>
+        <v>0.36105999999999999</v>
       </c>
       <c r="O105" s="2">
+        <v>0.44546999999999998</v>
+      </c>
+      <c r="P105" s="2">
         <v>0.44</v>
-      </c>
-      <c r="P105" s="2">
-        <v>0.6</v>
       </c>
       <c r="R105" s="4">
         <f t="shared" si="3"/>
@@ -4093,23 +4268,32 @@
       </c>
       <c r="T105" s="2">
         <f t="shared" ref="T105:T107" si="10">N105+O105+P105</f>
-        <v>1.4102669014660609</v>
+        <v>1.2465299999999999</v>
       </c>
       <c r="U105" s="2">
         <f t="shared" si="5"/>
-        <v>4.6451000000000002</v>
+        <v>4.763548396388412</v>
       </c>
       <c r="V105" s="2">
         <f t="shared" si="6"/>
-        <v>3.9089245090909093</v>
+        <v>3.8609261768469256</v>
       </c>
       <c r="W105" s="2">
         <f t="shared" si="7"/>
-        <v>2.8665446400000003</v>
-      </c>
-      <c r="X105" s="3"/>
-    </row>
-    <row r="106" spans="3:24">
+        <v>3.9089245090909093</v>
+      </c>
+      <c r="X105" s="2"/>
+      <c r="Y105" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z105" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>14</v>
       </c>
@@ -4144,13 +4328,13 @@
         <v>1</v>
       </c>
       <c r="N106" s="2">
-        <v>0.19962960455879811</v>
+        <v>0.19823000000000002</v>
       </c>
       <c r="O106" s="2">
-        <v>0.23</v>
+        <v>0.26186999999999999</v>
       </c>
       <c r="P106" s="2">
-        <v>0.35</v>
+        <v>0.21</v>
       </c>
       <c r="R106" s="4">
         <f t="shared" si="3"/>
@@ -4162,23 +4346,32 @@
       </c>
       <c r="T106" s="2">
         <f t="shared" si="10"/>
-        <v>0.77962960455879804</v>
+        <v>0.67010000000000003</v>
       </c>
       <c r="U106" s="2">
         <f t="shared" si="5"/>
-        <v>4.6327999999999996</v>
+        <v>4.6655099228169297</v>
       </c>
       <c r="V106" s="2">
         <f t="shared" si="6"/>
-        <v>4.0210610086956518</v>
+        <v>3.531691419406576</v>
       </c>
       <c r="W106" s="2">
         <f t="shared" si="7"/>
-        <v>2.64241152</v>
-      </c>
-      <c r="X106" s="3"/>
-    </row>
-    <row r="107" spans="3:24">
+        <v>4.4040191999999996</v>
+      </c>
+      <c r="X106" s="2"/>
+      <c r="Y106" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>7</v>
       </c>
@@ -4213,13 +4406,13 @@
         <v>1</v>
       </c>
       <c r="N107" s="2">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="O107" s="2">
-        <v>0.44</v>
+        <v>0.64302999999999999</v>
       </c>
       <c r="P107" s="2">
-        <v>0.32</v>
+        <v>0.23666000000000001</v>
       </c>
       <c r="R107" s="4">
         <f t="shared" si="3"/>
@@ -4231,23 +4424,32 @@
       </c>
       <c r="T107" s="2">
         <f t="shared" si="10"/>
-        <v>1.1200000000000001</v>
+        <v>1.1896900000000001</v>
       </c>
       <c r="U107" s="2">
         <f t="shared" si="5"/>
-        <v>2.5690111999999998</v>
+        <v>2.9833678451612906</v>
       </c>
       <c r="V107" s="2">
         <f t="shared" si="6"/>
-        <v>2.1019182545454544</v>
+        <v>1.4382595399903582</v>
       </c>
       <c r="W107" s="2">
         <f t="shared" si="7"/>
-        <v>2.8901376000000001</v>
-      </c>
-      <c r="X107" s="3"/>
-    </row>
-    <row r="108" spans="3:24">
+        <v>3.9079017662469364</v>
+      </c>
+      <c r="X107" s="2"/>
+      <c r="Y107" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z107" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>224</v>
       </c>
@@ -4282,13 +4484,13 @@
         <v>1</v>
       </c>
       <c r="N108" s="2">
-        <v>1.18</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P108" s="2">
-        <v>1.94</v>
+        <v>1.87</v>
       </c>
       <c r="R108" s="4">
         <f t="shared" si="3"/>
@@ -4300,22 +4502,31 @@
       </c>
       <c r="T108" s="2">
         <f>N108+P108</f>
-        <v>3.12</v>
+        <v>3</v>
       </c>
       <c r="U108" s="2">
         <f t="shared" si="5"/>
-        <v>1.175649193220339</v>
+        <v>1.2276690690265488</v>
       </c>
       <c r="V108" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W108" s="2">
         <f t="shared" si="7"/>
-        <v>0.71508559175257735</v>
-      </c>
-      <c r="X108" s="3"/>
-    </row>
-    <row r="109" spans="3:24">
+        <v>0.7418535016042781</v>
+      </c>
+      <c r="X108" s="2"/>
+      <c r="Y108" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z108" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>112</v>
       </c>
@@ -4350,13 +4561,13 @@
         <v>1</v>
       </c>
       <c r="N109" s="2">
-        <v>3.54</v>
+        <v>3.38</v>
       </c>
       <c r="O109" s="2">
-        <v>5.48</v>
+        <v>7.2712000000000003</v>
       </c>
       <c r="P109" s="2">
-        <v>4.75</v>
+        <v>4.66</v>
       </c>
       <c r="R109" s="4">
         <f t="shared" si="3"/>
@@ -4368,23 +4579,32 @@
       </c>
       <c r="T109" s="2">
         <f>N109+O109+P109</f>
-        <v>13.77</v>
+        <v>15.311199999999999</v>
       </c>
       <c r="U109" s="2">
         <f t="shared" si="5"/>
-        <v>4.1800860203389831</v>
+        <v>4.3779599147928998</v>
       </c>
       <c r="V109" s="2">
         <f t="shared" si="6"/>
-        <v>2.7002745459854012</v>
+        <v>2.0350842380899987</v>
       </c>
       <c r="W109" s="2">
         <f t="shared" si="7"/>
-        <v>3.1152641077894736</v>
-      </c>
-      <c r="X109" s="3"/>
-    </row>
-    <row r="110" spans="3:24">
+        <v>3.1754301527896995</v>
+      </c>
+      <c r="X109" s="2"/>
+      <c r="Y109" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z109" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="110" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C110">
         <f>112/2</f>
         <v>56</v>
@@ -4420,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="N110" s="2">
-        <v>3.48</v>
+        <v>3.25</v>
       </c>
       <c r="O110" s="2">
-        <v>4.09</v>
+        <v>3.67</v>
       </c>
       <c r="P110" s="2">
-        <v>4.33</v>
+        <v>3.93</v>
       </c>
       <c r="R110" s="4">
         <f t="shared" si="3"/>
@@ -4438,23 +4658,32 @@
       </c>
       <c r="T110" s="2">
         <f t="shared" ref="T110:T113" si="11">N110+O110+P110</f>
-        <v>11.9</v>
+        <v>10.85</v>
       </c>
       <c r="U110" s="2">
         <f t="shared" si="5"/>
-        <v>4.2521564689655174</v>
+        <v>4.5530783113846152</v>
       </c>
       <c r="V110" s="2">
         <f t="shared" si="6"/>
-        <v>3.6179717633251838</v>
+        <v>4.0320175782016348</v>
       </c>
       <c r="W110" s="2">
         <f t="shared" si="7"/>
-        <v>3.417437531639723</v>
-      </c>
-      <c r="X110" s="3"/>
-    </row>
-    <row r="111" spans="3:24">
+        <v>3.7652683236641216</v>
+      </c>
+      <c r="X110" s="2"/>
+      <c r="Y110" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z110" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA110" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="111" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C111">
         <f>56/2</f>
         <v>28</v>
@@ -4490,13 +4719,13 @@
         <v>1</v>
       </c>
       <c r="N111" s="2">
-        <v>3.3200000000000003</v>
+        <v>3.06</v>
       </c>
       <c r="O111" s="2">
-        <v>3.71</v>
+        <v>3.7976000000000001</v>
       </c>
       <c r="P111" s="2">
-        <v>3.84</v>
+        <v>3.62</v>
       </c>
       <c r="R111" s="4">
         <f t="shared" si="3"/>
@@ -4508,23 +4737,32 @@
       </c>
       <c r="T111" s="2">
         <f t="shared" si="11"/>
-        <v>10.870000000000001</v>
+        <v>10.477599999999999</v>
       </c>
       <c r="U111" s="2">
         <f t="shared" si="5"/>
-        <v>4.4570796722891561</v>
+        <v>4.8357857882352944</v>
       </c>
       <c r="V111" s="2">
         <f t="shared" si="6"/>
-        <v>3.9885456905660379</v>
+        <v>3.8965411080682539</v>
       </c>
       <c r="W111" s="2">
         <f t="shared" si="7"/>
-        <v>3.8535168000000004</v>
-      </c>
-      <c r="X111" s="3"/>
-    </row>
-    <row r="112" spans="3:24">
+        <v>4.0877084287292815</v>
+      </c>
+      <c r="X111" s="2"/>
+      <c r="Y111" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z111" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA111" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C112">
         <v>14</v>
       </c>
@@ -4559,13 +4797,13 @@
         <v>1</v>
       </c>
       <c r="N112" s="2">
-        <v>1.78</v>
+        <v>1.62</v>
       </c>
       <c r="O112" s="2">
-        <v>2</v>
+        <v>2.2144999999999997</v>
       </c>
       <c r="P112" s="2">
-        <v>2.2599999999999998</v>
+        <v>1.89</v>
       </c>
       <c r="R112" s="4">
         <f t="shared" si="3"/>
@@ -4577,23 +4815,32 @@
       </c>
       <c r="T112" s="2">
         <f t="shared" si="11"/>
-        <v>6.04</v>
+        <v>5.7244999999999999</v>
       </c>
       <c r="U112" s="2">
         <f t="shared" si="5"/>
-        <v>4.1566023910112362</v>
+        <v>4.5671310222222221</v>
       </c>
       <c r="V112" s="2">
         <f t="shared" si="6"/>
-        <v>3.6993761279999999</v>
+        <v>3.3410486592910367</v>
       </c>
       <c r="W112" s="2">
         <f t="shared" si="7"/>
-        <v>3.2737841840707969</v>
-      </c>
-      <c r="X112" s="3"/>
-    </row>
-    <row r="113" spans="3:24">
+        <v>3.9146837333333333</v>
+      </c>
+      <c r="X112" s="2"/>
+      <c r="Y112" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z112" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA112" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="113" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C113">
         <v>7</v>
       </c>
@@ -4628,13 +4875,13 @@
         <v>1</v>
       </c>
       <c r="N113" s="2">
-        <v>0.84</v>
+        <v>0.75</v>
       </c>
       <c r="O113" s="2">
-        <v>0.91</v>
+        <v>1.2293000000000001</v>
       </c>
       <c r="P113" s="2">
-        <v>0.65</v>
+        <v>0.48768</v>
       </c>
       <c r="R113" s="4">
         <f t="shared" si="3"/>
@@ -4646,23 +4893,32 @@
       </c>
       <c r="T113" s="2">
         <f t="shared" si="11"/>
-        <v>2.4</v>
+        <v>2.46698</v>
       </c>
       <c r="U113" s="2">
         <f t="shared" si="5"/>
-        <v>2.2020095999999998</v>
+        <v>2.4662507520000001</v>
       </c>
       <c r="V113" s="2">
         <f t="shared" si="6"/>
-        <v>2.0326242461538464</v>
+        <v>1.5046677491255185</v>
       </c>
       <c r="W113" s="2">
         <f t="shared" si="7"/>
-        <v>2.8456739446153847</v>
-      </c>
-      <c r="X113" s="3"/>
-    </row>
-    <row r="114" spans="3:24">
+        <v>3.7928314960629921</v>
+      </c>
+      <c r="X113" s="2"/>
+      <c r="Y113" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA113" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C114">
         <v>224</v>
       </c>
@@ -4697,13 +4953,13 @@
         <v>1</v>
       </c>
       <c r="N114" s="2">
-        <v>2.2800000000000002</v>
+        <v>2.19</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P114" s="2">
-        <v>2.08</v>
+        <v>1.98</v>
       </c>
       <c r="R114" s="4">
         <f t="shared" si="3"/>
@@ -4715,22 +4971,31 @@
       </c>
       <c r="T114" s="2">
         <f>N114+P114</f>
-        <v>4.3600000000000003</v>
+        <v>4.17</v>
       </c>
       <c r="U114" s="2">
         <f t="shared" si="5"/>
-        <v>1.2169000421052629</v>
+        <v>1.2669096328767122</v>
       </c>
       <c r="V114" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W114" s="2">
         <f t="shared" si="7"/>
-        <v>1.3339096615384614</v>
-      </c>
-      <c r="X114" s="3"/>
-    </row>
-    <row r="115" spans="3:24">
+        <v>1.4012788363636364</v>
+      </c>
+      <c r="X114" s="2"/>
+      <c r="Y114" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z114" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA114" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C115">
         <v>112</v>
       </c>
@@ -4765,13 +5030,13 @@
         <v>1</v>
       </c>
       <c r="N115" s="2">
-        <v>7.07</v>
+        <v>6.86</v>
       </c>
       <c r="O115" s="2">
-        <v>10.58</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="P115" s="2">
-        <v>9.25</v>
+        <v>9.17</v>
       </c>
       <c r="R115" s="4">
         <f t="shared" si="3"/>
@@ -4783,23 +5048,32 @@
       </c>
       <c r="T115" s="2">
         <f>N115+O115+P115</f>
-        <v>26.9</v>
+        <v>25.229999999999997</v>
       </c>
       <c r="U115" s="2">
         <f t="shared" si="5"/>
-        <v>4.185998447524752</v>
+        <v>4.3141412571428566</v>
       </c>
       <c r="V115" s="2">
         <f t="shared" si="6"/>
-        <v>2.7972598321361053</v>
+        <v>3.2168488069565218</v>
       </c>
       <c r="W115" s="2">
         <f t="shared" si="7"/>
-        <v>3.1994604350270275</v>
-      </c>
-      <c r="X115" s="3"/>
-    </row>
-    <row r="116" spans="3:24">
+        <v>3.2273728488549618</v>
+      </c>
+      <c r="X115" s="2"/>
+      <c r="Y115" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA115" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C116">
         <f>112/2</f>
         <v>56</v>
@@ -4835,13 +5109,13 @@
         <v>1</v>
       </c>
       <c r="N116" s="2">
-        <v>6.72</v>
+        <v>6.44</v>
       </c>
       <c r="O116" s="2">
-        <v>8.27</v>
+        <v>7.44</v>
       </c>
       <c r="P116" s="2">
-        <v>8.36</v>
+        <v>7.84</v>
       </c>
       <c r="R116" s="4">
         <f t="shared" si="3"/>
@@ -4853,23 +5127,32 @@
       </c>
       <c r="T116" s="2">
         <f t="shared" ref="T116:T119" si="12">N116+O116+P116</f>
-        <v>23.349999999999998</v>
+        <v>21.72</v>
       </c>
       <c r="U116" s="2">
         <f t="shared" si="5"/>
-        <v>4.4040191999999996</v>
+        <v>4.5954982956521739</v>
       </c>
       <c r="V116" s="2">
         <f t="shared" si="6"/>
-        <v>3.5785984309552603</v>
+        <v>3.9778237935483869</v>
       </c>
       <c r="W116" s="2">
         <f t="shared" si="7"/>
-        <v>3.5400728497607656</v>
-      </c>
-      <c r="X116" s="3"/>
-    </row>
-    <row r="117" spans="3:24">
+        <v>3.7748735999999998</v>
+      </c>
+      <c r="X116" s="2"/>
+      <c r="Y116" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z116" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA116" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="117" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C117">
         <f>56/2</f>
         <v>28</v>
@@ -4905,13 +5188,13 @@
         <v>1</v>
       </c>
       <c r="N117" s="2">
-        <v>6.41</v>
+        <v>6.07</v>
       </c>
       <c r="O117" s="2">
-        <v>7.41</v>
+        <v>7.4197999999999995</v>
       </c>
       <c r="P117" s="2">
-        <v>7.61</v>
+        <v>7.22</v>
       </c>
       <c r="R117" s="4">
         <f t="shared" si="3"/>
@@ -4923,23 +5206,32 @@
       </c>
       <c r="T117" s="2">
         <f t="shared" si="12"/>
-        <v>21.43</v>
+        <v>20.709799999999998</v>
       </c>
       <c r="U117" s="2">
         <f t="shared" si="5"/>
-        <v>4.6170060879875194</v>
+        <v>4.87561927907743</v>
       </c>
       <c r="V117" s="2">
         <f t="shared" si="6"/>
-        <v>3.9939283433198378</v>
+        <v>3.9886532014340008</v>
       </c>
       <c r="W117" s="2">
         <f t="shared" si="7"/>
-        <v>3.8889630780551903</v>
-      </c>
-      <c r="X117" s="3"/>
-    </row>
-    <row r="118" spans="3:24">
+        <v>4.0990317207756233</v>
+      </c>
+      <c r="X117" s="2"/>
+      <c r="Y117" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z117" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA117" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="118" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C118">
         <v>14</v>
       </c>
@@ -4974,13 +5266,13 @@
         <v>1</v>
       </c>
       <c r="N118" s="2">
-        <v>3.41</v>
+        <v>3.19</v>
       </c>
       <c r="O118" s="2">
-        <v>3.92</v>
+        <v>4.0324</v>
       </c>
       <c r="P118" s="2">
-        <v>4.3600000000000003</v>
+        <v>3.72</v>
       </c>
       <c r="R118" s="4">
         <f t="shared" si="3"/>
@@ -4992,23 +5284,32 @@
       </c>
       <c r="T118" s="2">
         <f t="shared" si="12"/>
-        <v>11.690000000000001</v>
+        <v>10.942400000000001</v>
       </c>
       <c r="U118" s="2">
         <f t="shared" si="5"/>
-        <v>4.3394441384164217</v>
+        <v>4.6387161479623815</v>
       </c>
       <c r="V118" s="2">
         <f t="shared" si="6"/>
-        <v>3.7748735999999998</v>
+        <v>3.6696519472274574</v>
       </c>
       <c r="W118" s="2">
         <f t="shared" si="7"/>
-        <v>3.3939230532110094</v>
-      </c>
-      <c r="X118" s="3"/>
-    </row>
-    <row r="119" spans="3:24">
+        <v>3.9778237935483869</v>
+      </c>
+      <c r="X118" s="2"/>
+      <c r="Y118" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z118" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA118" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="119" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C119">
         <v>7</v>
       </c>
@@ -5043,13 +5344,13 @@
         <v>1</v>
       </c>
       <c r="N119" s="2">
-        <v>1.61</v>
+        <v>1.46</v>
       </c>
       <c r="O119" s="2">
-        <v>1.74</v>
+        <v>2.0040999999999998</v>
       </c>
       <c r="P119" s="2">
-        <v>1.2</v>
+        <v>0.95377999999999996</v>
       </c>
       <c r="R119" s="4">
         <f t="shared" si="3"/>
@@ -5061,23 +5362,32 @@
       </c>
       <c r="T119" s="2">
         <f t="shared" si="12"/>
-        <v>4.55</v>
+        <v>4.4178799999999994</v>
       </c>
       <c r="U119" s="2">
         <f t="shared" si="5"/>
-        <v>2.297749147826087</v>
+        <v>2.5338192657534249</v>
       </c>
       <c r="V119" s="2">
         <f t="shared" si="6"/>
-        <v>2.1260782344827587</v>
+        <v>1.8459039608801955</v>
       </c>
       <c r="W119" s="2">
         <f t="shared" si="7"/>
-        <v>3.0828134400000007</v>
-      </c>
-      <c r="X119" s="3"/>
-    </row>
-    <row r="120" spans="3:24">
+        <v>3.87864720166076</v>
+      </c>
+      <c r="X119" s="2"/>
+      <c r="Y119" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z119" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA119" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="120" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C120">
         <v>224</v>
       </c>
@@ -5112,13 +5422,13 @@
         <v>2</v>
       </c>
       <c r="N120" s="2">
-        <v>1.48</v>
+        <v>1.1554</v>
       </c>
       <c r="O120" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P120" s="2">
-        <v>1.6</v>
+        <v>1.53</v>
       </c>
       <c r="R120" s="4">
         <f t="shared" si="3"/>
@@ -5130,22 +5440,31 @@
       </c>
       <c r="T120" s="2">
         <f>N120+P120</f>
-        <v>3.08</v>
+        <v>2.6854</v>
       </c>
       <c r="U120" s="2">
         <f t="shared" si="5"/>
-        <v>2.5516530162162163</v>
+        <v>3.2685186636662626</v>
       </c>
       <c r="V120" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W120" s="2">
         <f t="shared" si="7"/>
-        <v>2.36027904</v>
-      </c>
-      <c r="X120" s="3"/>
-    </row>
-    <row r="121" spans="3:24">
+        <v>2.4682656627450976</v>
+      </c>
+      <c r="X120" s="2"/>
+      <c r="Y120" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z120" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA120" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>28</v>
       </c>
@@ -5180,13 +5499,13 @@
         <v>1</v>
       </c>
       <c r="N121" s="2">
-        <v>0.89871654461495409</v>
+        <v>1.3607</v>
       </c>
       <c r="O121" s="2">
-        <v>0.88</v>
+        <v>0.89434000000000002</v>
       </c>
       <c r="P121" s="2">
-        <v>1.3</v>
+        <v>1.24</v>
       </c>
       <c r="R121" s="4">
         <f t="shared" si="3"/>
@@ -5198,23 +5517,32 @@
       </c>
       <c r="T121" s="2">
         <f>N121+O121+P121</f>
-        <v>3.078716544614954</v>
+        <v>3.4950400000000004</v>
       </c>
       <c r="U121" s="2">
         <f t="shared" si="5"/>
-        <v>4.2877999999999998</v>
+        <v>2.8320105827882704</v>
       </c>
       <c r="V121" s="2">
         <f t="shared" si="6"/>
-        <v>4.3789963636363636</v>
+        <v>4.3087827895431268</v>
       </c>
       <c r="W121" s="2">
         <f t="shared" si="7"/>
-        <v>2.9642436923076922</v>
-      </c>
-      <c r="X121" s="3"/>
-    </row>
-    <row r="122" spans="3:24">
+        <v>3.1076748387096771</v>
+      </c>
+      <c r="X121" s="2"/>
+      <c r="Y121" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z121" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA121" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C122">
         <v>28</v>
       </c>
@@ -5249,13 +5577,13 @@
         <v>1</v>
       </c>
       <c r="N122" s="2">
-        <v>0.1078246105417789</v>
+        <v>0.09</v>
       </c>
       <c r="O122" s="2">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="P122" s="2">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="R122" s="4">
         <f t="shared" si="3"/>
@@ -5267,23 +5595,32 @@
       </c>
       <c r="T122" s="2">
         <f t="shared" ref="T122:T126" si="13">N122+O122+P122</f>
-        <v>0.59782461054177882</v>
+        <v>0.7</v>
       </c>
       <c r="U122" s="2">
         <f t="shared" si="5"/>
-        <v>2.8590999999999993</v>
+        <v>3.425348266666667</v>
       </c>
       <c r="V122" s="2">
         <f t="shared" si="6"/>
-        <v>1.622533389473684</v>
+        <v>1.9267583999999998</v>
       </c>
       <c r="W122" s="2">
         <f t="shared" si="7"/>
-        <v>1.0276044800000002</v>
-      </c>
-      <c r="X122" s="3"/>
-    </row>
-    <row r="123" spans="3:24">
+        <v>0.68506965333333336</v>
+      </c>
+      <c r="X122" s="2"/>
+      <c r="Y122" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z122" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA122" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="123" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C123">
         <v>14</v>
       </c>
@@ -5318,13 +5655,13 @@
         <v>1</v>
       </c>
       <c r="N123" s="2">
-        <v>1.21</v>
+        <v>1.07</v>
       </c>
       <c r="O123" s="2">
-        <v>0.92</v>
+        <v>1.0742</v>
       </c>
       <c r="P123" s="2">
-        <v>1.01</v>
+        <v>0.89</v>
       </c>
       <c r="R123" s="4">
         <f t="shared" si="3"/>
@@ -5336,23 +5673,32 @@
       </c>
       <c r="T123" s="2">
         <f t="shared" si="13"/>
-        <v>3.1399999999999997</v>
+        <v>3.0342000000000002</v>
       </c>
       <c r="U123" s="2">
         <f t="shared" si="5"/>
-        <v>3.1847246280991737</v>
+        <v>3.6014175700934579</v>
       </c>
       <c r="V123" s="2">
         <f t="shared" si="6"/>
-        <v>4.188605217391304</v>
+        <v>3.5873364364177993</v>
       </c>
       <c r="W123" s="2">
         <f t="shared" si="7"/>
-        <v>3.8153631683168316</v>
-      </c>
-      <c r="X123" s="3"/>
-    </row>
-    <row r="124" spans="3:24">
+        <v>4.3297941573033709</v>
+      </c>
+      <c r="X123" s="2"/>
+      <c r="Y123" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z123" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA123" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="124" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C124">
         <v>14</v>
       </c>
@@ -5387,13 +5733,13 @@
         <v>1</v>
       </c>
       <c r="N124" s="2">
-        <v>0.179724447035504</v>
+        <v>0.18</v>
       </c>
       <c r="O124" s="2">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="P124" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="R124" s="4">
         <f t="shared" si="3"/>
@@ -5405,23 +5751,32 @@
       </c>
       <c r="T124" s="2">
         <f t="shared" si="13"/>
-        <v>1.019724447035504</v>
+        <v>0.99</v>
       </c>
       <c r="U124" s="2">
         <f t="shared" si="5"/>
-        <v>3.4306000000000001</v>
+        <v>3.425348266666667</v>
       </c>
       <c r="V124" s="2">
         <f t="shared" si="6"/>
-        <v>2.3713949538461532</v>
+        <v>2.5690111999999998</v>
       </c>
       <c r="W124" s="2">
         <f t="shared" si="7"/>
-        <v>1.0630391172413793</v>
-      </c>
-      <c r="X124" s="3"/>
-    </row>
-    <row r="125" spans="3:24">
+        <v>1.0816889263157896</v>
+      </c>
+      <c r="X124" s="2"/>
+      <c r="Y124" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z124" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA124" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C125">
         <v>7</v>
       </c>
@@ -5456,13 +5811,13 @@
         <v>1</v>
       </c>
       <c r="N125" s="2">
-        <v>0.15741490196078431</v>
+        <v>0.2</v>
       </c>
       <c r="O125" s="2">
-        <v>0.22</v>
+        <v>0.20283999999999999</v>
       </c>
       <c r="P125" s="2">
-        <v>0.38</v>
+        <v>0.21312</v>
       </c>
       <c r="R125" s="4">
         <f t="shared" si="3"/>
@@ -5474,23 +5829,32 @@
       </c>
       <c r="T125" s="2">
         <f t="shared" si="13"/>
-        <v>0.75741490196078431</v>
+        <v>0.61595999999999995</v>
       </c>
       <c r="U125" s="2">
         <f t="shared" si="5"/>
-        <v>2.1215999999999999</v>
+        <v>1.66985728</v>
       </c>
       <c r="V125" s="2">
         <f t="shared" si="6"/>
-        <v>1.5180520727272726</v>
+        <v>1.6464773023072372</v>
       </c>
       <c r="W125" s="2">
         <f t="shared" si="7"/>
-        <v>0.87887225263157887</v>
-      </c>
-      <c r="X125" s="3"/>
-    </row>
-    <row r="126" spans="3:24">
+        <v>1.5670582582582584</v>
+      </c>
+      <c r="X125" s="2"/>
+      <c r="Y125" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z125" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA125" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C126">
         <v>7</v>
       </c>
@@ -5525,13 +5889,13 @@
         <v>1</v>
       </c>
       <c r="N126" s="2">
-        <v>1.93</v>
+        <v>1.7</v>
       </c>
       <c r="O126" s="2">
-        <v>1.77</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="P126" s="2">
-        <v>1.27</v>
+        <v>1.0803</v>
       </c>
       <c r="R126" s="4">
         <f t="shared" si="3"/>
@@ -5543,31 +5907,40 @@
       </c>
       <c r="T126" s="2">
         <f t="shared" si="13"/>
-        <v>4.9700000000000006</v>
+        <v>4.9583000000000004</v>
       </c>
       <c r="U126" s="2">
         <f t="shared" si="5"/>
-        <v>2.1630275647668396</v>
+        <v>2.4556724705882353</v>
       </c>
       <c r="V126" s="2">
         <f t="shared" si="6"/>
-        <v>2.3585554802259887</v>
+        <v>1.9167324150596881</v>
       </c>
       <c r="W126" s="2">
         <f t="shared" si="7"/>
-        <v>3.2871206299212599</v>
-      </c>
-      <c r="X126" s="3"/>
-    </row>
-    <row r="129" spans="1:12">
+        <v>3.8643369434416366</v>
+      </c>
+      <c r="X126" s="2"/>
+      <c r="Y126" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA126" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L135" s="1"/>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -5593,7 +5966,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C138">
         <v>1760</v>
       </c>
@@ -5608,7 +5981,7 @@
       <c r="I138" s="9"/>
       <c r="J138" s="9"/>
     </row>
-    <row r="139" spans="1:12">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C139">
         <v>1760</v>
       </c>
@@ -5623,7 +5996,7 @@
       <c r="I139" s="9"/>
       <c r="J139" s="9"/>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C140">
         <v>1760</v>
       </c>
@@ -5638,7 +6011,7 @@
       <c r="I140" s="9"/>
       <c r="J140" s="9"/>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C141">
         <v>1760</v>
       </c>
@@ -5653,7 +6026,7 @@
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C142">
         <v>2048</v>
       </c>
@@ -5668,7 +6041,7 @@
       <c r="I142" s="9"/>
       <c r="J142" s="9"/>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C143">
         <v>2048</v>
       </c>
@@ -5683,7 +6056,7 @@
       <c r="I143" s="9"/>
       <c r="J143" s="9"/>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C144">
         <v>2048</v>
       </c>
@@ -5698,7 +6071,7 @@
       <c r="I144" s="9"/>
       <c r="J144" s="9"/>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C145">
         <v>2048</v>
       </c>
@@ -5713,7 +6086,7 @@
       <c r="I145" s="9"/>
       <c r="J145" s="9"/>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C146">
         <v>2560</v>
       </c>
@@ -5728,7 +6101,7 @@
       <c r="I146" s="9"/>
       <c r="J146" s="9"/>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C147">
         <v>2560</v>
       </c>
@@ -5743,7 +6116,7 @@
       <c r="I147" s="9"/>
       <c r="J147" s="9"/>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C148">
         <v>2560</v>
       </c>
@@ -5758,7 +6131,7 @@
       <c r="I148" s="9"/>
       <c r="J148" s="9"/>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C149">
         <v>2560</v>
       </c>
@@ -5773,10 +6146,10 @@
       <c r="I149" s="9"/>
       <c r="J149" s="9"/>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I151" s="1"/>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -5802,7 +6175,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C154">
         <v>512</v>
       </c>
@@ -5817,7 +6190,7 @@
       <c r="I154" s="9"/>
       <c r="J154" s="9"/>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C155">
         <v>512</v>
       </c>
@@ -5832,7 +6205,7 @@
       <c r="I155" s="9"/>
       <c r="J155" s="9"/>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C156">
         <v>512</v>
       </c>
@@ -5847,7 +6220,7 @@
       <c r="I156" s="9"/>
       <c r="J156" s="9"/>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C157">
         <v>512</v>
       </c>
@@ -5862,7 +6235,7 @@
       <c r="I157" s="9"/>
       <c r="J157" s="9"/>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C158">
         <v>1024</v>
       </c>
@@ -5877,7 +6250,7 @@
       <c r="I158" s="9"/>
       <c r="J158" s="9"/>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C159">
         <v>1024</v>
       </c>
@@ -5892,7 +6265,7 @@
       <c r="I159" s="9"/>
       <c r="J159" s="9"/>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C160">
         <v>1024</v>
       </c>
@@ -5907,7 +6280,7 @@
       <c r="I160" s="9"/>
       <c r="J160" s="9"/>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C161">
         <v>1024</v>
       </c>
@@ -5922,7 +6295,7 @@
       <c r="I161" s="9"/>
       <c r="J161" s="9"/>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C162">
         <v>2048</v>
       </c>
@@ -5937,7 +6310,7 @@
       <c r="I162" s="9"/>
       <c r="J162" s="9"/>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C163">
         <v>2048</v>
       </c>
@@ -5952,7 +6325,7 @@
       <c r="I163" s="9"/>
       <c r="J163" s="9"/>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C164">
         <v>2048</v>
       </c>
@@ -5967,7 +6340,7 @@
       <c r="I164" s="9"/>
       <c r="J164" s="9"/>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C165">
         <v>2048</v>
       </c>
@@ -5982,7 +6355,7 @@
       <c r="I165" s="9"/>
       <c r="J165" s="9"/>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C166">
         <v>4096</v>
       </c>
@@ -5997,7 +6370,7 @@
       <c r="I166" s="9"/>
       <c r="J166" s="9"/>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C167">
         <v>4096</v>
       </c>
@@ -6012,7 +6385,7 @@
       <c r="I167" s="9"/>
       <c r="J167" s="9"/>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C168">
         <v>4096</v>
       </c>
@@ -6027,7 +6400,7 @@
       <c r="I168" s="9"/>
       <c r="J168" s="9"/>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C169">
         <v>4096</v>
       </c>
@@ -6042,16 +6415,16 @@
       <c r="I169" s="9"/>
       <c r="J169" s="9"/>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I171" s="1"/>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
       <c r="K172" s="2"/>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>4</v>
       </c>
@@ -6074,7 +6447,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C175">
         <v>100000</v>
       </c>
@@ -6099,7 +6472,7 @@
       <c r="N175" s="2"/>
       <c r="O175" s="2"/>
     </row>
-    <row r="176" spans="1:15">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C176">
         <v>100000</v>
       </c>
@@ -6124,7 +6497,7 @@
       <c r="N176" s="2"/>
       <c r="O176" s="2"/>
     </row>
-    <row r="177" spans="3:15">
+    <row r="177" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C177">
         <v>100000</v>
       </c>
@@ -6149,7 +6522,7 @@
       <c r="N177" s="2"/>
       <c r="O177" s="2"/>
     </row>
-    <row r="178" spans="3:15">
+    <row r="178" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C178">
         <v>100000</v>
       </c>
@@ -6174,7 +6547,7 @@
       </c>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="3:15">
+    <row r="179" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C179">
         <v>100000</v>
       </c>
@@ -6199,7 +6572,7 @@
       </c>
       <c r="L179" s="2"/>
     </row>
-    <row r="180" spans="3:15">
+    <row r="180" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C180">
         <v>3097600</v>
       </c>
@@ -6224,7 +6597,7 @@
       <c r="N180" s="2"/>
       <c r="O180" s="2"/>
     </row>
-    <row r="181" spans="3:15">
+    <row r="181" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C181">
         <f>1760*1760</f>
         <v>3097600</v>
@@ -6250,7 +6623,7 @@
       <c r="N181" s="2"/>
       <c r="O181" s="2"/>
     </row>
-    <row r="182" spans="3:15">
+    <row r="182" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C182">
         <f>1760*1760</f>
         <v>3097600</v>
@@ -6276,7 +6649,7 @@
       <c r="N182" s="2"/>
       <c r="O182" s="2"/>
     </row>
-    <row r="183" spans="3:15">
+    <row r="183" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C183">
         <v>3097600</v>
       </c>
@@ -6301,7 +6674,7 @@
       </c>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="3:15">
+    <row r="184" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C184">
         <v>3097600</v>
       </c>
@@ -6326,7 +6699,7 @@
       </c>
       <c r="L184" s="2"/>
     </row>
-    <row r="185" spans="3:15">
+    <row r="185" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C185">
         <v>4194304</v>
       </c>
@@ -6351,7 +6724,7 @@
       <c r="N185" s="2"/>
       <c r="O185" s="2"/>
     </row>
-    <row r="186" spans="3:15">
+    <row r="186" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C186">
         <f>2048*2048</f>
         <v>4194304</v>
@@ -6377,7 +6750,7 @@
       <c r="N186" s="2"/>
       <c r="O186" s="2"/>
     </row>
-    <row r="187" spans="3:15">
+    <row r="187" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C187">
         <f>2048*2048</f>
         <v>4194304</v>
@@ -6403,7 +6776,7 @@
       <c r="N187" s="2"/>
       <c r="O187" s="2"/>
     </row>
-    <row r="188" spans="3:15">
+    <row r="188" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C188">
         <v>4194304</v>
       </c>
@@ -6429,7 +6802,7 @@
       <c r="L188" s="2"/>
       <c r="O188" s="2"/>
     </row>
-    <row r="189" spans="3:15">
+    <row r="189" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C189">
         <v>4194304</v>
       </c>
@@ -6455,7 +6828,7 @@
       <c r="L189" s="2"/>
       <c r="O189" s="2"/>
     </row>
-    <row r="190" spans="3:15">
+    <row r="190" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C190">
         <v>6553600</v>
       </c>
@@ -6480,7 +6853,7 @@
       <c r="N190" s="2"/>
       <c r="O190" s="2"/>
     </row>
-    <row r="191" spans="3:15">
+    <row r="191" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C191">
         <f>2560*2560</f>
         <v>6553600</v>
@@ -6506,7 +6879,7 @@
       <c r="N191" s="2"/>
       <c r="O191" s="2"/>
     </row>
-    <row r="192" spans="3:15">
+    <row r="192" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C192">
         <f>2560*2560</f>
         <v>6553600</v>
@@ -6532,7 +6905,7 @@
       <c r="N192" s="2"/>
       <c r="O192" s="2"/>
     </row>
-    <row r="193" spans="3:16">
+    <row r="193" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C193">
         <v>6553600</v>
       </c>
@@ -6557,7 +6930,7 @@
       </c>
       <c r="L193" s="2"/>
     </row>
-    <row r="194" spans="3:16">
+    <row r="194" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C194">
         <v>6553600</v>
       </c>
@@ -6582,7 +6955,7 @@
       </c>
       <c r="L194" s="2"/>
     </row>
-    <row r="195" spans="3:16">
+    <row r="195" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C195">
         <f t="shared" ref="C195:C197" si="15">4096*4096</f>
         <v>16777216</v>
@@ -6608,7 +6981,7 @@
       <c r="N195" s="2"/>
       <c r="O195" s="2"/>
     </row>
-    <row r="196" spans="3:16">
+    <row r="196" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C196">
         <f t="shared" si="15"/>
         <v>16777216</v>
@@ -6634,7 +7007,7 @@
       <c r="N196" s="2"/>
       <c r="O196" s="2"/>
     </row>
-    <row r="197" spans="3:16">
+    <row r="197" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C197">
         <f t="shared" si="15"/>
         <v>16777216</v>
@@ -6660,7 +7033,7 @@
       <c r="N197" s="2"/>
       <c r="O197" s="2"/>
     </row>
-    <row r="198" spans="3:16">
+    <row r="198" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C198">
         <v>16777216</v>
       </c>
@@ -6687,7 +7060,7 @@
       <c r="L198" s="2"/>
       <c r="N198" s="2"/>
     </row>
-    <row r="199" spans="3:16">
+    <row r="199" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C199">
         <v>16777216</v>
       </c>
@@ -6714,7 +7087,7 @@
       <c r="L199" s="2"/>
       <c r="N199" s="2"/>
     </row>
-    <row r="200" spans="3:16">
+    <row r="200" spans="3:16" x14ac:dyDescent="0.25">
       <c r="I200" s="2"/>
       <c r="J200" s="2"/>
       <c r="K200" s="2"/>
@@ -6724,10 +7097,10 @@
       <c r="O200" s="2"/>
       <c r="P200" s="2"/>
     </row>
-    <row r="201" spans="3:16">
+    <row r="201" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G201" s="1"/>
     </row>
-    <row r="207" spans="3:16">
+    <row r="207" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G207" s="1"/>
     </row>
   </sheetData>
@@ -6743,35 +7116,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -6779,48 +7152,57 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated KNL numbers with latest version of MKL and libxsmm (#14)
* + Fixed padding for the convolution kernels
+ Modified libxsmm_conv run script to directly call samples/dnn/ script
+ Added MKLML support for MKL convolutions

* Modified prepare_mkl.sh and Makfile

- Remove downloading of MKLML package.
- Dynamic linking of Intel MKL and MKLML

* minor fix - cleanup

* Updated results with MKL-2017 GOLD update 1 numbers
</commit_message>
<xml_diff>
--- a/results/DeepBench_IA_KNL7250.xlsx
+++ b/results/DeepBench_IA_KNL7250.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmudiger\Documents\Work\DL\DeepBench\my_DeepBench_gh_pub\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="25040" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="555" yWindow="0" windowWidth="25035" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Specs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="72">
   <si>
     <t xml:space="preserve">OSU MPI </t>
   </si>
@@ -193,9 +198,6 @@
     <t>16.0.3 20160415</t>
   </si>
   <si>
-    <t>11.3.3</t>
-  </si>
-  <si>
     <t>3.10.0-327.el7.mpsp_1.3.1.45.x86_64</t>
   </si>
   <si>
@@ -216,6 +218,30 @@
   <si>
     <t>Total Time</t>
   </si>
+  <si>
+    <t>FWD Lib</t>
+  </si>
+  <si>
+    <t>BWD INPUTS Lib</t>
+  </si>
+  <si>
+    <t>BWD PARAMS Lib</t>
+  </si>
+  <si>
+    <t>MKL</t>
+  </si>
+  <si>
+    <t>LIBXSMM</t>
+  </si>
+  <si>
+    <t>LIBXSMM version</t>
+  </si>
+  <si>
+    <t>master-1.5.2-190</t>
+  </si>
+  <si>
+    <t>MKL 2017 Gold u1, MKLML (2017.0.1)</t>
+  </si>
 </sst>
 </file>
 
@@ -224,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,6 +300,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -338,7 +370,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -354,6 +386,9 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="38">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -730,33 +765,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X207"/>
+  <dimension ref="A1:AA207"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView showRuler="0" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="32.625" customWidth="1"/>
+    <col min="9" max="9" width="26.125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" customWidth="1"/>
+    <col min="11" max="11" width="24.125" customWidth="1"/>
+    <col min="12" max="12" width="18.625" customWidth="1"/>
+    <col min="13" max="13" width="15.875" customWidth="1"/>
+    <col min="14" max="14" width="20.125" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" customWidth="1"/>
+    <col min="20" max="20" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="14.375" customWidth="1"/>
+    <col min="25" max="27" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -782,7 +818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1760</v>
       </c>
@@ -799,18 +835,18 @@
         <v>8</v>
       </c>
       <c r="I2" s="2">
-        <v>7.7499999999999999E-2</v>
+        <v>7.8700000000000006E-2</v>
       </c>
       <c r="J2" s="2">
         <f>(2*C2*D2*E2)/(I2/1000)/10^12</f>
-        <v>1.2790090322580645</v>
+        <v>1.2595069885641677</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1760</v>
       </c>
@@ -827,18 +863,18 @@
         <v>8</v>
       </c>
       <c r="I3" s="2">
-        <v>0.11</v>
+        <v>0.10390000000000001</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J66" si="0">(2*C3*D3*E3)/(I3/1000)/10^12</f>
-        <v>1.8022400000000001</v>
+        <v>1.9080500481231952</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1760</v>
       </c>
@@ -855,18 +891,18 @@
         <v>8</v>
       </c>
       <c r="I4" s="2">
-        <v>0.19990000000000002</v>
+        <v>0.1862</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>1.9834557278639315</v>
+        <v>2.1293920515574651</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1760</v>
       </c>
@@ -883,18 +919,18 @@
         <v>8</v>
       </c>
       <c r="I5" s="2">
-        <v>0.39989999999999998</v>
+        <v>0.39189999999999997</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>1.9829597399349839</v>
+        <v>2.0234386323041593</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1760</v>
       </c>
@@ -911,18 +947,18 @@
         <v>8</v>
       </c>
       <c r="I6" s="2">
-        <v>9.9863</v>
+        <v>10.011700000000001</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>4.342589347405946</v>
+        <v>4.3315720606889929</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2048</v>
       </c>
@@ -939,18 +975,18 @@
         <v>8</v>
       </c>
       <c r="I7" s="2">
-        <v>8.0799999999999997E-2</v>
+        <v>8.0500000000000002E-2</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6611104950495048</v>
+        <v>1.6673009689440994</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>2048</v>
       </c>
@@ -967,18 +1003,18 @@
         <v>8</v>
       </c>
       <c r="I8" s="2">
-        <v>0.1236</v>
+        <v>0.13069999999999998</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>2.1718078964401295</v>
+        <v>2.0538290436113238</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>2048</v>
       </c>
@@ -995,18 +1031,18 @@
         <v>8</v>
       </c>
       <c r="I9" s="2">
-        <v>0.19440000000000002</v>
+        <v>0.19219999999999998</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>2.7616816460905347</v>
+        <v>2.7932929864724247</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>2048</v>
       </c>
@@ -1023,18 +1059,18 @@
         <v>8</v>
       </c>
       <c r="I10" s="2">
-        <v>0.36669999999999997</v>
+        <v>0.36940000000000001</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>2.9281205999454598</v>
+        <v>2.9067185273416354</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>2048</v>
       </c>
@@ -1051,18 +1087,18 @@
         <v>8</v>
       </c>
       <c r="I11" s="2">
-        <v>13.766200000000001</v>
+        <v>13.191700000000001</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>4.2655384928302649</v>
+        <v>4.4513031679010284</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>2560</v>
       </c>
@@ -1079,18 +1115,18 @@
         <v>8</v>
       </c>
       <c r="I12" s="2">
-        <v>0.14899999999999999</v>
+        <v>0.1482</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>1.4074845637583895</v>
+        <v>1.4150823211875845</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>2560</v>
       </c>
@@ -1107,18 +1143,18 @@
         <v>8</v>
       </c>
       <c r="I13" s="2">
-        <v>0.2082</v>
+        <v>0.2162</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>2.0145552353506244</v>
+        <v>1.9400111008325625</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>2560</v>
       </c>
@@ -1135,18 +1171,18 @@
         <v>8</v>
       </c>
       <c r="I14" s="2">
-        <v>0.34510000000000002</v>
+        <v>0.31869999999999998</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>2.4307760069545057</v>
+        <v>2.6321330404769374</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>2560</v>
       </c>
@@ -1163,18 +1199,18 @@
         <v>8</v>
       </c>
       <c r="I15" s="2">
-        <v>0.57410000000000005</v>
+        <v>0.57950000000000002</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>2.922350809963421</v>
+        <v>2.8951192407247626</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>2560</v>
       </c>
@@ -1191,18 +1227,18 @@
         <v>8</v>
       </c>
       <c r="I16" s="2">
-        <v>20.121599999999997</v>
+        <v>20.099799999999998</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>4.5597964376590339</v>
+        <v>4.5647419377307248</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="3:18">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>4096</v>
       </c>
@@ -1219,18 +1255,18 @@
         <v>8</v>
       </c>
       <c r="I17" s="2">
-        <v>0.39200000000000002</v>
+        <v>0.37640000000000001</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>1.3695686530612243</v>
+        <v>1.4263307970244421</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="3:18">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>4096</v>
       </c>
@@ -1247,18 +1283,18 @@
         <v>8</v>
       </c>
       <c r="I18" s="2">
-        <v>0.4652</v>
+        <v>0.47110000000000002</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>2.3081294582975063</v>
+        <v>2.279222721290596</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="3:18">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>4096</v>
       </c>
@@ -1275,18 +1311,18 @@
         <v>8</v>
       </c>
       <c r="I19" s="2">
-        <v>0.68510000000000004</v>
+        <v>0.68720000000000003</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
-        <v>3.1345550255437162</v>
+        <v>3.1249762048894061</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="3:18">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>4096</v>
       </c>
@@ -1303,18 +1339,18 @@
         <v>8</v>
       </c>
       <c r="I20" s="2">
-        <v>1.2495000000000001</v>
+        <v>1.2370999999999999</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="0"/>
-        <v>3.4373487763105244</v>
+        <v>3.4718028421307898</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="3:18">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>4096</v>
       </c>
@@ -1331,18 +1367,18 @@
         <v>8</v>
       </c>
       <c r="I21" s="2">
-        <v>52.081099999999999</v>
+        <v>51.761600000000001</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
-        <v>4.5099090456998798</v>
+        <v>4.5377465920682507</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" spans="3:18">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>1760</v>
       </c>
@@ -1359,18 +1395,18 @@
         <v>8</v>
       </c>
       <c r="I22" s="2">
-        <v>7.9500000000000001E-2</v>
+        <v>9.1499999999999998E-2</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="0"/>
-        <v>1.2468327044025156</v>
+        <v>1.0833136612021859</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="3:18">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1760</v>
       </c>
@@ -1387,18 +1423,18 @@
         <v>8</v>
       </c>
       <c r="I23" s="2">
-        <v>0.10350000000000001</v>
+        <v>0.10070000000000001</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="0"/>
-        <v>1.9154241545893718</v>
+        <v>1.9686832174776563</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="3:18">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>1760</v>
       </c>
@@ -1415,18 +1451,18 @@
         <v>8</v>
       </c>
       <c r="I24" s="2">
-        <v>0.15530000000000002</v>
+        <v>0.16280000000000003</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="0"/>
-        <v>2.5530766258853825</v>
+        <v>2.4354594594594592</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="3:18">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>1760</v>
       </c>
@@ -1443,18 +1479,18 @@
         <v>8</v>
       </c>
       <c r="I25" s="2">
-        <v>0.27789999999999998</v>
+        <v>0.26350000000000001</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>2.853492623245772</v>
+        <v>3.0094330170777988</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="3:18">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1760</v>
       </c>
@@ -1471,18 +1507,18 @@
         <v>8</v>
       </c>
       <c r="I26" s="2">
-        <v>10.0008</v>
+        <v>10.022200000000002</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" si="0"/>
-        <v>4.336293096552275</v>
+        <v>4.3270339845542889</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="3:18">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>2048</v>
       </c>
@@ -1499,18 +1535,18 @@
         <v>8</v>
       </c>
       <c r="I27" s="2">
-        <v>8.5500000000000007E-2</v>
+        <v>8.1599999999999992E-2</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" si="0"/>
-        <v>1.5697979883040936</v>
+        <v>1.6448250980392158</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="3:18">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>2048</v>
       </c>
@@ -1527,18 +1563,18 @@
         <v>8</v>
       </c>
       <c r="I28" s="2">
-        <v>0.1245</v>
+        <v>0.1212</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="0"/>
-        <v>2.1561080803212853</v>
+        <v>2.21481399339934</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="3:18">
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>2048</v>
       </c>
@@ -1555,18 +1591,18 @@
         <v>8</v>
       </c>
       <c r="I29" s="2">
-        <v>0.19350000000000001</v>
+        <v>0.1961</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" si="0"/>
-        <v>2.774526677002584</v>
+        <v>2.7377404997450285</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="3:18">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>2048</v>
       </c>
@@ -1583,18 +1619,18 @@
         <v>8</v>
       </c>
       <c r="I30" s="2">
-        <v>0.35960000000000003</v>
+        <v>0.36969999999999997</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" si="0"/>
-        <v>2.9859338820912122</v>
+        <v>2.9043598160670814</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="3:18">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>2048</v>
       </c>
@@ -1611,18 +1647,18 @@
         <v>8</v>
       </c>
       <c r="I31" s="2">
-        <v>13.7113</v>
+        <v>13.147</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" si="0"/>
-        <v>4.2826176948939922</v>
+        <v>4.466437666387769</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="3:18">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>2560</v>
       </c>
@@ -1639,18 +1675,18 @@
         <v>8</v>
       </c>
       <c r="I32" s="2">
-        <v>0.16390000000000002</v>
+        <v>0.15940000000000001</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" si="0"/>
-        <v>1.2795314215985354</v>
+        <v>1.3156537013801755</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="3:18">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>2560</v>
       </c>
@@ -1667,18 +1703,18 @@
         <v>8</v>
       </c>
       <c r="I33" s="2">
-        <v>0.24980000000000002</v>
+        <v>0.2036</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="0"/>
-        <v>1.6790648518815052</v>
+        <v>2.0600707269155203</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="3:18">
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>2560</v>
       </c>
@@ -1695,18 +1731,18 @@
         <v>8</v>
       </c>
       <c r="I34" s="2">
-        <v>0.41930000000000001</v>
+        <v>0.32110000000000005</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" si="0"/>
-        <v>2.0006219890293346</v>
+        <v>2.6124596698847706</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="3:18">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>2560</v>
       </c>
@@ -1723,18 +1759,18 @@
         <v>8</v>
       </c>
       <c r="I35" s="2">
-        <v>0.80820000000000003</v>
+        <v>0.56329999999999991</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>2.0758742885424399</v>
+        <v>2.9783802591869351</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="3:18">
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>2560</v>
       </c>
@@ -1751,18 +1787,18 @@
         <v>8</v>
       </c>
       <c r="I36" s="2">
-        <v>20.717099999999999</v>
+        <v>20.104500000000002</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="0"/>
-        <v>4.4287279590290147</v>
+        <v>4.5636747991743141</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
     </row>
-    <row r="37" spans="3:18">
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>4096</v>
       </c>
@@ -1779,18 +1815,18 @@
         <v>8</v>
       </c>
       <c r="I37" s="2">
-        <v>0.38239999999999996</v>
+        <v>0.36860000000000004</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="0"/>
-        <v>1.403951129707113</v>
+        <v>1.4565135973955508</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
     </row>
-    <row r="38" spans="3:18">
+    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>4096</v>
       </c>
@@ -1807,18 +1843,18 @@
         <v>8</v>
       </c>
       <c r="I38" s="2">
-        <v>0.46400000000000002</v>
+        <v>0.46450000000000002</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" si="0"/>
-        <v>2.3140987586206894</v>
+        <v>2.3116078019375674</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="3:18">
+    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>4096</v>
       </c>
@@ -1835,18 +1871,18 @@
         <v>8</v>
       </c>
       <c r="I39" s="2">
-        <v>0.68889999999999996</v>
+        <v>0.69189999999999996</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="0"/>
-        <v>3.1172646944404123</v>
+        <v>3.1037485879462352</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="3:18">
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>4096</v>
       </c>
@@ -1863,18 +1899,18 @@
         <v>8</v>
       </c>
       <c r="I40" s="2">
-        <v>1.2384999999999999</v>
+        <v>1.2324999999999999</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" si="0"/>
-        <v>3.4678783173193377</v>
+        <v>3.4847604835699801</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
     </row>
-    <row r="41" spans="3:18">
+    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>4096</v>
       </c>
@@ -1891,18 +1927,18 @@
         <v>8</v>
       </c>
       <c r="I41" s="2">
-        <v>51.83</v>
+        <v>52.286099999999998</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" si="0"/>
-        <v>4.5317581323557787</v>
+        <v>4.4922268824792821</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="3:18">
+    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>1760</v>
       </c>
@@ -1922,18 +1958,18 @@
         <v>25</v>
       </c>
       <c r="I42" s="2">
-        <v>11.221299999999999</v>
+        <v>11.495200000000001</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" si="0"/>
-        <v>3.9380786183419034</v>
+        <v>3.8442446934372607</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="3:18">
+    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>2048</v>
       </c>
@@ -1950,18 +1986,18 @@
         <v>24</v>
       </c>
       <c r="I43" s="2">
-        <v>15.1691</v>
+        <v>15.4033</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" si="0"/>
-        <v>3.9445940012261773</v>
+        <v>3.8846182872501349</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="3:18">
+    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>2560</v>
       </c>
@@ -1978,18 +2014,18 @@
         <v>24</v>
       </c>
       <c r="I44" s="2">
-        <v>23.776</v>
+        <v>23.782799999999998</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="0"/>
-        <v>3.9322702557200544</v>
+        <v>3.9311459374001383</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
     </row>
-    <row r="45" spans="3:18">
+    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C45" s="3">
         <v>4096</v>
       </c>
@@ -2006,18 +2042,18 @@
         <v>24</v>
       </c>
       <c r="I45" s="2">
-        <v>54.2879</v>
+        <v>55.115699999999997</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="0"/>
-        <v>4.4087865519940905</v>
+        <v>4.342569602781059</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="3:18">
+    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="M46" s="2"/>
@@ -2025,7 +2061,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="3:18">
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="M47" s="2"/>
@@ -2033,7 +2069,7 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
-    <row r="48" spans="3:18">
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>5124</v>
       </c>
@@ -2050,18 +2086,18 @@
         <v>8</v>
       </c>
       <c r="I48" s="2">
-        <v>37.983199999999997</v>
+        <v>38.194600000000001</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="0"/>
-        <v>4.332569228501022</v>
+        <v>4.3085892644509958</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
-    <row r="49" spans="3:18">
+    <row r="49" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>35</v>
       </c>
@@ -2078,18 +2114,18 @@
         <v>8</v>
       </c>
       <c r="I49" s="2">
-        <v>0.56720000000000004</v>
+        <v>0.54730000000000001</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="0"/>
-        <v>1.8369224259520451</v>
+        <v>1.9037135026493697</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
     </row>
-    <row r="50" spans="3:18">
+    <row r="50" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>5124</v>
       </c>
@@ -2106,18 +2142,18 @@
         <v>8</v>
       </c>
       <c r="I50" s="2">
-        <v>44.197000000000003</v>
+        <v>44.437100000000001</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="0"/>
-        <v>4.3327292824399848</v>
+        <v>4.3093189271127059</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
     </row>
-    <row r="51" spans="3:18">
+    <row r="51" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>35</v>
       </c>
@@ -2134,18 +2170,18 @@
         <v>8</v>
       </c>
       <c r="I51" s="2">
-        <v>0.65629999999999999</v>
+        <v>0.66190000000000004</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" si="0"/>
-        <v>1.8473190918787141</v>
+        <v>1.8316898625169964</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
     </row>
-    <row r="52" spans="3:18">
+    <row r="52" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>5124</v>
       </c>
@@ -2162,18 +2198,18 @@
         <v>8</v>
       </c>
       <c r="I52" s="2">
-        <v>55.025400000000005</v>
+        <v>55.539699999999996</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" si="0"/>
-        <v>4.3501191289840691</v>
+        <v>4.3098368395940208</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
-    <row r="53" spans="3:18">
+    <row r="53" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>35</v>
       </c>
@@ -2190,18 +2226,18 @@
         <v>8</v>
       </c>
       <c r="I53" s="2">
-        <v>0.79670000000000007</v>
+        <v>0.80349999999999999</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" si="0"/>
-        <v>1.9022146353709048</v>
+        <v>1.8861162414436841</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="3:18">
+    <row r="54" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>5124</v>
       </c>
@@ -2218,18 +2254,18 @@
         <v>8</v>
       </c>
       <c r="I54" s="2">
-        <v>88.071600000000004</v>
+        <v>87.715199999999996</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" si="0"/>
-        <v>4.3485899221996647</v>
+        <v>4.3662588946043561</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="3:18">
+    <row r="55" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>35</v>
       </c>
@@ -2246,18 +2282,18 @@
         <v>8</v>
       </c>
       <c r="I55" s="2">
-        <v>1.35</v>
+        <v>1.2481</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" si="0"/>
-        <v>1.796141511111111</v>
+        <v>1.9427858665171061</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="3:18">
+    <row r="56" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>5124</v>
       </c>
@@ -2274,18 +2310,18 @@
         <v>8</v>
       </c>
       <c r="I56" s="2">
-        <v>37.591900000000003</v>
+        <v>37.909599999999998</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" si="0"/>
-        <v>4.3776676230783753</v>
+        <v>4.340980741553591</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="3:18">
+    <row r="57" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>35</v>
       </c>
@@ -2302,18 +2338,18 @@
         <v>8</v>
       </c>
       <c r="I57" s="2">
-        <v>0.58250000000000002</v>
+        <v>0.53960000000000008</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" si="0"/>
-        <v>1.7886736480686694</v>
+        <v>1.930879169755374</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="3:18">
+    <row r="58" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>5124</v>
       </c>
@@ -2330,18 +2366,18 @@
         <v>8</v>
       </c>
       <c r="I58" s="2">
-        <v>44.316600000000001</v>
+        <v>44.522400000000005</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="0"/>
-        <v>4.3210362729992831</v>
+        <v>4.3010627480998327</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
     </row>
-    <row r="59" spans="3:18">
+    <row r="59" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>35</v>
       </c>
@@ -2358,18 +2394,18 @@
         <v>8</v>
       </c>
       <c r="I59" s="2">
-        <v>0.72150000000000003</v>
+        <v>0.64229999999999998</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" si="0"/>
-        <v>1.680381871101871</v>
+        <v>1.8875844932274639</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
     </row>
-    <row r="60" spans="3:18">
+    <row r="60" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>5124</v>
       </c>
@@ -2386,18 +2422,18 @@
         <v>8</v>
       </c>
       <c r="I60" s="2">
-        <v>55.169600000000003</v>
+        <v>55.704500000000003</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" si="0"/>
-        <v>4.338748968997419</v>
+        <v>4.2970863237260897</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
-    <row r="61" spans="3:18">
+    <row r="61" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>35</v>
       </c>
@@ -2414,18 +2450,18 @@
         <v>8</v>
       </c>
       <c r="I61" s="2">
-        <v>0.87620000000000009</v>
+        <v>0.83720000000000006</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" si="0"/>
-        <v>1.7296215475918739</v>
+        <v>1.8101939799331102</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="3:18">
+    <row r="62" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>5124</v>
       </c>
@@ -2442,18 +2478,18 @@
         <v>8</v>
       </c>
       <c r="I62" s="2">
-        <v>88.371399999999994</v>
+        <v>87.778100000000009</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" si="0"/>
-        <v>4.3338373296337958</v>
+        <v>4.3631301223425885</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
     </row>
-    <row r="63" spans="3:18">
+    <row r="63" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>35</v>
       </c>
@@ -2470,18 +2506,18 @@
         <v>8</v>
       </c>
       <c r="I63" s="2">
-        <v>1.2795000000000001</v>
+        <v>1.2887999999999999</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" si="0"/>
-        <v>1.8951082766705745</v>
+        <v>1.8814331471135943</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
     </row>
-    <row r="64" spans="3:18">
+    <row r="64" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="M64" s="2"/>
@@ -2489,7 +2525,7 @@
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
     </row>
-    <row r="65" spans="3:18">
+    <row r="65" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>7680</v>
       </c>
@@ -2517,7 +2553,7 @@
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
     </row>
-    <row r="66" spans="3:18">
+    <row r="66" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>7680</v>
       </c>
@@ -2534,18 +2570,18 @@
         <v>8</v>
       </c>
       <c r="I66" s="2">
-        <v>0.58629999999999993</v>
+        <v>0.59089999999999998</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" si="0"/>
-        <v>2.1461558928876006</v>
+        <v>2.1294486376713491</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
     </row>
-    <row r="67" spans="3:18">
+    <row r="67" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>7680</v>
       </c>
@@ -2562,18 +2598,18 @@
         <v>8</v>
       </c>
       <c r="I67" s="2">
-        <v>0.82529999999999992</v>
+        <v>0.82400000000000007</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" ref="J67:J83" si="1">(2*C67*D67*E67)/(I67/1000)/10^12</f>
-        <v>3.0492940748818613</v>
+        <v>3.0541048543689318</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
-    <row r="68" spans="3:18">
+    <row r="68" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>7680</v>
       </c>
@@ -2590,18 +2626,18 @@
         <v>8</v>
       </c>
       <c r="I68" s="2">
-        <v>1.3689000000000002</v>
+        <v>1.3814000000000002</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" si="1"/>
-        <v>3.6767950909489366</v>
+        <v>3.6435245403214132</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
     </row>
-    <row r="69" spans="3:18">
+    <row r="69" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>7680</v>
       </c>
@@ -2618,18 +2654,18 @@
         <v>8</v>
       </c>
       <c r="I69" s="2">
-        <v>0.43810000000000004</v>
+        <v>0.43280000000000002</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" si="1"/>
-        <v>1.4360776078520885</v>
+        <v>1.4536635859519409</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="3:18">
+    <row r="70" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>7680</v>
       </c>
@@ -2646,18 +2682,18 @@
         <v>8</v>
       </c>
       <c r="I70" s="2">
-        <v>0.52949999999999997</v>
+        <v>0.52860000000000007</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" si="1"/>
-        <v>2.3763762039660055</v>
+        <v>2.3804222474460839</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
     </row>
-    <row r="71" spans="3:18">
+    <row r="71" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>7680</v>
       </c>
@@ -2674,18 +2710,18 @@
         <v>8</v>
       </c>
       <c r="I71" s="2">
-        <v>0.77179999999999993</v>
+        <v>0.76290000000000002</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" si="1"/>
-        <v>3.2606664939103398</v>
+        <v>3.2987054659850568</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
     </row>
-    <row r="72" spans="3:18">
+    <row r="72" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>7680</v>
       </c>
@@ -2702,18 +2738,18 @@
         <v>8</v>
       </c>
       <c r="I72" s="2">
-        <v>1.3352999999999999</v>
+        <v>1.3599000000000001</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" si="1"/>
-        <v>3.7693138620534712</v>
+        <v>3.7011286123979703</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
     </row>
-    <row r="73" spans="3:18">
+    <row r="73" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C73">
         <f t="shared" ref="C73:C80" si="2">3*1024</f>
         <v>3072</v>
@@ -2731,18 +2767,18 @@
         <v>8</v>
       </c>
       <c r="I73" s="2">
-        <v>5.9500000000000004E-2</v>
+        <v>5.6399999999999999E-2</v>
       </c>
       <c r="J73" s="2">
         <f t="shared" si="1"/>
-        <v>1.691820100840336</v>
+        <v>1.7848102127659573</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
     </row>
-    <row r="74" spans="3:18">
+    <row r="74" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C74">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2760,18 +2796,18 @@
         <v>8</v>
       </c>
       <c r="I74" s="2">
-        <v>9.5200000000000007E-2</v>
+        <v>9.06E-2</v>
       </c>
       <c r="J74" s="2">
         <f t="shared" si="1"/>
-        <v>2.1147751260504197</v>
+        <v>2.2221478145695359</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="Q74" s="2"/>
       <c r="R74" s="2"/>
     </row>
-    <row r="75" spans="3:18">
+    <row r="75" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C75">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2789,18 +2825,18 @@
         <v>8</v>
       </c>
       <c r="I75" s="2">
-        <v>0.14319999999999999</v>
+        <v>0.16419999999999998</v>
       </c>
       <c r="J75" s="2">
         <f t="shared" si="1"/>
-        <v>2.8118239106145255</v>
+        <v>2.4522118392204635</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
     </row>
-    <row r="76" spans="3:18">
+    <row r="76" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C76">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2818,18 +2854,18 @@
         <v>8</v>
       </c>
       <c r="I76" s="2">
-        <v>0.25800000000000001</v>
+        <v>0.25630000000000003</v>
       </c>
       <c r="J76" s="2">
         <f t="shared" si="1"/>
-        <v>3.1213425116279074</v>
+        <v>3.1420459149434254</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
     </row>
-    <row r="77" spans="3:18">
+    <row r="77" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C77">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2847,18 +2883,18 @@
         <v>8</v>
       </c>
       <c r="I77" s="2">
-        <v>8.1299999999999997E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="J77" s="2">
         <f t="shared" si="1"/>
-        <v>1.238170922509225</v>
+        <v>1.2742189367088608</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="3:18">
+    <row r="78" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C78">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2876,18 +2912,18 @@
         <v>8</v>
       </c>
       <c r="I78" s="2">
-        <v>0.1095</v>
+        <v>0.1077</v>
       </c>
       <c r="J78" s="2">
         <f t="shared" si="1"/>
-        <v>1.8385990136986301</v>
+        <v>1.8693276880222842</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
     </row>
-    <row r="79" spans="3:18">
+    <row r="79" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C79">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2905,18 +2941,18 @@
         <v>8</v>
       </c>
       <c r="I79" s="2">
-        <v>0.159</v>
+        <v>0.15959999999999999</v>
       </c>
       <c r="J79" s="2">
         <f t="shared" si="1"/>
-        <v>2.5324099622641509</v>
+        <v>2.5228896240601504</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="Q79" s="2"/>
       <c r="R79" s="2"/>
     </row>
-    <row r="80" spans="3:18">
+    <row r="80" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C80">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2934,18 +2970,18 @@
         <v>8</v>
       </c>
       <c r="I80" s="2">
-        <v>0.27430000000000004</v>
+        <v>0.27239999999999998</v>
       </c>
       <c r="J80" s="2">
         <f t="shared" si="1"/>
-        <v>2.9358598906306956</v>
+        <v>2.9563376211453751</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="Q80" s="2"/>
       <c r="R80" s="2"/>
     </row>
-    <row r="81" spans="1:24">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="M81" s="2"/>
@@ -2953,7 +2989,7 @@
       <c r="Q81" s="2"/>
       <c r="R81" s="2"/>
     </row>
-    <row r="82" spans="1:24">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C82">
         <v>3072</v>
       </c>
@@ -2970,18 +3006,18 @@
         <v>24</v>
       </c>
       <c r="I82" s="2">
-        <v>10.896600000000001</v>
+        <v>10.945200000000002</v>
       </c>
       <c r="J82" s="2">
         <f t="shared" si="1"/>
-        <v>4.2928046693464017</v>
+        <v>4.2737433176186812</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
     </row>
-    <row r="83" spans="1:24">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C83">
         <v>7680</v>
       </c>
@@ -2998,31 +3034,31 @@
         <v>24</v>
       </c>
       <c r="I83" s="2">
-        <v>51.992699999999999</v>
+        <v>52.102900000000005</v>
       </c>
       <c r="J83" s="2">
         <f t="shared" si="1"/>
-        <v>4.1452298034147104</v>
+        <v>4.1364624541052413</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="Q83" s="2"/>
       <c r="R83" s="2"/>
     </row>
-    <row r="85" spans="1:24">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J85" s="2"/>
       <c r="N85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="87" spans="1:24">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J87" s="1"/>
     </row>
-    <row r="89" spans="1:24">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:24">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>22</v>
       </c>
@@ -3072,7 +3108,7 @@
         <v>38</v>
       </c>
       <c r="T90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U90" t="s">
         <v>39</v>
@@ -3083,8 +3119,17 @@
       <c r="W90" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="91" spans="1:24">
+      <c r="Y90" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z90" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA90" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>700</v>
       </c>
@@ -3119,13 +3164,13 @@
         <v>2</v>
       </c>
       <c r="N91" s="2">
-        <v>0.19317863360107504</v>
+        <v>0.17917</v>
       </c>
       <c r="O91" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P91" s="2">
-        <v>3.1055000000000001</v>
+        <v>2.6216999999999997</v>
       </c>
       <c r="R91" s="4">
         <f>(D91-H91+1+2*J91)/L91</f>
@@ -3137,21 +3182,31 @@
       </c>
       <c r="T91" s="10">
         <f>N91+P91</f>
-        <v>3.2986786336010754</v>
+        <v>2.8008699999999997</v>
       </c>
       <c r="U91" s="2">
         <f>(2*$R91*$S91*$F91*$G91*$E91*$H91*$I91)/(N91/1000)/10^12</f>
-        <v>3.5421557096891694</v>
+        <v>3.8191036445833566</v>
       </c>
       <c r="V91" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W91" s="2">
         <f>(2*$R91*$S91*$F91*$G91*$E91*$H91*$I91)/(P91/1000)/10^12</f>
-        <v>0.22034094348736111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:24">
+        <v>0.26100194530266624</v>
+      </c>
+      <c r="X91" s="2"/>
+      <c r="Y91" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA91" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C92">
         <v>700</v>
       </c>
@@ -3186,13 +3241,13 @@
         <v>2</v>
       </c>
       <c r="N92" s="2">
-        <v>0.41029079233289006</v>
+        <v>0.35833000000000004</v>
       </c>
       <c r="O92" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P92" s="2">
-        <v>5.9086000000000007</v>
+        <v>2.6246</v>
       </c>
       <c r="R92" s="4">
         <f t="shared" ref="R92:R126" si="3">(D92-H92+1+2*J92)/L92</f>
@@ -3204,21 +3259,31 @@
       </c>
       <c r="T92" s="10">
         <f>N92+P92</f>
-        <v>6.3188907923328905</v>
+        <v>2.9829300000000001</v>
       </c>
       <c r="U92" s="2">
         <f>(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(N92/1000)/10^12</f>
-        <v>3.3355308614618751</v>
+        <v>3.8192102252113971</v>
       </c>
       <c r="V92" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W92" s="2">
         <f>(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(P92/1000)/10^12</f>
-        <v>0.23161791287276171</v>
-      </c>
-    </row>
-    <row r="93" spans="1:24">
+        <v>0.52142711270288811</v>
+      </c>
+      <c r="X92" s="2"/>
+      <c r="Y92" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>700</v>
       </c>
@@ -3253,13 +3318,13 @@
         <v>2</v>
       </c>
       <c r="N93" s="2">
-        <v>0.88766066729817916</v>
+        <v>0.76228000000000007</v>
       </c>
       <c r="O93" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P93" s="2">
-        <v>11.585000000000001</v>
+        <v>2.6320999999999999</v>
       </c>
       <c r="R93" s="4">
         <f t="shared" si="3"/>
@@ -3271,21 +3336,31 @@
       </c>
       <c r="T93" s="10">
         <f>N93+P93</f>
-        <v>12.472660667298181</v>
+        <v>3.39438</v>
       </c>
       <c r="U93" s="2">
         <f>(2*$R93*$S93*$F93*$G93*$E93*$H93*$I93)/(N93/1000)/10^12</f>
-        <v>3.0834701827343367</v>
+        <v>3.5906428084168547</v>
       </c>
       <c r="V93" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W93" s="2">
         <f>(2*$R93*$S93*$F93*$G93*$E93*$H93*$I93)/(P93/1000)/10^12</f>
-        <v>0.23626026758739746</v>
-      </c>
-    </row>
-    <row r="94" spans="1:24">
+        <v>1.0398826792295126</v>
+      </c>
+      <c r="X93" s="2"/>
+      <c r="Y93" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z93" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA93" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C94">
         <v>700</v>
       </c>
@@ -3320,13 +3395,13 @@
         <v>2</v>
       </c>
       <c r="N94" s="2">
-        <v>1.7338353263662845</v>
+        <v>1.5425</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P94" s="2">
-        <v>22.779</v>
+        <v>2.6388000000000003</v>
       </c>
       <c r="R94" s="4">
         <f t="shared" si="3"/>
@@ -3338,21 +3413,31 @@
       </c>
       <c r="T94" s="10">
         <f>N94+P94</f>
-        <v>24.512835326366286</v>
+        <v>4.1813000000000002</v>
       </c>
       <c r="U94" s="2">
         <f>(2*$R94*$S94*$F94*$G94*$E94*$H94*$I94)/(N94/1000)/10^12</f>
-        <v>3.1572493170228255</v>
+        <v>3.5488819448946516</v>
       </c>
       <c r="V94" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W94" s="2">
         <f>(2*$R94*$S94*$F94*$G94*$E94*$H94*$I94)/(P94/1000)/10^12</f>
-        <v>0.24031565915975242</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24">
+        <v>2.0744847658026373</v>
+      </c>
+      <c r="X94" s="2"/>
+      <c r="Y94" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z94" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>341</v>
       </c>
@@ -3387,13 +3472,13 @@
         <v>2</v>
       </c>
       <c r="N95" s="2">
-        <v>0.91041034119945885</v>
+        <v>1.0842000000000001</v>
       </c>
       <c r="O95" s="2">
-        <v>68.790000000000006</v>
+        <v>86.45</v>
       </c>
       <c r="P95" s="2">
-        <v>74.98</v>
+        <v>3.63</v>
       </c>
       <c r="R95" s="4">
         <f t="shared" si="3"/>
@@ -3405,23 +3490,32 @@
       </c>
       <c r="T95" s="2">
         <f>N95+O95+P95</f>
-        <v>144.68041034119949</v>
+        <v>91.164199999999994</v>
       </c>
       <c r="U95" s="2">
         <f t="shared" ref="U95:U126" si="5">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(N95/1000)/10^12</f>
-        <v>2.8006711749788678</v>
+        <v>2.3517432208079687</v>
       </c>
       <c r="V95" s="2">
         <f t="shared" ref="V95:V126" si="6">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(O95/1000)/10^12</f>
-        <v>3.7065852594853906E-2</v>
+        <v>2.9494042799305956E-2</v>
       </c>
       <c r="W95" s="2">
         <f t="shared" ref="W95:W126" si="7">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(P95/1000)/10^12</f>
-        <v>3.4005868231528402E-2</v>
-      </c>
-      <c r="X95" s="3"/>
-    </row>
-    <row r="96" spans="1:24">
+        <v>0.70241322314049581</v>
+      </c>
+      <c r="X95" s="2"/>
+      <c r="Y95" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z95" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C96">
         <v>341</v>
       </c>
@@ -3456,13 +3550,13 @@
         <v>2</v>
       </c>
       <c r="N96" s="2">
-        <v>1.6416750237159505</v>
+        <v>1.8062</v>
       </c>
       <c r="O96" s="2">
-        <v>69.460000000000008</v>
+        <v>86.61</v>
       </c>
       <c r="P96" s="2">
-        <v>74.36</v>
+        <v>3.67</v>
       </c>
       <c r="R96" s="4">
         <f t="shared" si="3"/>
@@ -3474,23 +3568,32 @@
       </c>
       <c r="T96" s="2">
         <f t="shared" ref="T96:T98" si="8">N96+O96+P96</f>
-        <v>145.46167502371594</v>
+        <v>92.086200000000005</v>
       </c>
       <c r="U96" s="2">
         <f t="shared" si="5"/>
-        <v>3.10629078613694</v>
+        <v>2.8233418226110065</v>
       </c>
       <c r="V96" s="2">
         <f t="shared" si="6"/>
-        <v>7.3416642672041454E-2</v>
+        <v>5.8879113266366481E-2</v>
       </c>
       <c r="W96" s="2">
         <f t="shared" si="7"/>
-        <v>6.8578805809575039E-2</v>
-      </c>
-      <c r="X96" s="3"/>
-    </row>
-    <row r="97" spans="3:24">
+        <v>1.3895149863760217</v>
+      </c>
+      <c r="X96" s="2"/>
+      <c r="Y96" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z96" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA96" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="97" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>341</v>
       </c>
@@ -3525,13 +3628,13 @@
         <v>2</v>
       </c>
       <c r="N97" s="2">
-        <v>3.2716008372155834</v>
+        <v>3.6389999999999998</v>
       </c>
       <c r="O97" s="2">
-        <v>70.600000000000009</v>
+        <v>86.84</v>
       </c>
       <c r="P97" s="2">
-        <v>77.61</v>
+        <v>3.73</v>
       </c>
       <c r="R97" s="4">
         <f t="shared" si="3"/>
@@ -3543,23 +3646,32 @@
       </c>
       <c r="T97" s="2">
         <f t="shared" si="8"/>
-        <v>151.48160083721558</v>
+        <v>94.209000000000003</v>
       </c>
       <c r="U97" s="2">
         <f t="shared" si="5"/>
-        <v>3.1174463229078615</v>
+        <v>2.802704039571311</v>
       </c>
       <c r="V97" s="2">
         <f t="shared" si="6"/>
-        <v>0.14446232294617564</v>
+        <v>0.11744633809304468</v>
       </c>
       <c r="W97" s="2">
         <f t="shared" si="7"/>
-        <v>0.13141399304213375</v>
-      </c>
-      <c r="X97" s="3"/>
-    </row>
-    <row r="98" spans="3:24">
+        <v>2.7343270777479893</v>
+      </c>
+      <c r="X97" s="2"/>
+      <c r="Y97" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z97" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA97" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>341</v>
       </c>
@@ -3594,13 +3706,13 @@
         <v>2</v>
       </c>
       <c r="N98" s="2">
-        <v>6.2727829379591569</v>
+        <v>6.2116000000000007</v>
       </c>
       <c r="O98" s="2">
-        <v>73.27</v>
+        <v>87.55</v>
       </c>
       <c r="P98" s="2">
-        <v>95.18</v>
+        <v>7.24</v>
       </c>
       <c r="R98" s="4">
         <f t="shared" si="3"/>
@@ -3612,23 +3724,32 @@
       </c>
       <c r="T98" s="2">
         <f t="shared" si="8"/>
-        <v>174.72278293795915</v>
+        <v>101.0016</v>
       </c>
       <c r="U98" s="2">
         <f t="shared" si="5"/>
-        <v>3.2518389687235847</v>
+        <v>3.2838688904630042</v>
       </c>
       <c r="V98" s="2">
         <f t="shared" si="6"/>
-        <v>0.27839606933260541</v>
+        <v>0.23298777841233581</v>
       </c>
       <c r="W98" s="2">
         <f t="shared" si="7"/>
-        <v>0.21431056944736288</v>
-      </c>
-      <c r="X98" s="3"/>
-    </row>
-    <row r="99" spans="3:24">
+        <v>2.8174143646408836</v>
+      </c>
+      <c r="X98" s="2"/>
+      <c r="Y98" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z98" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA98" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>480</v>
       </c>
@@ -3663,13 +3784,13 @@
         <v>1</v>
       </c>
       <c r="N99" s="2">
-        <v>0.24355559633869375</v>
-      </c>
-      <c r="O99" s="2" t="s">
-        <v>63</v>
+        <v>8.4348000000000006E-2</v>
+      </c>
+      <c r="O99" s="2">
+        <v>2.94</v>
       </c>
       <c r="P99" s="2">
-        <v>25.55</v>
+        <v>0.66164999999999996</v>
       </c>
       <c r="R99" s="4">
         <f t="shared" si="3"/>
@@ -3681,22 +3802,31 @@
       </c>
       <c r="T99" s="2">
         <f>N99+P99</f>
-        <v>25.793555596338695</v>
+        <v>0.74599799999999994</v>
       </c>
       <c r="U99" s="2">
         <f t="shared" si="5"/>
-        <v>0.43591000000000002</v>
+        <v>1.2586939820742638</v>
       </c>
       <c r="V99" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W99" s="2">
         <f t="shared" si="7"/>
-        <v>4.1553158512720153E-3</v>
-      </c>
-      <c r="X99" s="3"/>
-    </row>
-    <row r="100" spans="3:24">
+        <v>0.16045994105644981</v>
+      </c>
+      <c r="X99" s="2"/>
+      <c r="Y99" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z99" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA99" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>240</v>
       </c>
@@ -3731,13 +3861,13 @@
         <v>1</v>
       </c>
       <c r="N100" s="2">
-        <v>0.19266549314944201</v>
+        <v>0.21876000000000001</v>
       </c>
       <c r="O100" s="2">
-        <v>582.05999999999995</v>
+        <v>11.76</v>
       </c>
       <c r="P100" s="2">
-        <v>0.74</v>
+        <v>0.67</v>
       </c>
       <c r="R100" s="4">
         <f t="shared" si="3"/>
@@ -3749,23 +3879,32 @@
       </c>
       <c r="T100" s="2">
         <f>N100+O100+P100</f>
-        <v>582.99266549314939</v>
+        <v>12.648759999999999</v>
       </c>
       <c r="U100" s="2">
         <f t="shared" si="5"/>
-        <v>4.4083999999999994</v>
+        <v>3.8825496434448712</v>
       </c>
       <c r="V100" s="2">
         <f t="shared" si="6"/>
-        <v>1.4592079167096178E-3</v>
+        <v>7.2223346938775509E-2</v>
       </c>
       <c r="W100" s="2">
         <f t="shared" si="7"/>
-        <v>1.1477656216216217</v>
-      </c>
-      <c r="X100" s="3"/>
-    </row>
-    <row r="101" spans="3:24">
+        <v>1.2676814328358208</v>
+      </c>
+      <c r="X100" s="2"/>
+      <c r="Y100" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z100" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>120</v>
       </c>
@@ -3800,13 +3939,13 @@
         <v>1</v>
       </c>
       <c r="N101" s="2">
-        <v>0.22</v>
+        <v>0.19597000000000001</v>
       </c>
       <c r="O101" s="2">
-        <v>571.42999999999995</v>
+        <v>6.02</v>
       </c>
       <c r="P101" s="2">
-        <v>0.31</v>
+        <v>0.23</v>
       </c>
       <c r="R101" s="4">
         <f t="shared" si="3"/>
@@ -3818,23 +3957,32 @@
       </c>
       <c r="T101" s="2">
         <f t="shared" ref="T101:T102" si="9">N101+O101+P101</f>
-        <v>571.95999999999992</v>
+        <v>6.44597</v>
       </c>
       <c r="U101" s="2">
         <f t="shared" si="5"/>
-        <v>3.8606661818181816</v>
+        <v>4.334064193499005</v>
       </c>
       <c r="V101" s="2">
         <f t="shared" si="6"/>
-        <v>1.4863527641180896E-3</v>
+        <v>0.1410874684385382</v>
       </c>
       <c r="W101" s="2">
         <f t="shared" si="7"/>
-        <v>2.7398276129032255</v>
-      </c>
-      <c r="X101" s="3"/>
-    </row>
-    <row r="102" spans="3:24">
+        <v>3.6928111304347828</v>
+      </c>
+      <c r="X101" s="2"/>
+      <c r="Y101" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z101" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA101" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C102">
         <v>60</v>
       </c>
@@ -3869,13 +4017,13 @@
         <v>1</v>
       </c>
       <c r="N102" s="2">
-        <v>0.23</v>
+        <v>0.19139999999999999</v>
       </c>
       <c r="O102" s="2">
-        <v>0.22</v>
+        <v>0.24948000000000001</v>
       </c>
       <c r="P102" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="R102" s="4">
         <f t="shared" si="3"/>
@@ -3887,23 +4035,32 @@
       </c>
       <c r="T102" s="2">
         <f t="shared" si="9"/>
-        <v>0.74</v>
+        <v>0.64088000000000001</v>
       </c>
       <c r="U102" s="2">
         <f t="shared" si="5"/>
-        <v>3.6928111304347828</v>
+        <v>4.4375473354231971</v>
       </c>
       <c r="V102" s="2">
         <f t="shared" si="6"/>
-        <v>3.8606661818181816</v>
+        <v>3.4044675324675322</v>
       </c>
       <c r="W102" s="2">
         <f t="shared" si="7"/>
-        <v>2.9287812413793106</v>
-      </c>
-      <c r="X102" s="3"/>
-    </row>
-    <row r="103" spans="3:24">
+        <v>4.2467328000000002</v>
+      </c>
+      <c r="X102" s="2"/>
+      <c r="Y102" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z102" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA102" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>108</v>
       </c>
@@ -3940,11 +4097,11 @@
       <c r="N103" s="2">
         <v>0.04</v>
       </c>
-      <c r="O103" s="2" t="s">
-        <v>63</v>
+      <c r="O103" s="2">
+        <v>2.89</v>
       </c>
       <c r="P103" s="2">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="R103" s="4">
         <f t="shared" si="3"/>
@@ -3956,22 +4113,31 @@
       </c>
       <c r="T103" s="2">
         <f>N103+P103</f>
-        <v>0.13</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="U103" s="2">
         <f t="shared" si="5"/>
         <v>2.0155391999999996</v>
       </c>
       <c r="V103" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W103" s="2">
         <f t="shared" si="7"/>
-        <v>0.89579520000000012</v>
-      </c>
-      <c r="X103" s="3"/>
-    </row>
-    <row r="104" spans="3:24">
+        <v>1.1517366857142857</v>
+      </c>
+      <c r="X103" s="2"/>
+      <c r="Y103" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z103" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA103" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="104" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C104">
         <v>54</v>
       </c>
@@ -4006,13 +4172,13 @@
         <v>1</v>
       </c>
       <c r="N104" s="2">
-        <v>0.39754224852071013</v>
+        <v>0.66998999999999997</v>
       </c>
       <c r="O104" s="2">
-        <v>1</v>
+        <v>0.90490999999999999</v>
       </c>
       <c r="P104" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.53</v>
       </c>
       <c r="R104" s="4">
         <f t="shared" si="3"/>
@@ -4024,23 +4190,32 @@
       </c>
       <c r="T104" s="2">
         <f>N104+O104+P104</f>
-        <v>1.9775422485207099</v>
+        <v>2.1048999999999998</v>
       </c>
       <c r="U104" s="2">
         <f t="shared" si="5"/>
-        <v>4.3263999999999996</v>
+        <v>2.5670932163166618</v>
       </c>
       <c r="V104" s="2">
         <f t="shared" si="6"/>
-        <v>1.7199267840000001</v>
+        <v>1.9006606005017073</v>
       </c>
       <c r="W104" s="2">
         <f t="shared" si="7"/>
-        <v>2.9653910068965517</v>
-      </c>
-      <c r="X104" s="3"/>
-    </row>
-    <row r="105" spans="3:24">
+        <v>3.2451448754716981</v>
+      </c>
+      <c r="X104" s="2"/>
+      <c r="Y104" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z104" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>27</v>
       </c>
@@ -4075,13 +4250,13 @@
         <v>1</v>
       </c>
       <c r="N105" s="2">
-        <v>0.370266901466061</v>
+        <v>0.36105999999999999</v>
       </c>
       <c r="O105" s="2">
+        <v>0.44546999999999998</v>
+      </c>
+      <c r="P105" s="2">
         <v>0.44</v>
-      </c>
-      <c r="P105" s="2">
-        <v>0.6</v>
       </c>
       <c r="R105" s="4">
         <f t="shared" si="3"/>
@@ -4093,23 +4268,32 @@
       </c>
       <c r="T105" s="2">
         <f t="shared" ref="T105:T107" si="10">N105+O105+P105</f>
-        <v>1.4102669014660609</v>
+        <v>1.2465299999999999</v>
       </c>
       <c r="U105" s="2">
         <f t="shared" si="5"/>
-        <v>4.6451000000000002</v>
+        <v>4.763548396388412</v>
       </c>
       <c r="V105" s="2">
         <f t="shared" si="6"/>
-        <v>3.9089245090909093</v>
+        <v>3.8609261768469256</v>
       </c>
       <c r="W105" s="2">
         <f t="shared" si="7"/>
-        <v>2.8665446400000003</v>
-      </c>
-      <c r="X105" s="3"/>
-    </row>
-    <row r="106" spans="3:24">
+        <v>3.9089245090909093</v>
+      </c>
+      <c r="X105" s="2"/>
+      <c r="Y105" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z105" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>14</v>
       </c>
@@ -4144,13 +4328,13 @@
         <v>1</v>
       </c>
       <c r="N106" s="2">
-        <v>0.19962960455879811</v>
+        <v>0.19823000000000002</v>
       </c>
       <c r="O106" s="2">
-        <v>0.23</v>
+        <v>0.26186999999999999</v>
       </c>
       <c r="P106" s="2">
-        <v>0.35</v>
+        <v>0.21</v>
       </c>
       <c r="R106" s="4">
         <f t="shared" si="3"/>
@@ -4162,23 +4346,32 @@
       </c>
       <c r="T106" s="2">
         <f t="shared" si="10"/>
-        <v>0.77962960455879804</v>
+        <v>0.67010000000000003</v>
       </c>
       <c r="U106" s="2">
         <f t="shared" si="5"/>
-        <v>4.6327999999999996</v>
+        <v>4.6655099228169297</v>
       </c>
       <c r="V106" s="2">
         <f t="shared" si="6"/>
-        <v>4.0210610086956518</v>
+        <v>3.531691419406576</v>
       </c>
       <c r="W106" s="2">
         <f t="shared" si="7"/>
-        <v>2.64241152</v>
-      </c>
-      <c r="X106" s="3"/>
-    </row>
-    <row r="107" spans="3:24">
+        <v>4.4040191999999996</v>
+      </c>
+      <c r="X106" s="2"/>
+      <c r="Y106" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>7</v>
       </c>
@@ -4213,13 +4406,13 @@
         <v>1</v>
       </c>
       <c r="N107" s="2">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="O107" s="2">
-        <v>0.44</v>
+        <v>0.64302999999999999</v>
       </c>
       <c r="P107" s="2">
-        <v>0.32</v>
+        <v>0.23666000000000001</v>
       </c>
       <c r="R107" s="4">
         <f t="shared" si="3"/>
@@ -4231,23 +4424,32 @@
       </c>
       <c r="T107" s="2">
         <f t="shared" si="10"/>
-        <v>1.1200000000000001</v>
+        <v>1.1896900000000001</v>
       </c>
       <c r="U107" s="2">
         <f t="shared" si="5"/>
-        <v>2.5690111999999998</v>
+        <v>2.9833678451612906</v>
       </c>
       <c r="V107" s="2">
         <f t="shared" si="6"/>
-        <v>2.1019182545454544</v>
+        <v>1.4382595399903582</v>
       </c>
       <c r="W107" s="2">
         <f t="shared" si="7"/>
-        <v>2.8901376000000001</v>
-      </c>
-      <c r="X107" s="3"/>
-    </row>
-    <row r="108" spans="3:24">
+        <v>3.9079017662469364</v>
+      </c>
+      <c r="X107" s="2"/>
+      <c r="Y107" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z107" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>224</v>
       </c>
@@ -4282,13 +4484,13 @@
         <v>1</v>
       </c>
       <c r="N108" s="2">
-        <v>1.18</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P108" s="2">
-        <v>1.94</v>
+        <v>1.87</v>
       </c>
       <c r="R108" s="4">
         <f t="shared" si="3"/>
@@ -4300,22 +4502,31 @@
       </c>
       <c r="T108" s="2">
         <f>N108+P108</f>
-        <v>3.12</v>
+        <v>3</v>
       </c>
       <c r="U108" s="2">
         <f t="shared" si="5"/>
-        <v>1.175649193220339</v>
+        <v>1.2276690690265488</v>
       </c>
       <c r="V108" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W108" s="2">
         <f t="shared" si="7"/>
-        <v>0.71508559175257735</v>
-      </c>
-      <c r="X108" s="3"/>
-    </row>
-    <row r="109" spans="3:24">
+        <v>0.7418535016042781</v>
+      </c>
+      <c r="X108" s="2"/>
+      <c r="Y108" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z108" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>112</v>
       </c>
@@ -4350,13 +4561,13 @@
         <v>1</v>
       </c>
       <c r="N109" s="2">
-        <v>3.54</v>
+        <v>3.38</v>
       </c>
       <c r="O109" s="2">
-        <v>5.48</v>
+        <v>7.2712000000000003</v>
       </c>
       <c r="P109" s="2">
-        <v>4.75</v>
+        <v>4.66</v>
       </c>
       <c r="R109" s="4">
         <f t="shared" si="3"/>
@@ -4368,23 +4579,32 @@
       </c>
       <c r="T109" s="2">
         <f>N109+O109+P109</f>
-        <v>13.77</v>
+        <v>15.311199999999999</v>
       </c>
       <c r="U109" s="2">
         <f t="shared" si="5"/>
-        <v>4.1800860203389831</v>
+        <v>4.3779599147928998</v>
       </c>
       <c r="V109" s="2">
         <f t="shared" si="6"/>
-        <v>2.7002745459854012</v>
+        <v>2.0350842380899987</v>
       </c>
       <c r="W109" s="2">
         <f t="shared" si="7"/>
-        <v>3.1152641077894736</v>
-      </c>
-      <c r="X109" s="3"/>
-    </row>
-    <row r="110" spans="3:24">
+        <v>3.1754301527896995</v>
+      </c>
+      <c r="X109" s="2"/>
+      <c r="Y109" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z109" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="110" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C110">
         <f>112/2</f>
         <v>56</v>
@@ -4420,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="N110" s="2">
-        <v>3.48</v>
+        <v>3.25</v>
       </c>
       <c r="O110" s="2">
-        <v>4.09</v>
+        <v>3.67</v>
       </c>
       <c r="P110" s="2">
-        <v>4.33</v>
+        <v>3.93</v>
       </c>
       <c r="R110" s="4">
         <f t="shared" si="3"/>
@@ -4438,23 +4658,32 @@
       </c>
       <c r="T110" s="2">
         <f t="shared" ref="T110:T113" si="11">N110+O110+P110</f>
-        <v>11.9</v>
+        <v>10.85</v>
       </c>
       <c r="U110" s="2">
         <f t="shared" si="5"/>
-        <v>4.2521564689655174</v>
+        <v>4.5530783113846152</v>
       </c>
       <c r="V110" s="2">
         <f t="shared" si="6"/>
-        <v>3.6179717633251838</v>
+        <v>4.0320175782016348</v>
       </c>
       <c r="W110" s="2">
         <f t="shared" si="7"/>
-        <v>3.417437531639723</v>
-      </c>
-      <c r="X110" s="3"/>
-    </row>
-    <row r="111" spans="3:24">
+        <v>3.7652683236641216</v>
+      </c>
+      <c r="X110" s="2"/>
+      <c r="Y110" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z110" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA110" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="111" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C111">
         <f>56/2</f>
         <v>28</v>
@@ -4490,13 +4719,13 @@
         <v>1</v>
       </c>
       <c r="N111" s="2">
-        <v>3.3200000000000003</v>
+        <v>3.06</v>
       </c>
       <c r="O111" s="2">
-        <v>3.71</v>
+        <v>3.7976000000000001</v>
       </c>
       <c r="P111" s="2">
-        <v>3.84</v>
+        <v>3.62</v>
       </c>
       <c r="R111" s="4">
         <f t="shared" si="3"/>
@@ -4508,23 +4737,32 @@
       </c>
       <c r="T111" s="2">
         <f t="shared" si="11"/>
-        <v>10.870000000000001</v>
+        <v>10.477599999999999</v>
       </c>
       <c r="U111" s="2">
         <f t="shared" si="5"/>
-        <v>4.4570796722891561</v>
+        <v>4.8357857882352944</v>
       </c>
       <c r="V111" s="2">
         <f t="shared" si="6"/>
-        <v>3.9885456905660379</v>
+        <v>3.8965411080682539</v>
       </c>
       <c r="W111" s="2">
         <f t="shared" si="7"/>
-        <v>3.8535168000000004</v>
-      </c>
-      <c r="X111" s="3"/>
-    </row>
-    <row r="112" spans="3:24">
+        <v>4.0877084287292815</v>
+      </c>
+      <c r="X111" s="2"/>
+      <c r="Y111" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z111" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA111" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C112">
         <v>14</v>
       </c>
@@ -4559,13 +4797,13 @@
         <v>1</v>
       </c>
       <c r="N112" s="2">
-        <v>1.78</v>
+        <v>1.62</v>
       </c>
       <c r="O112" s="2">
-        <v>2</v>
+        <v>2.2144999999999997</v>
       </c>
       <c r="P112" s="2">
-        <v>2.2599999999999998</v>
+        <v>1.89</v>
       </c>
       <c r="R112" s="4">
         <f t="shared" si="3"/>
@@ -4577,23 +4815,32 @@
       </c>
       <c r="T112" s="2">
         <f t="shared" si="11"/>
-        <v>6.04</v>
+        <v>5.7244999999999999</v>
       </c>
       <c r="U112" s="2">
         <f t="shared" si="5"/>
-        <v>4.1566023910112362</v>
+        <v>4.5671310222222221</v>
       </c>
       <c r="V112" s="2">
         <f t="shared" si="6"/>
-        <v>3.6993761279999999</v>
+        <v>3.3410486592910367</v>
       </c>
       <c r="W112" s="2">
         <f t="shared" si="7"/>
-        <v>3.2737841840707969</v>
-      </c>
-      <c r="X112" s="3"/>
-    </row>
-    <row r="113" spans="3:24">
+        <v>3.9146837333333333</v>
+      </c>
+      <c r="X112" s="2"/>
+      <c r="Y112" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z112" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA112" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="113" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C113">
         <v>7</v>
       </c>
@@ -4628,13 +4875,13 @@
         <v>1</v>
       </c>
       <c r="N113" s="2">
-        <v>0.84</v>
+        <v>0.75</v>
       </c>
       <c r="O113" s="2">
-        <v>0.91</v>
+        <v>1.2293000000000001</v>
       </c>
       <c r="P113" s="2">
-        <v>0.65</v>
+        <v>0.48768</v>
       </c>
       <c r="R113" s="4">
         <f t="shared" si="3"/>
@@ -4646,23 +4893,32 @@
       </c>
       <c r="T113" s="2">
         <f t="shared" si="11"/>
-        <v>2.4</v>
+        <v>2.46698</v>
       </c>
       <c r="U113" s="2">
         <f t="shared" si="5"/>
-        <v>2.2020095999999998</v>
+        <v>2.4662507520000001</v>
       </c>
       <c r="V113" s="2">
         <f t="shared" si="6"/>
-        <v>2.0326242461538464</v>
+        <v>1.5046677491255185</v>
       </c>
       <c r="W113" s="2">
         <f t="shared" si="7"/>
-        <v>2.8456739446153847</v>
-      </c>
-      <c r="X113" s="3"/>
-    </row>
-    <row r="114" spans="3:24">
+        <v>3.7928314960629921</v>
+      </c>
+      <c r="X113" s="2"/>
+      <c r="Y113" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA113" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C114">
         <v>224</v>
       </c>
@@ -4697,13 +4953,13 @@
         <v>1</v>
       </c>
       <c r="N114" s="2">
-        <v>2.2800000000000002</v>
+        <v>2.19</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P114" s="2">
-        <v>2.08</v>
+        <v>1.98</v>
       </c>
       <c r="R114" s="4">
         <f t="shared" si="3"/>
@@ -4715,22 +4971,31 @@
       </c>
       <c r="T114" s="2">
         <f>N114+P114</f>
-        <v>4.3600000000000003</v>
+        <v>4.17</v>
       </c>
       <c r="U114" s="2">
         <f t="shared" si="5"/>
-        <v>1.2169000421052629</v>
+        <v>1.2669096328767122</v>
       </c>
       <c r="V114" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W114" s="2">
         <f t="shared" si="7"/>
-        <v>1.3339096615384614</v>
-      </c>
-      <c r="X114" s="3"/>
-    </row>
-    <row r="115" spans="3:24">
+        <v>1.4012788363636364</v>
+      </c>
+      <c r="X114" s="2"/>
+      <c r="Y114" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z114" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA114" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C115">
         <v>112</v>
       </c>
@@ -4765,13 +5030,13 @@
         <v>1</v>
       </c>
       <c r="N115" s="2">
-        <v>7.07</v>
+        <v>6.86</v>
       </c>
       <c r="O115" s="2">
-        <v>10.58</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="P115" s="2">
-        <v>9.25</v>
+        <v>9.17</v>
       </c>
       <c r="R115" s="4">
         <f t="shared" si="3"/>
@@ -4783,23 +5048,32 @@
       </c>
       <c r="T115" s="2">
         <f>N115+O115+P115</f>
-        <v>26.9</v>
+        <v>25.229999999999997</v>
       </c>
       <c r="U115" s="2">
         <f t="shared" si="5"/>
-        <v>4.185998447524752</v>
+        <v>4.3141412571428566</v>
       </c>
       <c r="V115" s="2">
         <f t="shared" si="6"/>
-        <v>2.7972598321361053</v>
+        <v>3.2168488069565218</v>
       </c>
       <c r="W115" s="2">
         <f t="shared" si="7"/>
-        <v>3.1994604350270275</v>
-      </c>
-      <c r="X115" s="3"/>
-    </row>
-    <row r="116" spans="3:24">
+        <v>3.2273728488549618</v>
+      </c>
+      <c r="X115" s="2"/>
+      <c r="Y115" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA115" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C116">
         <f>112/2</f>
         <v>56</v>
@@ -4835,13 +5109,13 @@
         <v>1</v>
       </c>
       <c r="N116" s="2">
-        <v>6.72</v>
+        <v>6.44</v>
       </c>
       <c r="O116" s="2">
-        <v>8.27</v>
+        <v>7.44</v>
       </c>
       <c r="P116" s="2">
-        <v>8.36</v>
+        <v>7.84</v>
       </c>
       <c r="R116" s="4">
         <f t="shared" si="3"/>
@@ -4853,23 +5127,32 @@
       </c>
       <c r="T116" s="2">
         <f t="shared" ref="T116:T119" si="12">N116+O116+P116</f>
-        <v>23.349999999999998</v>
+        <v>21.72</v>
       </c>
       <c r="U116" s="2">
         <f t="shared" si="5"/>
-        <v>4.4040191999999996</v>
+        <v>4.5954982956521739</v>
       </c>
       <c r="V116" s="2">
         <f t="shared" si="6"/>
-        <v>3.5785984309552603</v>
+        <v>3.9778237935483869</v>
       </c>
       <c r="W116" s="2">
         <f t="shared" si="7"/>
-        <v>3.5400728497607656</v>
-      </c>
-      <c r="X116" s="3"/>
-    </row>
-    <row r="117" spans="3:24">
+        <v>3.7748735999999998</v>
+      </c>
+      <c r="X116" s="2"/>
+      <c r="Y116" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z116" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA116" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="117" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C117">
         <f>56/2</f>
         <v>28</v>
@@ -4905,13 +5188,13 @@
         <v>1</v>
       </c>
       <c r="N117" s="2">
-        <v>6.41</v>
+        <v>6.07</v>
       </c>
       <c r="O117" s="2">
-        <v>7.41</v>
+        <v>7.4197999999999995</v>
       </c>
       <c r="P117" s="2">
-        <v>7.61</v>
+        <v>7.22</v>
       </c>
       <c r="R117" s="4">
         <f t="shared" si="3"/>
@@ -4923,23 +5206,32 @@
       </c>
       <c r="T117" s="2">
         <f t="shared" si="12"/>
-        <v>21.43</v>
+        <v>20.709799999999998</v>
       </c>
       <c r="U117" s="2">
         <f t="shared" si="5"/>
-        <v>4.6170060879875194</v>
+        <v>4.87561927907743</v>
       </c>
       <c r="V117" s="2">
         <f t="shared" si="6"/>
-        <v>3.9939283433198378</v>
+        <v>3.9886532014340008</v>
       </c>
       <c r="W117" s="2">
         <f t="shared" si="7"/>
-        <v>3.8889630780551903</v>
-      </c>
-      <c r="X117" s="3"/>
-    </row>
-    <row r="118" spans="3:24">
+        <v>4.0990317207756233</v>
+      </c>
+      <c r="X117" s="2"/>
+      <c r="Y117" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z117" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA117" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="118" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C118">
         <v>14</v>
       </c>
@@ -4974,13 +5266,13 @@
         <v>1</v>
       </c>
       <c r="N118" s="2">
-        <v>3.41</v>
+        <v>3.19</v>
       </c>
       <c r="O118" s="2">
-        <v>3.92</v>
+        <v>4.0324</v>
       </c>
       <c r="P118" s="2">
-        <v>4.3600000000000003</v>
+        <v>3.72</v>
       </c>
       <c r="R118" s="4">
         <f t="shared" si="3"/>
@@ -4992,23 +5284,32 @@
       </c>
       <c r="T118" s="2">
         <f t="shared" si="12"/>
-        <v>11.690000000000001</v>
+        <v>10.942400000000001</v>
       </c>
       <c r="U118" s="2">
         <f t="shared" si="5"/>
-        <v>4.3394441384164217</v>
+        <v>4.6387161479623815</v>
       </c>
       <c r="V118" s="2">
         <f t="shared" si="6"/>
-        <v>3.7748735999999998</v>
+        <v>3.6696519472274574</v>
       </c>
       <c r="W118" s="2">
         <f t="shared" si="7"/>
-        <v>3.3939230532110094</v>
-      </c>
-      <c r="X118" s="3"/>
-    </row>
-    <row r="119" spans="3:24">
+        <v>3.9778237935483869</v>
+      </c>
+      <c r="X118" s="2"/>
+      <c r="Y118" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z118" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA118" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="119" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C119">
         <v>7</v>
       </c>
@@ -5043,13 +5344,13 @@
         <v>1</v>
       </c>
       <c r="N119" s="2">
-        <v>1.61</v>
+        <v>1.46</v>
       </c>
       <c r="O119" s="2">
-        <v>1.74</v>
+        <v>2.0040999999999998</v>
       </c>
       <c r="P119" s="2">
-        <v>1.2</v>
+        <v>0.95377999999999996</v>
       </c>
       <c r="R119" s="4">
         <f t="shared" si="3"/>
@@ -5061,23 +5362,32 @@
       </c>
       <c r="T119" s="2">
         <f t="shared" si="12"/>
-        <v>4.55</v>
+        <v>4.4178799999999994</v>
       </c>
       <c r="U119" s="2">
         <f t="shared" si="5"/>
-        <v>2.297749147826087</v>
+        <v>2.5338192657534249</v>
       </c>
       <c r="V119" s="2">
         <f t="shared" si="6"/>
-        <v>2.1260782344827587</v>
+        <v>1.8459039608801955</v>
       </c>
       <c r="W119" s="2">
         <f t="shared" si="7"/>
-        <v>3.0828134400000007</v>
-      </c>
-      <c r="X119" s="3"/>
-    </row>
-    <row r="120" spans="3:24">
+        <v>3.87864720166076</v>
+      </c>
+      <c r="X119" s="2"/>
+      <c r="Y119" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z119" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA119" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="120" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C120">
         <v>224</v>
       </c>
@@ -5112,13 +5422,13 @@
         <v>2</v>
       </c>
       <c r="N120" s="2">
-        <v>1.48</v>
+        <v>1.1554</v>
       </c>
       <c r="O120" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P120" s="2">
-        <v>1.6</v>
+        <v>1.53</v>
       </c>
       <c r="R120" s="4">
         <f t="shared" si="3"/>
@@ -5130,22 +5440,31 @@
       </c>
       <c r="T120" s="2">
         <f>N120+P120</f>
-        <v>3.08</v>
+        <v>2.6854</v>
       </c>
       <c r="U120" s="2">
         <f t="shared" si="5"/>
-        <v>2.5516530162162163</v>
+        <v>3.2685186636662626</v>
       </c>
       <c r="V120" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W120" s="2">
         <f t="shared" si="7"/>
-        <v>2.36027904</v>
-      </c>
-      <c r="X120" s="3"/>
-    </row>
-    <row r="121" spans="3:24">
+        <v>2.4682656627450976</v>
+      </c>
+      <c r="X120" s="2"/>
+      <c r="Y120" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z120" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA120" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>28</v>
       </c>
@@ -5180,13 +5499,13 @@
         <v>1</v>
       </c>
       <c r="N121" s="2">
-        <v>0.89871654461495409</v>
+        <v>1.3607</v>
       </c>
       <c r="O121" s="2">
-        <v>0.88</v>
+        <v>0.89434000000000002</v>
       </c>
       <c r="P121" s="2">
-        <v>1.3</v>
+        <v>1.24</v>
       </c>
       <c r="R121" s="4">
         <f t="shared" si="3"/>
@@ -5198,23 +5517,32 @@
       </c>
       <c r="T121" s="2">
         <f>N121+O121+P121</f>
-        <v>3.078716544614954</v>
+        <v>3.4950400000000004</v>
       </c>
       <c r="U121" s="2">
         <f t="shared" si="5"/>
-        <v>4.2877999999999998</v>
+        <v>2.8320105827882704</v>
       </c>
       <c r="V121" s="2">
         <f t="shared" si="6"/>
-        <v>4.3789963636363636</v>
+        <v>4.3087827895431268</v>
       </c>
       <c r="W121" s="2">
         <f t="shared" si="7"/>
-        <v>2.9642436923076922</v>
-      </c>
-      <c r="X121" s="3"/>
-    </row>
-    <row r="122" spans="3:24">
+        <v>3.1076748387096771</v>
+      </c>
+      <c r="X121" s="2"/>
+      <c r="Y121" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z121" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA121" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C122">
         <v>28</v>
       </c>
@@ -5249,13 +5577,13 @@
         <v>1</v>
       </c>
       <c r="N122" s="2">
-        <v>0.1078246105417789</v>
+        <v>0.09</v>
       </c>
       <c r="O122" s="2">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="P122" s="2">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="R122" s="4">
         <f t="shared" si="3"/>
@@ -5267,23 +5595,32 @@
       </c>
       <c r="T122" s="2">
         <f t="shared" ref="T122:T126" si="13">N122+O122+P122</f>
-        <v>0.59782461054177882</v>
+        <v>0.7</v>
       </c>
       <c r="U122" s="2">
         <f t="shared" si="5"/>
-        <v>2.8590999999999993</v>
+        <v>3.425348266666667</v>
       </c>
       <c r="V122" s="2">
         <f t="shared" si="6"/>
-        <v>1.622533389473684</v>
+        <v>1.9267583999999998</v>
       </c>
       <c r="W122" s="2">
         <f t="shared" si="7"/>
-        <v>1.0276044800000002</v>
-      </c>
-      <c r="X122" s="3"/>
-    </row>
-    <row r="123" spans="3:24">
+        <v>0.68506965333333336</v>
+      </c>
+      <c r="X122" s="2"/>
+      <c r="Y122" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z122" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA122" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="123" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C123">
         <v>14</v>
       </c>
@@ -5318,13 +5655,13 @@
         <v>1</v>
       </c>
       <c r="N123" s="2">
-        <v>1.21</v>
+        <v>1.07</v>
       </c>
       <c r="O123" s="2">
-        <v>0.92</v>
+        <v>1.0742</v>
       </c>
       <c r="P123" s="2">
-        <v>1.01</v>
+        <v>0.89</v>
       </c>
       <c r="R123" s="4">
         <f t="shared" si="3"/>
@@ -5336,23 +5673,32 @@
       </c>
       <c r="T123" s="2">
         <f t="shared" si="13"/>
-        <v>3.1399999999999997</v>
+        <v>3.0342000000000002</v>
       </c>
       <c r="U123" s="2">
         <f t="shared" si="5"/>
-        <v>3.1847246280991737</v>
+        <v>3.6014175700934579</v>
       </c>
       <c r="V123" s="2">
         <f t="shared" si="6"/>
-        <v>4.188605217391304</v>
+        <v>3.5873364364177993</v>
       </c>
       <c r="W123" s="2">
         <f t="shared" si="7"/>
-        <v>3.8153631683168316</v>
-      </c>
-      <c r="X123" s="3"/>
-    </row>
-    <row r="124" spans="3:24">
+        <v>4.3297941573033709</v>
+      </c>
+      <c r="X123" s="2"/>
+      <c r="Y123" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z123" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA123" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="124" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C124">
         <v>14</v>
       </c>
@@ -5387,13 +5733,13 @@
         <v>1</v>
       </c>
       <c r="N124" s="2">
-        <v>0.179724447035504</v>
+        <v>0.18</v>
       </c>
       <c r="O124" s="2">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="P124" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="R124" s="4">
         <f t="shared" si="3"/>
@@ -5405,23 +5751,32 @@
       </c>
       <c r="T124" s="2">
         <f t="shared" si="13"/>
-        <v>1.019724447035504</v>
+        <v>0.99</v>
       </c>
       <c r="U124" s="2">
         <f t="shared" si="5"/>
-        <v>3.4306000000000001</v>
+        <v>3.425348266666667</v>
       </c>
       <c r="V124" s="2">
         <f t="shared" si="6"/>
-        <v>2.3713949538461532</v>
+        <v>2.5690111999999998</v>
       </c>
       <c r="W124" s="2">
         <f t="shared" si="7"/>
-        <v>1.0630391172413793</v>
-      </c>
-      <c r="X124" s="3"/>
-    </row>
-    <row r="125" spans="3:24">
+        <v>1.0816889263157896</v>
+      </c>
+      <c r="X124" s="2"/>
+      <c r="Y124" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z124" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA124" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C125">
         <v>7</v>
       </c>
@@ -5456,13 +5811,13 @@
         <v>1</v>
       </c>
       <c r="N125" s="2">
-        <v>0.15741490196078431</v>
+        <v>0.2</v>
       </c>
       <c r="O125" s="2">
-        <v>0.22</v>
+        <v>0.20283999999999999</v>
       </c>
       <c r="P125" s="2">
-        <v>0.38</v>
+        <v>0.21312</v>
       </c>
       <c r="R125" s="4">
         <f t="shared" si="3"/>
@@ -5474,23 +5829,32 @@
       </c>
       <c r="T125" s="2">
         <f t="shared" si="13"/>
-        <v>0.75741490196078431</v>
+        <v>0.61595999999999995</v>
       </c>
       <c r="U125" s="2">
         <f t="shared" si="5"/>
-        <v>2.1215999999999999</v>
+        <v>1.66985728</v>
       </c>
       <c r="V125" s="2">
         <f t="shared" si="6"/>
-        <v>1.5180520727272726</v>
+        <v>1.6464773023072372</v>
       </c>
       <c r="W125" s="2">
         <f t="shared" si="7"/>
-        <v>0.87887225263157887</v>
-      </c>
-      <c r="X125" s="3"/>
-    </row>
-    <row r="126" spans="3:24">
+        <v>1.5670582582582584</v>
+      </c>
+      <c r="X125" s="2"/>
+      <c r="Y125" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z125" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA125" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C126">
         <v>7</v>
       </c>
@@ -5525,13 +5889,13 @@
         <v>1</v>
       </c>
       <c r="N126" s="2">
-        <v>1.93</v>
+        <v>1.7</v>
       </c>
       <c r="O126" s="2">
-        <v>1.77</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="P126" s="2">
-        <v>1.27</v>
+        <v>1.0803</v>
       </c>
       <c r="R126" s="4">
         <f t="shared" si="3"/>
@@ -5543,31 +5907,40 @@
       </c>
       <c r="T126" s="2">
         <f t="shared" si="13"/>
-        <v>4.9700000000000006</v>
+        <v>4.9583000000000004</v>
       </c>
       <c r="U126" s="2">
         <f t="shared" si="5"/>
-        <v>2.1630275647668396</v>
+        <v>2.4556724705882353</v>
       </c>
       <c r="V126" s="2">
         <f t="shared" si="6"/>
-        <v>2.3585554802259887</v>
+        <v>1.9167324150596881</v>
       </c>
       <c r="W126" s="2">
         <f t="shared" si="7"/>
-        <v>3.2871206299212599</v>
-      </c>
-      <c r="X126" s="3"/>
-    </row>
-    <row r="129" spans="1:12">
+        <v>3.8643369434416366</v>
+      </c>
+      <c r="X126" s="2"/>
+      <c r="Y126" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA126" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L135" s="1"/>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -5593,7 +5966,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C138">
         <v>1760</v>
       </c>
@@ -5608,7 +5981,7 @@
       <c r="I138" s="9"/>
       <c r="J138" s="9"/>
     </row>
-    <row r="139" spans="1:12">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C139">
         <v>1760</v>
       </c>
@@ -5623,7 +5996,7 @@
       <c r="I139" s="9"/>
       <c r="J139" s="9"/>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C140">
         <v>1760</v>
       </c>
@@ -5638,7 +6011,7 @@
       <c r="I140" s="9"/>
       <c r="J140" s="9"/>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C141">
         <v>1760</v>
       </c>
@@ -5653,7 +6026,7 @@
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C142">
         <v>2048</v>
       </c>
@@ -5668,7 +6041,7 @@
       <c r="I142" s="9"/>
       <c r="J142" s="9"/>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C143">
         <v>2048</v>
       </c>
@@ -5683,7 +6056,7 @@
       <c r="I143" s="9"/>
       <c r="J143" s="9"/>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C144">
         <v>2048</v>
       </c>
@@ -5698,7 +6071,7 @@
       <c r="I144" s="9"/>
       <c r="J144" s="9"/>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C145">
         <v>2048</v>
       </c>
@@ -5713,7 +6086,7 @@
       <c r="I145" s="9"/>
       <c r="J145" s="9"/>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C146">
         <v>2560</v>
       </c>
@@ -5728,7 +6101,7 @@
       <c r="I146" s="9"/>
       <c r="J146" s="9"/>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C147">
         <v>2560</v>
       </c>
@@ -5743,7 +6116,7 @@
       <c r="I147" s="9"/>
       <c r="J147" s="9"/>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C148">
         <v>2560</v>
       </c>
@@ -5758,7 +6131,7 @@
       <c r="I148" s="9"/>
       <c r="J148" s="9"/>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C149">
         <v>2560</v>
       </c>
@@ -5773,10 +6146,10 @@
       <c r="I149" s="9"/>
       <c r="J149" s="9"/>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I151" s="1"/>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -5802,7 +6175,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C154">
         <v>512</v>
       </c>
@@ -5817,7 +6190,7 @@
       <c r="I154" s="9"/>
       <c r="J154" s="9"/>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C155">
         <v>512</v>
       </c>
@@ -5832,7 +6205,7 @@
       <c r="I155" s="9"/>
       <c r="J155" s="9"/>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C156">
         <v>512</v>
       </c>
@@ -5847,7 +6220,7 @@
       <c r="I156" s="9"/>
       <c r="J156" s="9"/>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C157">
         <v>512</v>
       </c>
@@ -5862,7 +6235,7 @@
       <c r="I157" s="9"/>
       <c r="J157" s="9"/>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C158">
         <v>1024</v>
       </c>
@@ -5877,7 +6250,7 @@
       <c r="I158" s="9"/>
       <c r="J158" s="9"/>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C159">
         <v>1024</v>
       </c>
@@ -5892,7 +6265,7 @@
       <c r="I159" s="9"/>
       <c r="J159" s="9"/>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C160">
         <v>1024</v>
       </c>
@@ -5907,7 +6280,7 @@
       <c r="I160" s="9"/>
       <c r="J160" s="9"/>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C161">
         <v>1024</v>
       </c>
@@ -5922,7 +6295,7 @@
       <c r="I161" s="9"/>
       <c r="J161" s="9"/>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C162">
         <v>2048</v>
       </c>
@@ -5937,7 +6310,7 @@
       <c r="I162" s="9"/>
       <c r="J162" s="9"/>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C163">
         <v>2048</v>
       </c>
@@ -5952,7 +6325,7 @@
       <c r="I163" s="9"/>
       <c r="J163" s="9"/>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C164">
         <v>2048</v>
       </c>
@@ -5967,7 +6340,7 @@
       <c r="I164" s="9"/>
       <c r="J164" s="9"/>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C165">
         <v>2048</v>
       </c>
@@ -5982,7 +6355,7 @@
       <c r="I165" s="9"/>
       <c r="J165" s="9"/>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C166">
         <v>4096</v>
       </c>
@@ -5997,7 +6370,7 @@
       <c r="I166" s="9"/>
       <c r="J166" s="9"/>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C167">
         <v>4096</v>
       </c>
@@ -6012,7 +6385,7 @@
       <c r="I167" s="9"/>
       <c r="J167" s="9"/>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C168">
         <v>4096</v>
       </c>
@@ -6027,7 +6400,7 @@
       <c r="I168" s="9"/>
       <c r="J168" s="9"/>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C169">
         <v>4096</v>
       </c>
@@ -6042,16 +6415,16 @@
       <c r="I169" s="9"/>
       <c r="J169" s="9"/>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I171" s="1"/>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
       <c r="K172" s="2"/>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>4</v>
       </c>
@@ -6074,7 +6447,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C175">
         <v>100000</v>
       </c>
@@ -6099,7 +6472,7 @@
       <c r="N175" s="2"/>
       <c r="O175" s="2"/>
     </row>
-    <row r="176" spans="1:15">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C176">
         <v>100000</v>
       </c>
@@ -6124,7 +6497,7 @@
       <c r="N176" s="2"/>
       <c r="O176" s="2"/>
     </row>
-    <row r="177" spans="3:15">
+    <row r="177" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C177">
         <v>100000</v>
       </c>
@@ -6149,7 +6522,7 @@
       <c r="N177" s="2"/>
       <c r="O177" s="2"/>
     </row>
-    <row r="178" spans="3:15">
+    <row r="178" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C178">
         <v>100000</v>
       </c>
@@ -6174,7 +6547,7 @@
       </c>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="3:15">
+    <row r="179" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C179">
         <v>100000</v>
       </c>
@@ -6199,7 +6572,7 @@
       </c>
       <c r="L179" s="2"/>
     </row>
-    <row r="180" spans="3:15">
+    <row r="180" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C180">
         <v>3097600</v>
       </c>
@@ -6224,7 +6597,7 @@
       <c r="N180" s="2"/>
       <c r="O180" s="2"/>
     </row>
-    <row r="181" spans="3:15">
+    <row r="181" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C181">
         <f>1760*1760</f>
         <v>3097600</v>
@@ -6250,7 +6623,7 @@
       <c r="N181" s="2"/>
       <c r="O181" s="2"/>
     </row>
-    <row r="182" spans="3:15">
+    <row r="182" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C182">
         <f>1760*1760</f>
         <v>3097600</v>
@@ -6276,7 +6649,7 @@
       <c r="N182" s="2"/>
       <c r="O182" s="2"/>
     </row>
-    <row r="183" spans="3:15">
+    <row r="183" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C183">
         <v>3097600</v>
       </c>
@@ -6301,7 +6674,7 @@
       </c>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="3:15">
+    <row r="184" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C184">
         <v>3097600</v>
       </c>
@@ -6326,7 +6699,7 @@
       </c>
       <c r="L184" s="2"/>
     </row>
-    <row r="185" spans="3:15">
+    <row r="185" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C185">
         <v>4194304</v>
       </c>
@@ -6351,7 +6724,7 @@
       <c r="N185" s="2"/>
       <c r="O185" s="2"/>
     </row>
-    <row r="186" spans="3:15">
+    <row r="186" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C186">
         <f>2048*2048</f>
         <v>4194304</v>
@@ -6377,7 +6750,7 @@
       <c r="N186" s="2"/>
       <c r="O186" s="2"/>
     </row>
-    <row r="187" spans="3:15">
+    <row r="187" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C187">
         <f>2048*2048</f>
         <v>4194304</v>
@@ -6403,7 +6776,7 @@
       <c r="N187" s="2"/>
       <c r="O187" s="2"/>
     </row>
-    <row r="188" spans="3:15">
+    <row r="188" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C188">
         <v>4194304</v>
       </c>
@@ -6429,7 +6802,7 @@
       <c r="L188" s="2"/>
       <c r="O188" s="2"/>
     </row>
-    <row r="189" spans="3:15">
+    <row r="189" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C189">
         <v>4194304</v>
       </c>
@@ -6455,7 +6828,7 @@
       <c r="L189" s="2"/>
       <c r="O189" s="2"/>
     </row>
-    <row r="190" spans="3:15">
+    <row r="190" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C190">
         <v>6553600</v>
       </c>
@@ -6480,7 +6853,7 @@
       <c r="N190" s="2"/>
       <c r="O190" s="2"/>
     </row>
-    <row r="191" spans="3:15">
+    <row r="191" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C191">
         <f>2560*2560</f>
         <v>6553600</v>
@@ -6506,7 +6879,7 @@
       <c r="N191" s="2"/>
       <c r="O191" s="2"/>
     </row>
-    <row r="192" spans="3:15">
+    <row r="192" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C192">
         <f>2560*2560</f>
         <v>6553600</v>
@@ -6532,7 +6905,7 @@
       <c r="N192" s="2"/>
       <c r="O192" s="2"/>
     </row>
-    <row r="193" spans="3:16">
+    <row r="193" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C193">
         <v>6553600</v>
       </c>
@@ -6557,7 +6930,7 @@
       </c>
       <c r="L193" s="2"/>
     </row>
-    <row r="194" spans="3:16">
+    <row r="194" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C194">
         <v>6553600</v>
       </c>
@@ -6582,7 +6955,7 @@
       </c>
       <c r="L194" s="2"/>
     </row>
-    <row r="195" spans="3:16">
+    <row r="195" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C195">
         <f t="shared" ref="C195:C197" si="15">4096*4096</f>
         <v>16777216</v>
@@ -6608,7 +6981,7 @@
       <c r="N195" s="2"/>
       <c r="O195" s="2"/>
     </row>
-    <row r="196" spans="3:16">
+    <row r="196" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C196">
         <f t="shared" si="15"/>
         <v>16777216</v>
@@ -6634,7 +7007,7 @@
       <c r="N196" s="2"/>
       <c r="O196" s="2"/>
     </row>
-    <row r="197" spans="3:16">
+    <row r="197" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C197">
         <f t="shared" si="15"/>
         <v>16777216</v>
@@ -6660,7 +7033,7 @@
       <c r="N197" s="2"/>
       <c r="O197" s="2"/>
     </row>
-    <row r="198" spans="3:16">
+    <row r="198" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C198">
         <v>16777216</v>
       </c>
@@ -6687,7 +7060,7 @@
       <c r="L198" s="2"/>
       <c r="N198" s="2"/>
     </row>
-    <row r="199" spans="3:16">
+    <row r="199" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C199">
         <v>16777216</v>
       </c>
@@ -6714,7 +7087,7 @@
       <c r="L199" s="2"/>
       <c r="N199" s="2"/>
     </row>
-    <row r="200" spans="3:16">
+    <row r="200" spans="3:16" x14ac:dyDescent="0.25">
       <c r="I200" s="2"/>
       <c r="J200" s="2"/>
       <c r="K200" s="2"/>
@@ -6724,10 +7097,10 @@
       <c r="O200" s="2"/>
       <c r="P200" s="2"/>
     </row>
-    <row r="201" spans="3:16">
+    <row r="201" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G201" s="1"/>
     </row>
-    <row r="207" spans="3:16">
+    <row r="207" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G207" s="1"/>
     </row>
   </sheetData>
@@ -6743,35 +7116,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -6779,48 +7152,57 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Explicitly mark a couple of kernels that aren't used for backward_wrt_inputs calculations.
</commit_message>
<xml_diff>
--- a/results/DeepBench_IA_KNL7250.xlsx
+++ b/results/DeepBench_IA_KNL7250.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmudiger\Documents\Work\DL\DeepBench\my_DeepBench_gh_pub\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="555" yWindow="0" windowWidth="25035" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="34420" windowHeight="19800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Specs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="72">
   <si>
     <t xml:space="preserve">OSU MPI </t>
   </si>
@@ -767,32 +762,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA207"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="32.625" customWidth="1"/>
-    <col min="9" max="9" width="26.125" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="24.125" customWidth="1"/>
-    <col min="12" max="12" width="18.625" customWidth="1"/>
-    <col min="13" max="13" width="15.875" customWidth="1"/>
-    <col min="14" max="14" width="20.125" customWidth="1"/>
+    <col min="11" max="11" width="24.1640625" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="20" max="20" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="14.375" customWidth="1"/>
-    <col min="25" max="27" width="15.625" customWidth="1"/>
+    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="14.33203125" customWidth="1"/>
+    <col min="25" max="27" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -818,7 +811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="C2">
         <v>1760</v>
       </c>
@@ -846,7 +839,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="C3">
         <v>1760</v>
       </c>
@@ -874,7 +867,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="C4">
         <v>1760</v>
       </c>
@@ -902,7 +895,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="C5">
         <v>1760</v>
       </c>
@@ -930,7 +923,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="C6">
         <v>1760</v>
       </c>
@@ -958,7 +951,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="C7">
         <v>2048</v>
       </c>
@@ -986,7 +979,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="C8">
         <v>2048</v>
       </c>
@@ -1014,7 +1007,7 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="C9">
         <v>2048</v>
       </c>
@@ -1042,7 +1035,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="C10">
         <v>2048</v>
       </c>
@@ -1070,7 +1063,7 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="C11">
         <v>2048</v>
       </c>
@@ -1098,7 +1091,7 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="C12">
         <v>2560</v>
       </c>
@@ -1126,7 +1119,7 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="C13">
         <v>2560</v>
       </c>
@@ -1154,7 +1147,7 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="C14">
         <v>2560</v>
       </c>
@@ -1182,7 +1175,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="C15">
         <v>2560</v>
       </c>
@@ -1210,7 +1203,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="C16">
         <v>2560</v>
       </c>
@@ -1238,7 +1231,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:18">
       <c r="C17">
         <v>4096</v>
       </c>
@@ -1266,7 +1259,7 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:18">
       <c r="C18">
         <v>4096</v>
       </c>
@@ -1294,7 +1287,7 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:18">
       <c r="C19">
         <v>4096</v>
       </c>
@@ -1322,7 +1315,7 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:18">
       <c r="C20">
         <v>4096</v>
       </c>
@@ -1350,7 +1343,7 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:18">
       <c r="C21">
         <v>4096</v>
       </c>
@@ -1378,7 +1371,7 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:18">
       <c r="C22">
         <v>1760</v>
       </c>
@@ -1406,7 +1399,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:18">
       <c r="C23">
         <v>1760</v>
       </c>
@@ -1434,7 +1427,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:18">
       <c r="C24">
         <v>1760</v>
       </c>
@@ -1462,7 +1455,7 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:18">
       <c r="C25">
         <v>1760</v>
       </c>
@@ -1490,7 +1483,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:18">
       <c r="C26">
         <v>1760</v>
       </c>
@@ -1518,7 +1511,7 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:18">
       <c r="C27">
         <v>2048</v>
       </c>
@@ -1546,7 +1539,7 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:18">
       <c r="C28">
         <v>2048</v>
       </c>
@@ -1574,7 +1567,7 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:18">
       <c r="C29">
         <v>2048</v>
       </c>
@@ -1602,7 +1595,7 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:18">
       <c r="C30">
         <v>2048</v>
       </c>
@@ -1630,7 +1623,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:18">
       <c r="C31">
         <v>2048</v>
       </c>
@@ -1658,7 +1651,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:18">
       <c r="C32">
         <v>2560</v>
       </c>
@@ -1686,7 +1679,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:18">
       <c r="C33">
         <v>2560</v>
       </c>
@@ -1714,7 +1707,7 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:18">
       <c r="C34">
         <v>2560</v>
       </c>
@@ -1742,7 +1735,7 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:18">
       <c r="C35">
         <v>2560</v>
       </c>
@@ -1770,7 +1763,7 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:18">
       <c r="C36">
         <v>2560</v>
       </c>
@@ -1798,7 +1791,7 @@
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
     </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:18">
       <c r="C37">
         <v>4096</v>
       </c>
@@ -1826,7 +1819,7 @@
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
     </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:18">
       <c r="C38">
         <v>4096</v>
       </c>
@@ -1854,7 +1847,7 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:18">
       <c r="C39">
         <v>4096</v>
       </c>
@@ -1882,7 +1875,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:18">
       <c r="C40">
         <v>4096</v>
       </c>
@@ -1910,7 +1903,7 @@
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
     </row>
-    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:18">
       <c r="C41">
         <v>4096</v>
       </c>
@@ -1938,7 +1931,7 @@
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:18">
       <c r="C42">
         <v>1760</v>
       </c>
@@ -1969,7 +1962,7 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:18">
       <c r="C43">
         <v>2048</v>
       </c>
@@ -1997,7 +1990,7 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:18">
       <c r="C44">
         <v>2560</v>
       </c>
@@ -2025,7 +2018,7 @@
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
     </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:18">
       <c r="C45" s="3">
         <v>4096</v>
       </c>
@@ -2053,7 +2046,7 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:18">
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="M46" s="2"/>
@@ -2061,7 +2054,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:18">
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="M47" s="2"/>
@@ -2069,7 +2062,7 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:18">
       <c r="C48">
         <v>5124</v>
       </c>
@@ -2097,7 +2090,7 @@
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
-    <row r="49" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:18">
       <c r="C49">
         <v>35</v>
       </c>
@@ -2125,7 +2118,7 @@
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
     </row>
-    <row r="50" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:18">
       <c r="C50">
         <v>5124</v>
       </c>
@@ -2153,7 +2146,7 @@
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
     </row>
-    <row r="51" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:18">
       <c r="C51">
         <v>35</v>
       </c>
@@ -2181,7 +2174,7 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
     </row>
-    <row r="52" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:18">
       <c r="C52">
         <v>5124</v>
       </c>
@@ -2209,7 +2202,7 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
-    <row r="53" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:18">
       <c r="C53">
         <v>35</v>
       </c>
@@ -2237,7 +2230,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:18">
       <c r="C54">
         <v>5124</v>
       </c>
@@ -2265,7 +2258,7 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:18">
       <c r="C55">
         <v>35</v>
       </c>
@@ -2293,7 +2286,7 @@
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:18">
       <c r="C56">
         <v>5124</v>
       </c>
@@ -2321,7 +2314,7 @@
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:18">
       <c r="C57">
         <v>35</v>
       </c>
@@ -2349,7 +2342,7 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:18">
       <c r="C58">
         <v>5124</v>
       </c>
@@ -2377,7 +2370,7 @@
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
     </row>
-    <row r="59" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:18">
       <c r="C59">
         <v>35</v>
       </c>
@@ -2405,7 +2398,7 @@
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
     </row>
-    <row r="60" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:18">
       <c r="C60">
         <v>5124</v>
       </c>
@@ -2433,7 +2426,7 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
-    <row r="61" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:18">
       <c r="C61">
         <v>35</v>
       </c>
@@ -2461,7 +2454,7 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:18">
       <c r="C62">
         <v>5124</v>
       </c>
@@ -2489,7 +2482,7 @@
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
     </row>
-    <row r="63" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:18">
       <c r="C63">
         <v>35</v>
       </c>
@@ -2517,7 +2510,7 @@
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
     </row>
-    <row r="64" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:18">
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="M64" s="2"/>
@@ -2525,7 +2518,7 @@
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
     </row>
-    <row r="65" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:18">
       <c r="C65">
         <v>7680</v>
       </c>
@@ -2553,7 +2546,7 @@
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
     </row>
-    <row r="66" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:18">
       <c r="C66">
         <v>7680</v>
       </c>
@@ -2581,7 +2574,7 @@
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
     </row>
-    <row r="67" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:18">
       <c r="C67">
         <v>7680</v>
       </c>
@@ -2609,7 +2602,7 @@
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
-    <row r="68" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:18">
       <c r="C68">
         <v>7680</v>
       </c>
@@ -2637,7 +2630,7 @@
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
     </row>
-    <row r="69" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:18">
       <c r="C69">
         <v>7680</v>
       </c>
@@ -2665,7 +2658,7 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:18">
       <c r="C70">
         <v>7680</v>
       </c>
@@ -2693,7 +2686,7 @@
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
     </row>
-    <row r="71" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:18">
       <c r="C71">
         <v>7680</v>
       </c>
@@ -2721,7 +2714,7 @@
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
     </row>
-    <row r="72" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:18">
       <c r="C72">
         <v>7680</v>
       </c>
@@ -2749,7 +2742,7 @@
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
     </row>
-    <row r="73" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:18">
       <c r="C73">
         <f t="shared" ref="C73:C80" si="2">3*1024</f>
         <v>3072</v>
@@ -2778,7 +2771,7 @@
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
     </row>
-    <row r="74" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:18">
       <c r="C74">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2807,7 +2800,7 @@
       <c r="Q74" s="2"/>
       <c r="R74" s="2"/>
     </row>
-    <row r="75" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:18">
       <c r="C75">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2836,7 +2829,7 @@
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
     </row>
-    <row r="76" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:18">
       <c r="C76">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2865,7 +2858,7 @@
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
     </row>
-    <row r="77" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:18">
       <c r="C77">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2894,7 +2887,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:18">
       <c r="C78">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2923,7 +2916,7 @@
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
     </row>
-    <row r="79" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:18">
       <c r="C79">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2952,7 +2945,7 @@
       <c r="Q79" s="2"/>
       <c r="R79" s="2"/>
     </row>
-    <row r="80" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:18">
       <c r="C80">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2981,7 +2974,7 @@
       <c r="Q80" s="2"/>
       <c r="R80" s="2"/>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27">
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="M81" s="2"/>
@@ -2989,7 +2982,7 @@
       <c r="Q81" s="2"/>
       <c r="R81" s="2"/>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27">
       <c r="C82">
         <v>3072</v>
       </c>
@@ -3017,7 +3010,7 @@
       <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27">
       <c r="C83">
         <v>7680</v>
       </c>
@@ -3045,20 +3038,20 @@
       <c r="Q83" s="2"/>
       <c r="R83" s="2"/>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27">
       <c r="J85" s="2"/>
       <c r="N85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27">
       <c r="J87" s="1"/>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27">
       <c r="A89" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27">
       <c r="C90" t="s">
         <v>22</v>
       </c>
@@ -3129,7 +3122,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27">
       <c r="C91">
         <v>700</v>
       </c>
@@ -3206,7 +3199,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27">
       <c r="C92">
         <v>700</v>
       </c>
@@ -3283,7 +3276,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27">
       <c r="C93">
         <v>700</v>
       </c>
@@ -3360,7 +3353,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27">
       <c r="C94">
         <v>700</v>
       </c>
@@ -3437,7 +3430,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27">
       <c r="C95">
         <v>341</v>
       </c>
@@ -3515,7 +3508,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27">
       <c r="C96">
         <v>341</v>
       </c>
@@ -3593,7 +3586,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:27">
       <c r="C97">
         <v>341</v>
       </c>
@@ -3671,7 +3664,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:27">
       <c r="C98">
         <v>341</v>
       </c>
@@ -3749,7 +3742,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="99" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:27">
       <c r="C99">
         <v>480</v>
       </c>
@@ -3786,8 +3779,8 @@
       <c r="N99" s="2">
         <v>8.4348000000000006E-2</v>
       </c>
-      <c r="O99" s="2">
-        <v>2.94</v>
+      <c r="O99" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="P99" s="2">
         <v>0.66164999999999996</v>
@@ -3826,7 +3819,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:27">
       <c r="C100">
         <v>240</v>
       </c>
@@ -3904,7 +3897,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="101" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:27">
       <c r="C101">
         <v>120</v>
       </c>
@@ -3982,7 +3975,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="102" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:27">
       <c r="C102">
         <v>60</v>
       </c>
@@ -4060,7 +4053,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:27">
       <c r="C103">
         <v>108</v>
       </c>
@@ -4097,8 +4090,8 @@
       <c r="N103" s="2">
         <v>0.04</v>
       </c>
-      <c r="O103" s="2">
-        <v>2.89</v>
+      <c r="O103" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="P103" s="2">
         <v>7.0000000000000007E-2</v>
@@ -4137,7 +4130,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:27">
       <c r="C104">
         <v>54</v>
       </c>
@@ -4215,7 +4208,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="105" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:27">
       <c r="C105">
         <v>27</v>
       </c>
@@ -4293,7 +4286,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="106" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:27">
       <c r="C106">
         <v>14</v>
       </c>
@@ -4371,7 +4364,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:27">
       <c r="C107">
         <v>7</v>
       </c>
@@ -4449,7 +4442,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:27">
       <c r="C108">
         <v>224</v>
       </c>
@@ -4526,7 +4519,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:27">
       <c r="C109">
         <v>112</v>
       </c>
@@ -4604,7 +4597,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="110" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:27">
       <c r="C110">
         <f>112/2</f>
         <v>56</v>
@@ -4683,7 +4676,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="111" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:27">
       <c r="C111">
         <f>56/2</f>
         <v>28</v>
@@ -4762,7 +4755,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:27">
       <c r="C112">
         <v>14</v>
       </c>
@@ -4840,7 +4833,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="113" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:27">
       <c r="C113">
         <v>7</v>
       </c>
@@ -4918,7 +4911,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="114" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:27">
       <c r="C114">
         <v>224</v>
       </c>
@@ -4995,7 +4988,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="115" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:27">
       <c r="C115">
         <v>112</v>
       </c>
@@ -5073,7 +5066,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="116" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:27">
       <c r="C116">
         <f>112/2</f>
         <v>56</v>
@@ -5152,7 +5145,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="117" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:27">
       <c r="C117">
         <f>56/2</f>
         <v>28</v>
@@ -5231,7 +5224,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="118" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:27">
       <c r="C118">
         <v>14</v>
       </c>
@@ -5309,7 +5302,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="119" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:27">
       <c r="C119">
         <v>7</v>
       </c>
@@ -5387,7 +5380,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:27">
       <c r="C120">
         <v>224</v>
       </c>
@@ -5464,7 +5457,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="121" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:27">
       <c r="C121">
         <v>28</v>
       </c>
@@ -5542,7 +5535,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="122" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:27">
       <c r="C122">
         <v>28</v>
       </c>
@@ -5620,7 +5613,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="123" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:27">
       <c r="C123">
         <v>14</v>
       </c>
@@ -5698,7 +5691,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="124" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:27">
       <c r="C124">
         <v>14</v>
       </c>
@@ -5776,7 +5769,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:27">
       <c r="C125">
         <v>7</v>
       </c>
@@ -5854,7 +5847,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:27">
       <c r="C126">
         <v>7</v>
       </c>
@@ -5932,15 +5925,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12">
       <c r="D129" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12">
       <c r="L135" s="1"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -5966,7 +5959,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12">
       <c r="C138">
         <v>1760</v>
       </c>
@@ -5981,7 +5974,7 @@
       <c r="I138" s="9"/>
       <c r="J138" s="9"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12">
       <c r="C139">
         <v>1760</v>
       </c>
@@ -5996,7 +5989,7 @@
       <c r="I139" s="9"/>
       <c r="J139" s="9"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12">
       <c r="C140">
         <v>1760</v>
       </c>
@@ -6011,7 +6004,7 @@
       <c r="I140" s="9"/>
       <c r="J140" s="9"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12">
       <c r="C141">
         <v>1760</v>
       </c>
@@ -6026,7 +6019,7 @@
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12">
       <c r="C142">
         <v>2048</v>
       </c>
@@ -6041,7 +6034,7 @@
       <c r="I142" s="9"/>
       <c r="J142" s="9"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12">
       <c r="C143">
         <v>2048</v>
       </c>
@@ -6056,7 +6049,7 @@
       <c r="I143" s="9"/>
       <c r="J143" s="9"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12">
       <c r="C144">
         <v>2048</v>
       </c>
@@ -6071,7 +6064,7 @@
       <c r="I144" s="9"/>
       <c r="J144" s="9"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="C145">
         <v>2048</v>
       </c>
@@ -6086,7 +6079,7 @@
       <c r="I145" s="9"/>
       <c r="J145" s="9"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="C146">
         <v>2560</v>
       </c>
@@ -6101,7 +6094,7 @@
       <c r="I146" s="9"/>
       <c r="J146" s="9"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="C147">
         <v>2560</v>
       </c>
@@ -6116,7 +6109,7 @@
       <c r="I147" s="9"/>
       <c r="J147" s="9"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="C148">
         <v>2560</v>
       </c>
@@ -6131,7 +6124,7 @@
       <c r="I148" s="9"/>
       <c r="J148" s="9"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="C149">
         <v>2560</v>
       </c>
@@ -6146,10 +6139,10 @@
       <c r="I149" s="9"/>
       <c r="J149" s="9"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="I151" s="1"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -6175,7 +6168,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="C154">
         <v>512</v>
       </c>
@@ -6190,7 +6183,7 @@
       <c r="I154" s="9"/>
       <c r="J154" s="9"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="C155">
         <v>512</v>
       </c>
@@ -6205,7 +6198,7 @@
       <c r="I155" s="9"/>
       <c r="J155" s="9"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="C156">
         <v>512</v>
       </c>
@@ -6220,7 +6213,7 @@
       <c r="I156" s="9"/>
       <c r="J156" s="9"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="C157">
         <v>512</v>
       </c>
@@ -6235,7 +6228,7 @@
       <c r="I157" s="9"/>
       <c r="J157" s="9"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="C158">
         <v>1024</v>
       </c>
@@ -6250,7 +6243,7 @@
       <c r="I158" s="9"/>
       <c r="J158" s="9"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="C159">
         <v>1024</v>
       </c>
@@ -6265,7 +6258,7 @@
       <c r="I159" s="9"/>
       <c r="J159" s="9"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="C160">
         <v>1024</v>
       </c>
@@ -6280,7 +6273,7 @@
       <c r="I160" s="9"/>
       <c r="J160" s="9"/>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15">
       <c r="C161">
         <v>1024</v>
       </c>
@@ -6295,7 +6288,7 @@
       <c r="I161" s="9"/>
       <c r="J161" s="9"/>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15">
       <c r="C162">
         <v>2048</v>
       </c>
@@ -6310,7 +6303,7 @@
       <c r="I162" s="9"/>
       <c r="J162" s="9"/>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15">
       <c r="C163">
         <v>2048</v>
       </c>
@@ -6325,7 +6318,7 @@
       <c r="I163" s="9"/>
       <c r="J163" s="9"/>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15">
       <c r="C164">
         <v>2048</v>
       </c>
@@ -6340,7 +6333,7 @@
       <c r="I164" s="9"/>
       <c r="J164" s="9"/>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15">
       <c r="C165">
         <v>2048</v>
       </c>
@@ -6355,7 +6348,7 @@
       <c r="I165" s="9"/>
       <c r="J165" s="9"/>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15">
       <c r="C166">
         <v>4096</v>
       </c>
@@ -6370,7 +6363,7 @@
       <c r="I166" s="9"/>
       <c r="J166" s="9"/>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15">
       <c r="C167">
         <v>4096</v>
       </c>
@@ -6385,7 +6378,7 @@
       <c r="I167" s="9"/>
       <c r="J167" s="9"/>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15">
       <c r="C168">
         <v>4096</v>
       </c>
@@ -6400,7 +6393,7 @@
       <c r="I168" s="9"/>
       <c r="J168" s="9"/>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15">
       <c r="C169">
         <v>4096</v>
       </c>
@@ -6415,16 +6408,16 @@
       <c r="I169" s="9"/>
       <c r="J169" s="9"/>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15">
       <c r="I171" s="1"/>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15">
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
       <c r="K172" s="2"/>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15">
       <c r="A173" t="s">
         <v>4</v>
       </c>
@@ -6447,7 +6440,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15">
       <c r="C175">
         <v>100000</v>
       </c>
@@ -6472,7 +6465,7 @@
       <c r="N175" s="2"/>
       <c r="O175" s="2"/>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15">
       <c r="C176">
         <v>100000</v>
       </c>
@@ -6497,7 +6490,7 @@
       <c r="N176" s="2"/>
       <c r="O176" s="2"/>
     </row>
-    <row r="177" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:15">
       <c r="C177">
         <v>100000</v>
       </c>
@@ -6522,7 +6515,7 @@
       <c r="N177" s="2"/>
       <c r="O177" s="2"/>
     </row>
-    <row r="178" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:15">
       <c r="C178">
         <v>100000</v>
       </c>
@@ -6547,7 +6540,7 @@
       </c>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:15">
       <c r="C179">
         <v>100000</v>
       </c>
@@ -6572,7 +6565,7 @@
       </c>
       <c r="L179" s="2"/>
     </row>
-    <row r="180" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:15">
       <c r="C180">
         <v>3097600</v>
       </c>
@@ -6597,7 +6590,7 @@
       <c r="N180" s="2"/>
       <c r="O180" s="2"/>
     </row>
-    <row r="181" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:15">
       <c r="C181">
         <f>1760*1760</f>
         <v>3097600</v>
@@ -6623,7 +6616,7 @@
       <c r="N181" s="2"/>
       <c r="O181" s="2"/>
     </row>
-    <row r="182" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:15">
       <c r="C182">
         <f>1760*1760</f>
         <v>3097600</v>
@@ -6649,7 +6642,7 @@
       <c r="N182" s="2"/>
       <c r="O182" s="2"/>
     </row>
-    <row r="183" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:15">
       <c r="C183">
         <v>3097600</v>
       </c>
@@ -6674,7 +6667,7 @@
       </c>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:15">
       <c r="C184">
         <v>3097600</v>
       </c>
@@ -6699,7 +6692,7 @@
       </c>
       <c r="L184" s="2"/>
     </row>
-    <row r="185" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:15">
       <c r="C185">
         <v>4194304</v>
       </c>
@@ -6724,7 +6717,7 @@
       <c r="N185" s="2"/>
       <c r="O185" s="2"/>
     </row>
-    <row r="186" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:15">
       <c r="C186">
         <f>2048*2048</f>
         <v>4194304</v>
@@ -6750,7 +6743,7 @@
       <c r="N186" s="2"/>
       <c r="O186" s="2"/>
     </row>
-    <row r="187" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:15">
       <c r="C187">
         <f>2048*2048</f>
         <v>4194304</v>
@@ -6776,7 +6769,7 @@
       <c r="N187" s="2"/>
       <c r="O187" s="2"/>
     </row>
-    <row r="188" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:15">
       <c r="C188">
         <v>4194304</v>
       </c>
@@ -6802,7 +6795,7 @@
       <c r="L188" s="2"/>
       <c r="O188" s="2"/>
     </row>
-    <row r="189" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:15">
       <c r="C189">
         <v>4194304</v>
       </c>
@@ -6828,7 +6821,7 @@
       <c r="L189" s="2"/>
       <c r="O189" s="2"/>
     </row>
-    <row r="190" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:15">
       <c r="C190">
         <v>6553600</v>
       </c>
@@ -6853,7 +6846,7 @@
       <c r="N190" s="2"/>
       <c r="O190" s="2"/>
     </row>
-    <row r="191" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:15">
       <c r="C191">
         <f>2560*2560</f>
         <v>6553600</v>
@@ -6879,7 +6872,7 @@
       <c r="N191" s="2"/>
       <c r="O191" s="2"/>
     </row>
-    <row r="192" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:15">
       <c r="C192">
         <f>2560*2560</f>
         <v>6553600</v>
@@ -6905,7 +6898,7 @@
       <c r="N192" s="2"/>
       <c r="O192" s="2"/>
     </row>
-    <row r="193" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:16">
       <c r="C193">
         <v>6553600</v>
       </c>
@@ -6930,7 +6923,7 @@
       </c>
       <c r="L193" s="2"/>
     </row>
-    <row r="194" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:16">
       <c r="C194">
         <v>6553600</v>
       </c>
@@ -6955,7 +6948,7 @@
       </c>
       <c r="L194" s="2"/>
     </row>
-    <row r="195" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:16">
       <c r="C195">
         <f t="shared" ref="C195:C197" si="15">4096*4096</f>
         <v>16777216</v>
@@ -6981,7 +6974,7 @@
       <c r="N195" s="2"/>
       <c r="O195" s="2"/>
     </row>
-    <row r="196" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:16">
       <c r="C196">
         <f t="shared" si="15"/>
         <v>16777216</v>
@@ -7007,7 +7000,7 @@
       <c r="N196" s="2"/>
       <c r="O196" s="2"/>
     </row>
-    <row r="197" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:16">
       <c r="C197">
         <f t="shared" si="15"/>
         <v>16777216</v>
@@ -7033,7 +7026,7 @@
       <c r="N197" s="2"/>
       <c r="O197" s="2"/>
     </row>
-    <row r="198" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:16">
       <c r="C198">
         <v>16777216</v>
       </c>
@@ -7060,7 +7053,7 @@
       <c r="L198" s="2"/>
       <c r="N198" s="2"/>
     </row>
-    <row r="199" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:16">
       <c r="C199">
         <v>16777216</v>
       </c>
@@ -7087,7 +7080,7 @@
       <c r="L199" s="2"/>
       <c r="N199" s="2"/>
     </row>
-    <row r="200" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:16">
       <c r="I200" s="2"/>
       <c r="J200" s="2"/>
       <c r="K200" s="2"/>
@@ -7097,10 +7090,10 @@
       <c r="O200" s="2"/>
       <c r="P200" s="2"/>
     </row>
-    <row r="201" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:16">
       <c r="G201" s="1"/>
     </row>
-    <row r="207" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:16">
       <c r="G207" s="1"/>
     </row>
   </sheetData>
@@ -7118,17 +7111,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>47</v>
       </c>
@@ -7136,7 +7129,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -7144,7 +7137,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -7152,7 +7145,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
@@ -7160,7 +7153,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>69</v>
       </c>
@@ -7168,7 +7161,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
@@ -7176,23 +7169,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
@@ -7202,7 +7195,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>